<commit_message>
factor analysis and LCA
excluding prayer and spiritual healing
</commit_message>
<xml_diff>
--- a/R/Factor analysis  - factor loadings.xlsx
+++ b/R/Factor analysis  - factor loadings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\git\AHL\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3167CB43-CDC9-4EB8-8869-5457C9296EA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0025DDB9-2E90-41D0-A33A-62307B528938}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="19320" windowHeight="10320" activeTab="1" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,6 +43,41 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>hanna</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{C157D167-B9CE-4BD4-9C6F-10FEBE7BB0DD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Dropped prayer and spiritual healing 
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -236,63 +271,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="94">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -392,12 +371,10 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -428,136 +405,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -646,386 +493,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2544,31 +2011,31 @@
   </sheetData>
   <autoFilter ref="A1:AC1" xr:uid="{99B320C6-A597-4E1B-B5FD-F0989543660C}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC16">
-      <sortCondition sortBy="cellColor" ref="AC1" dxfId="50"/>
+      <sortCondition sortBy="cellColor" ref="AC1" dxfId="25"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:C16">
-    <cfRule type="cellIs" dxfId="48" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H16">
-    <cfRule type="cellIs" dxfId="47" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:N16">
-    <cfRule type="cellIs" dxfId="46" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:U16">
-    <cfRule type="cellIs" dxfId="45" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:AC16">
-    <cfRule type="cellIs" dxfId="44" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2578,11 +2045,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D61808F-2A1D-4F74-9E35-43CB27586058}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D61808F-2A1D-4F74-9E35-43CB27586058}">
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2632,40 +2099,46 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>0.70799999999999996</v>
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="C2">
+        <v>-0.2</v>
       </c>
       <c r="D2">
-        <v>-0.11799999999999999</v>
+        <v>0.53200000000000003</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>0.17799999999999999</v>
+        <v>0.188</v>
+      </c>
+      <c r="H2">
+        <v>0.49099999999999999</v>
       </c>
       <c r="I2">
-        <v>0.33900000000000002</v>
+        <v>-0.20300000000000001</v>
       </c>
       <c r="J2">
-        <v>0.50700000000000001</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
+        <v>0.29099999999999998</v>
       </c>
       <c r="L2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M2">
-        <v>0.504</v>
+        <v>0.157</v>
+      </c>
+      <c r="O2">
+        <v>0.42699999999999999</v>
       </c>
       <c r="P2">
-        <v>0.14799999999999999</v>
+        <v>0.151</v>
       </c>
       <c r="Q2">
-        <v>-0.378</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="R2" t="s">
         <v>25</v>
@@ -2731,93 +2204,75 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>0.37</v>
-      </c>
-      <c r="C5">
-        <v>0.48399999999999999</v>
-      </c>
-      <c r="D5">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
+        <v>0.58499999999999996</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G5">
-        <v>0.51400000000000001</v>
-      </c>
-      <c r="H5">
-        <v>0.318</v>
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="I5">
+        <v>-0.24099999999999999</v>
       </c>
       <c r="J5">
-        <v>0.154</v>
-      </c>
-      <c r="K5" t="s">
-        <v>19</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="L5" t="s">
-        <v>5</v>
-      </c>
-      <c r="M5">
-        <v>0.34499999999999997</v>
-      </c>
-      <c r="N5">
-        <v>0.41099999999999998</v>
+        <v>12</v>
       </c>
       <c r="O5">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="P5">
-        <v>0.155</v>
+        <v>0.90800000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>0.20100000000000001</v>
+        <v>0.37</v>
       </c>
       <c r="C6">
-        <v>-0.2</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="D6">
-        <v>0.53200000000000003</v>
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G6">
-        <v>0.188</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="H6">
-        <v>0.49099999999999999</v>
-      </c>
-      <c r="I6">
-        <v>-0.20300000000000001</v>
+        <v>0.318</v>
       </c>
       <c r="J6">
-        <v>0.29099999999999998</v>
+        <v>0.154</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
       </c>
       <c r="L6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M6">
-        <v>0.157</v>
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="N6">
+        <v>0.41099999999999998</v>
       </c>
       <c r="O6">
-        <v>0.42699999999999999</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="P6">
-        <v>0.151</v>
-      </c>
-      <c r="Q6">
-        <v>0.44500000000000001</v>
+        <v>0.155</v>
       </c>
       <c r="R6" t="s">
         <v>25</v>
@@ -2863,155 +2318,167 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>0.109</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>0.48699999999999999</v>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="D8">
+        <v>0.41599999999999998</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8">
-        <v>0.85</v>
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="I8">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="J8">
+        <v>0.13800000000000001</v>
       </c>
       <c r="L8" t="s">
-        <v>7</v>
-      </c>
-      <c r="M8">
-        <v>0.82699999999999996</v>
+        <v>11</v>
+      </c>
+      <c r="N8">
+        <v>0.85199999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="F9" t="s">
         <v>11</v>
       </c>
-      <c r="C9">
-        <v>0.91</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9">
-        <v>0.75</v>
-      </c>
-      <c r="I9">
-        <v>0.114</v>
-      </c>
-      <c r="J9">
-        <v>-0.217</v>
+      <c r="G9">
+        <v>0.89400000000000002</v>
       </c>
       <c r="L9" t="s">
-        <v>8</v>
-      </c>
-      <c r="M9">
-        <v>0.74</v>
-      </c>
-      <c r="Q9">
-        <v>0.224</v>
+        <v>14</v>
+      </c>
+      <c r="N9">
+        <v>0.745</v>
+      </c>
+      <c r="P9">
+        <v>0.191</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10">
-        <v>0.90500000000000003</v>
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="D10">
+        <v>-0.11799999999999999</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10">
-        <v>0.82099999999999995</v>
+        <v>12</v>
+      </c>
+      <c r="G10">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="I10">
+        <v>0.33900000000000002</v>
       </c>
       <c r="J10">
-        <v>0.105</v>
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="K10" t="s">
+        <v>19</v>
       </c>
       <c r="L10" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="M10">
-        <v>0.83899999999999997</v>
+        <v>0.504</v>
+      </c>
+      <c r="P10">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="Q10">
+        <v>-0.378</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>0.58499999999999996</v>
+        <v>0.109</v>
+      </c>
+      <c r="C11">
+        <v>0.48699999999999999</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11">
-        <v>0.59699999999999998</v>
-      </c>
-      <c r="I11">
-        <v>-0.24099999999999999</v>
-      </c>
-      <c r="J11">
-        <v>0.13300000000000001</v>
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>0.85</v>
       </c>
       <c r="L11" t="s">
-        <v>12</v>
-      </c>
-      <c r="O11">
-        <v>0.90800000000000003</v>
+        <v>7</v>
+      </c>
+      <c r="M11">
+        <v>0.82699999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C12">
-        <v>0.26500000000000001</v>
-      </c>
-      <c r="D12">
-        <v>0.41599999999999998</v>
+        <v>0.91</v>
       </c>
       <c r="F12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <v>0.55500000000000005</v>
+        <v>8</v>
+      </c>
+      <c r="H12">
+        <v>0.75</v>
       </c>
       <c r="I12">
-        <v>0.20399999999999999</v>
+        <v>0.114</v>
       </c>
       <c r="J12">
-        <v>0.13800000000000001</v>
+        <v>-0.217</v>
       </c>
       <c r="L12" t="s">
-        <v>11</v>
-      </c>
-      <c r="N12">
-        <v>0.85199999999999998</v>
+        <v>8</v>
+      </c>
+      <c r="M12">
+        <v>0.74</v>
+      </c>
+      <c r="Q12">
+        <v>0.224</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>0.89200000000000002</v>
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>0.90500000000000003</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13">
-        <v>0.89400000000000002</v>
+        <v>9</v>
+      </c>
+      <c r="H13">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="J13">
+        <v>0.105</v>
       </c>
       <c r="L13" t="s">
-        <v>14</v>
-      </c>
-      <c r="N13">
-        <v>0.745</v>
-      </c>
-      <c r="P13">
-        <v>0.191</v>
+        <v>9</v>
+      </c>
+      <c r="M13">
+        <v>0.83899999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.45">
@@ -3222,25 +2689,26 @@
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{85F09F99-28C1-4BB1-A75C-F2C0B1518057}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q14">
-      <sortCondition sortBy="cellColor" ref="J1" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="Q1" dxfId="1"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:Q14">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3248,9 +2716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8727E6E-4063-4F85-BAE5-AB6F095D427F}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -3679,21 +3145,21 @@
   </sheetData>
   <autoFilter ref="A1:F14" xr:uid="{F6EC43A2-0E96-4311-A986-12EE04542C46}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
-      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="92"/>
+      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="16"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:E1048576">
-    <cfRule type="cellIs" dxfId="43" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:K1">
-    <cfRule type="cellIs" dxfId="42" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K12">
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3919,11 +3385,11 @@
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{20237AFA-AF5A-4959-9459-F55DA7A9A145}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H12">
-      <sortCondition sortBy="cellColor" ref="E1" dxfId="91"/>
+      <sortCondition sortBy="cellColor" ref="E1" dxfId="12"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E12">
-    <cfRule type="cellIs" dxfId="40" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Factor Analysis and examine total CAMs used
</commit_message>
<xml_diff>
--- a/R/Factor analysis  - factor loadings.xlsx
+++ b/R/Factor analysis  - factor loadings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\git\AHL\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0025DDB9-2E90-41D0-A33A-62307B528938}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7712CFC6-0CBD-45F5-A552-6E739DCB7EA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="19320" windowHeight="10320" activeTab="1" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
   </bookViews>
@@ -17,12 +17,14 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AC$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$Q$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$A$1:$F$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet4!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet5!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -137,8 +139,43 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>hanna</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{93B109C3-C5E5-457F-BA6A-EE399D655DD0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Models excluding prayer and spiritual healing, tetrachoric matrix on numeric variables 
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="26">
   <si>
     <t>ML2</t>
   </si>
@@ -271,7 +308,55 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="39">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -371,10 +456,72 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -443,6 +590,14 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -817,7 +972,7 @@
   <dimension ref="A1:AD21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD5" sqref="AD5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2011,31 +2166,31 @@
   </sheetData>
   <autoFilter ref="A1:AC1" xr:uid="{99B320C6-A597-4E1B-B5FD-F0989543660C}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC16">
-      <sortCondition sortBy="cellColor" ref="AC1" dxfId="25"/>
+      <sortCondition sortBy="cellColor" ref="AC1" dxfId="38"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:C16">
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H16">
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:N16">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:U16">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:AC16">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2048,8 +2203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D61808F-2A1D-4F74-9E35-43CB27586058}">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="164" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2099,46 +2254,40 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="C2">
-        <v>-0.2</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="D2">
-        <v>0.53200000000000003</v>
+        <v>-0.11799999999999999</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="I2">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="J2">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
         <v>2</v>
       </c>
-      <c r="G2">
-        <v>0.188</v>
-      </c>
-      <c r="H2">
-        <v>0.49099999999999999</v>
-      </c>
-      <c r="I2">
-        <v>-0.20300000000000001</v>
-      </c>
-      <c r="J2">
-        <v>0.29099999999999998</v>
-      </c>
-      <c r="L2" t="s">
-        <v>6</v>
-      </c>
       <c r="M2">
-        <v>0.157</v>
-      </c>
-      <c r="O2">
-        <v>0.42699999999999999</v>
+        <v>0.504</v>
       </c>
       <c r="P2">
-        <v>0.151</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="Q2">
-        <v>0.44500000000000001</v>
+        <v>-0.378</v>
       </c>
       <c r="R2" t="s">
         <v>25</v>
@@ -2204,75 +2353,93 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>0.58499999999999996</v>
+        <v>0.37</v>
+      </c>
+      <c r="C5">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="D5">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>0.59699999999999998</v>
-      </c>
-      <c r="I5">
-        <v>-0.24099999999999999</v>
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="H5">
+        <v>0.318</v>
       </c>
       <c r="J5">
-        <v>0.13300000000000001</v>
+        <v>0.154</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
       </c>
       <c r="L5" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="N5">
+        <v>0.41099999999999998</v>
       </c>
       <c r="O5">
-        <v>0.90800000000000003</v>
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="P5">
+        <v>0.155</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>0.37</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="C6">
-        <v>0.48399999999999999</v>
+        <v>-0.2</v>
       </c>
       <c r="D6">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
+        <v>0.53200000000000003</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G6">
-        <v>0.51400000000000001</v>
+        <v>0.188</v>
       </c>
       <c r="H6">
-        <v>0.318</v>
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="I6">
+        <v>-0.20300000000000001</v>
       </c>
       <c r="J6">
-        <v>0.154</v>
-      </c>
-      <c r="K6" t="s">
-        <v>19</v>
+        <v>0.29099999999999998</v>
       </c>
       <c r="L6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M6">
-        <v>0.34499999999999997</v>
-      </c>
-      <c r="N6">
-        <v>0.41099999999999998</v>
+        <v>0.157</v>
       </c>
       <c r="O6">
-        <v>0.16500000000000001</v>
+        <v>0.42699999999999999</v>
       </c>
       <c r="P6">
-        <v>0.155</v>
+        <v>0.151</v>
+      </c>
+      <c r="Q6">
+        <v>0.44500000000000001</v>
       </c>
       <c r="R6" t="s">
         <v>25</v>
@@ -2318,167 +2485,155 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0.109</v>
       </c>
       <c r="C8">
-        <v>0.26500000000000001</v>
-      </c>
-      <c r="D8">
-        <v>0.41599999999999998</v>
+        <v>0.48699999999999999</v>
       </c>
       <c r="F8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8">
-        <v>0.55500000000000005</v>
-      </c>
-      <c r="I8">
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="J8">
-        <v>0.13800000000000001</v>
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>0.85</v>
       </c>
       <c r="L8" t="s">
-        <v>11</v>
-      </c>
-      <c r="N8">
-        <v>0.85199999999999998</v>
+        <v>7</v>
+      </c>
+      <c r="M8">
+        <v>0.82699999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>0.89200000000000002</v>
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>0.91</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9">
-        <v>0.89400000000000002</v>
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>0.75</v>
+      </c>
+      <c r="I9">
+        <v>0.114</v>
+      </c>
+      <c r="J9">
+        <v>-0.217</v>
       </c>
       <c r="L9" t="s">
-        <v>14</v>
-      </c>
-      <c r="N9">
-        <v>0.745</v>
-      </c>
-      <c r="P9">
-        <v>0.191</v>
+        <v>8</v>
+      </c>
+      <c r="M9">
+        <v>0.74</v>
+      </c>
+      <c r="Q9">
+        <v>0.224</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>0.70799999999999996</v>
-      </c>
-      <c r="D10">
-        <v>-0.11799999999999999</v>
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>0.90500000000000003</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="I10">
-        <v>0.33900000000000002</v>
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>0.82099999999999995</v>
       </c>
       <c r="J10">
-        <v>0.50700000000000001</v>
-      </c>
-      <c r="K10" t="s">
-        <v>19</v>
+        <v>0.105</v>
       </c>
       <c r="L10" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="M10">
-        <v>0.504</v>
-      </c>
-      <c r="P10">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="Q10">
-        <v>-0.378</v>
+        <v>0.83899999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="F11" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>0.109</v>
-      </c>
-      <c r="C11">
-        <v>0.48699999999999999</v>
-      </c>
-      <c r="F11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11">
-        <v>0.85</v>
+      <c r="G11">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="I11">
+        <v>-0.24099999999999999</v>
+      </c>
+      <c r="J11">
+        <v>0.13300000000000001</v>
       </c>
       <c r="L11" t="s">
-        <v>7</v>
-      </c>
-      <c r="M11">
-        <v>0.82699999999999996</v>
+        <v>12</v>
+      </c>
+      <c r="O11">
+        <v>0.90800000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="I12">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="J12">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="L12" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
-        <v>0.91</v>
-      </c>
-      <c r="F12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12">
-        <v>0.75</v>
-      </c>
-      <c r="I12">
-        <v>0.114</v>
-      </c>
-      <c r="J12">
-        <v>-0.217</v>
-      </c>
-      <c r="L12" t="s">
-        <v>8</v>
-      </c>
-      <c r="M12">
-        <v>0.74</v>
-      </c>
-      <c r="Q12">
-        <v>0.224</v>
+      <c r="N12">
+        <v>0.85199999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="L13" t="s">
         <v>14</v>
       </c>
-      <c r="C13">
-        <v>0.90500000000000003</v>
-      </c>
-      <c r="F13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13">
-        <v>0.82099999999999995</v>
-      </c>
-      <c r="J13">
-        <v>0.105</v>
-      </c>
-      <c r="L13" t="s">
-        <v>9</v>
-      </c>
-      <c r="M13">
-        <v>0.83899999999999997</v>
+      <c r="N13">
+        <v>0.745</v>
+      </c>
+      <c r="P13">
+        <v>0.191</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.45">
@@ -2689,22 +2844,25 @@
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{85F09F99-28C1-4BB1-A75C-F2C0B1518057}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q14">
-      <sortCondition sortBy="cellColor" ref="Q1" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="J1" dxfId="1"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="19" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:Q14">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="greaterThan">
       <formula>0.299</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="lessThan">
+      <formula>-0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2716,7 +2874,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8727E6E-4063-4F85-BAE5-AB6F095D427F}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -3145,21 +3305,21 @@
   </sheetData>
   <autoFilter ref="A1:F14" xr:uid="{F6EC43A2-0E96-4311-A986-12EE04542C46}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
-      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="16"/>
+      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="32"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:E1048576">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:K1">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K12">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3385,14 +3545,284 @@
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{20237AFA-AF5A-4959-9459-F55DA7A9A145}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H12">
-      <sortCondition sortBy="cellColor" ref="E1" dxfId="12"/>
+      <sortCondition sortBy="cellColor" ref="E1" dxfId="28"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E12">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C8C1A-CFC6-49AC-B896-635D55B44BA8}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="14.265625" customWidth="1"/>
+    <col min="6" max="6" width="13.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="J2">
+        <v>0.35699999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="J3">
+        <v>0.374</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>-0.108</v>
+      </c>
+      <c r="D4">
+        <v>0.313</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>0.36199999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>0.70799999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="C6">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>0.26</v>
+      </c>
+      <c r="H6">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="J6">
+        <v>-0.11899999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>0.71099999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="D8">
+        <v>0.215</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8">
+        <v>0.49</v>
+      </c>
+      <c r="J8">
+        <v>0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>0.64700000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>0.39</v>
+      </c>
+      <c r="J10">
+        <v>0.23200000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>0.627</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>0.317</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="J12">
+        <v>-0.13600000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>0.23499999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>0.23799999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:J1" xr:uid="{76B16ADE-8397-4523-89E6-FD43024CAE02}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J14">
+      <sortCondition sortBy="cellColor" ref="J1" dxfId="10"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="B2:D14">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:J14">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Many changes - haven't committed in awhile
Been working on factor analysis and LCA.
</commit_message>
<xml_diff>
--- a/R/Factor analysis  - factor loadings.xlsx
+++ b/R/Factor analysis  - factor loadings.xlsx
@@ -1,30 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\git\AHL\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7712CFC6-0CBD-45F5-A552-6E739DCB7EA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B0FDBF-D918-4467-AE15-C0ADE9B8CBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="19320" windowHeight="10320" activeTab="1" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AC$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AC$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$Q$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$A$1:$F$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet4!$A$1:$H$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet5!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet4!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet5!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet6!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -145,6 +147,66 @@
     <author>hanna</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{D5712E48-0578-4E7B-970F-9D684F744419}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Four factor model excluding prayer and spiritual healing using MIDUS-complete data
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{6A9F4E1D-6D92-4062-8A79-2B5448FE1065}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Four factor model, prayer and spiritual healing dropped. 
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>hanna</author>
+  </authors>
+  <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{93B109C3-C5E5-457F-BA6A-EE399D655DD0}">
       <text>
         <r>
@@ -175,7 +237,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="26">
   <si>
     <t>ML2</t>
   </si>
@@ -308,7 +370,615 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="182">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -556,14 +1226,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -594,14 +1256,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -618,6 +1272,596 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -971,8 +2215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A59E54-D4A7-4C25-9D11-CD018EBC24D4}">
   <dimension ref="A1:AD21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="V1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1049,102 +2293,126 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>0.872</v>
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>1.0069999999999999</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F2">
-        <v>0.54800000000000004</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="G2">
-        <v>0.27500000000000002</v>
+        <v>0.126</v>
       </c>
       <c r="H2">
-        <v>0.245</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2">
-        <v>0.75900000000000001</v>
+        <v>8</v>
+      </c>
+      <c r="K2">
+        <v>0.77200000000000002</v>
       </c>
       <c r="M2">
-        <v>0.16300000000000001</v>
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="N2">
+        <v>0.191</v>
       </c>
       <c r="P2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q2">
-        <v>0.90200000000000002</v>
+        <v>13</v>
+      </c>
+      <c r="R2">
+        <v>0.188</v>
+      </c>
+      <c r="T2">
+        <v>0.317</v>
+      </c>
+      <c r="U2">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="V2" t="s">
+        <v>25</v>
       </c>
       <c r="W2" t="s">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="X2">
+        <v>0.55500000000000005</v>
       </c>
       <c r="Y2">
-        <v>0.16300000000000001</v>
-      </c>
-      <c r="AA2">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="AC2">
-        <v>0.75800000000000001</v>
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="Z2">
+        <v>-0.17599999999999999</v>
+      </c>
+      <c r="AB2">
+        <v>0.23</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>0.74099999999999999</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="C3">
-        <v>-0.104</v>
+        <v>-0.106</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>0.55400000000000005</v>
+        <v>0.22800000000000001</v>
       </c>
       <c r="G3">
-        <v>0.17</v>
+        <v>0.50900000000000001</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3">
-        <v>0.96</v>
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>0.63800000000000001</v>
       </c>
       <c r="N3">
-        <v>0.11</v>
+        <v>-0.16400000000000001</v>
       </c>
       <c r="P3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q3">
-        <v>0.40799999999999997</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="R3">
-        <v>-0.114</v>
+        <v>0.36899999999999999</v>
       </c>
       <c r="S3">
-        <v>0.128</v>
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="T3">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="U3">
+        <v>-0.13200000000000001</v>
+      </c>
+      <c r="V3" t="s">
+        <v>25</v>
       </c>
       <c r="W3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="Y3">
-        <v>0.20100000000000001</v>
+        <v>0.57799999999999996</v>
       </c>
       <c r="Z3">
-        <v>0.27800000000000002</v>
-      </c>
-      <c r="AB3">
-        <v>0.53200000000000003</v>
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="AC3">
+        <v>-0.14699999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.45">
@@ -1193,55 +2461,49 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B5">
-        <v>0.44800000000000001</v>
+        <v>0.185</v>
+      </c>
+      <c r="C5">
+        <v>0.64800000000000002</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>0.53200000000000003</v>
-      </c>
-      <c r="G5">
-        <v>-0.14399999999999999</v>
+        <v>16</v>
+      </c>
+      <c r="H5">
+        <v>0.998</v>
       </c>
       <c r="J5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5">
-        <v>0.505</v>
-      </c>
-      <c r="M5">
-        <v>0.223</v>
-      </c>
-      <c r="N5">
-        <v>-0.22</v>
+        <v>7</v>
+      </c>
+      <c r="K5">
+        <v>0.88600000000000001</v>
       </c>
       <c r="P5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="R5">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="S5">
+        <v>0.35</v>
+      </c>
+      <c r="T5">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="U5">
+        <v>-0.15</v>
+      </c>
+      <c r="W5" t="s">
         <v>6</v>
       </c>
-      <c r="S5">
-        <v>0.98499999999999999</v>
-      </c>
-      <c r="W5" t="s">
-        <v>5</v>
-      </c>
-      <c r="X5">
-        <v>0.318</v>
-      </c>
-      <c r="Y5">
-        <v>0.375</v>
-      </c>
       <c r="Z5">
-        <v>0.13400000000000001</v>
-      </c>
-      <c r="AA5">
-        <v>0.33700000000000002</v>
-      </c>
-      <c r="AC5">
-        <v>-0.124</v>
+        <v>0.96099999999999997</v>
       </c>
       <c r="AD5" t="s">
         <v>25</v>
@@ -1249,624 +2511,603 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="G6">
+        <v>-0.14399999999999999</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>0.505</v>
+      </c>
+      <c r="M6">
+        <v>0.223</v>
+      </c>
+      <c r="N6">
+        <v>-0.22</v>
+      </c>
+      <c r="P6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>0.61799999999999999</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6">
-        <v>0.47299999999999998</v>
-      </c>
-      <c r="G6">
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6">
-        <v>0.443</v>
-      </c>
-      <c r="L6">
-        <v>0.27300000000000002</v>
-      </c>
-      <c r="N6">
-        <v>-0.13900000000000001</v>
-      </c>
-      <c r="P6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q6">
-        <v>0.248</v>
-      </c>
       <c r="S6">
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="T6">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="U6">
-        <v>0.111</v>
-      </c>
-      <c r="V6" t="s">
-        <v>25</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="W6" t="s">
-        <v>16</v>
+        <v>5</v>
+      </c>
+      <c r="X6">
+        <v>0.318</v>
+      </c>
+      <c r="Y6">
+        <v>0.375</v>
+      </c>
+      <c r="Z6">
+        <v>0.13400000000000001</v>
       </c>
       <c r="AA6">
-        <v>0.94899999999999995</v>
+        <v>0.33700000000000002</v>
       </c>
       <c r="AC6">
-        <v>0.128</v>
+        <v>-0.124</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>0.185</v>
+        <v>0.71899999999999997</v>
       </c>
       <c r="C7">
-        <v>0.64800000000000002</v>
+        <v>-0.13100000000000001</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7">
-        <v>0.998</v>
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0.67900000000000005</v>
       </c>
       <c r="J7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K7">
-        <v>0.88600000000000001</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="P7" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q7">
-        <v>0.27500000000000002</v>
+        <v>14</v>
       </c>
       <c r="R7">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="S7">
-        <v>0.35</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="T7">
-        <v>0.10299999999999999</v>
+        <v>-0.109</v>
       </c>
       <c r="U7">
-        <v>-0.15</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="W7" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="X7">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="Y7">
+        <v>0.501</v>
       </c>
       <c r="Z7">
-        <v>0.96099999999999997</v>
+        <v>-0.17399999999999999</v>
+      </c>
+      <c r="AA7">
+        <v>0.223</v>
+      </c>
+      <c r="AC7">
+        <v>-0.19400000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B8">
-        <v>0.55900000000000005</v>
+        <v>0.41499999999999998</v>
       </c>
       <c r="C8">
-        <v>0.105</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8">
-        <v>0.65300000000000002</v>
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <v>0.99199999999999999</v>
       </c>
       <c r="J8" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>0.46700000000000003</v>
       </c>
       <c r="L8">
-        <v>0.99199999999999999</v>
-      </c>
-      <c r="M8">
-        <v>-0.11</v>
-      </c>
-      <c r="N8">
-        <v>0.16600000000000001</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="P8" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q8">
-        <v>0.70299999999999996</v>
+        <v>11</v>
+      </c>
+      <c r="R8">
+        <v>0.71599999999999997</v>
       </c>
       <c r="S8">
-        <v>0.10100000000000001</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="T8">
-        <v>-0.13200000000000001</v>
-      </c>
-      <c r="U8">
-        <v>0.19800000000000001</v>
+        <v>0.17299999999999999</v>
       </c>
       <c r="W8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y8">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="AA8">
-        <v>-0.114</v>
-      </c>
-      <c r="AC8">
-        <v>0.193</v>
+        <v>9</v>
+      </c>
+      <c r="X8">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="AB8">
+        <v>0.111</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="C9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>0.192</v>
+      </c>
+      <c r="G9">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="H9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>0.41</v>
+      </c>
+      <c r="L9">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="M9">
+        <v>0.311</v>
+      </c>
+      <c r="N9">
+        <v>-0.13100000000000001</v>
+      </c>
+      <c r="O9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" t="s">
+        <v>3</v>
+      </c>
+      <c r="R9">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="S9">
+        <v>0.224</v>
+      </c>
+      <c r="U9">
+        <v>-0.17299999999999999</v>
+      </c>
+      <c r="W9" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>0.81</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9">
-        <v>0.878</v>
-      </c>
-      <c r="J9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="M9">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="N9">
-        <v>0.72899999999999998</v>
-      </c>
-      <c r="P9" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q9">
-        <v>0.68700000000000006</v>
-      </c>
-      <c r="R9">
-        <v>0.126</v>
-      </c>
-      <c r="S9">
-        <v>-0.152</v>
-      </c>
-      <c r="U9">
-        <v>-0.107</v>
-      </c>
-      <c r="W9" t="s">
-        <v>11</v>
-      </c>
       <c r="X9">
-        <v>0.108</v>
-      </c>
-      <c r="Y9">
-        <v>0.70399999999999996</v>
-      </c>
-      <c r="Z9">
-        <v>0.125</v>
-      </c>
-      <c r="AA9">
-        <v>0.191</v>
+        <v>0.85699999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>0.67200000000000004</v>
-      </c>
-      <c r="C10">
-        <v>-0.106</v>
+        <v>0.56499999999999995</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F10">
-        <v>0.22800000000000001</v>
+        <v>0.188</v>
       </c>
       <c r="G10">
-        <v>0.50900000000000001</v>
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="H10">
+        <v>0.122</v>
       </c>
       <c r="J10" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>0.49199999999999999</v>
       </c>
       <c r="L10">
-        <v>0.63800000000000001</v>
-      </c>
-      <c r="N10">
-        <v>-0.16400000000000001</v>
+        <v>-0.107</v>
       </c>
       <c r="P10" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Q10">
-        <v>0.35099999999999998</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="R10">
-        <v>0.36899999999999999</v>
+        <v>0.503</v>
       </c>
       <c r="S10">
-        <v>0.14599999999999999</v>
+        <v>-0.17</v>
       </c>
       <c r="T10">
-        <v>0.32400000000000001</v>
+        <v>0.21199999999999999</v>
       </c>
       <c r="U10">
-        <v>-0.13200000000000001</v>
-      </c>
-      <c r="V10" t="s">
-        <v>25</v>
+        <v>-0.21</v>
       </c>
       <c r="W10" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y10">
-        <v>0.57799999999999996</v>
+        <v>8</v>
+      </c>
+      <c r="X10">
+        <v>0.77600000000000002</v>
       </c>
       <c r="Z10">
-        <v>0.21199999999999999</v>
+        <v>0.111</v>
+      </c>
+      <c r="AA10">
+        <v>-0.107</v>
+      </c>
+      <c r="AB10">
+        <v>-0.13600000000000001</v>
       </c>
       <c r="AC10">
-        <v>-0.14699999999999999</v>
+        <v>0.13500000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>0.81</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>0.878</v>
+      </c>
+      <c r="J11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="M11">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="N11">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="P11" t="s">
         <v>2</v>
       </c>
-      <c r="B11">
-        <v>0.71899999999999997</v>
-      </c>
-      <c r="C11">
-        <v>-0.13100000000000001</v>
-      </c>
-      <c r="E11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>0.67900000000000005</v>
-      </c>
-      <c r="J11" t="s">
-        <v>9</v>
-      </c>
-      <c r="K11">
-        <v>0.85899999999999999</v>
-      </c>
-      <c r="P11" t="s">
-        <v>14</v>
+      <c r="Q11">
+        <v>0.68700000000000006</v>
       </c>
       <c r="R11">
-        <v>0.97099999999999997</v>
-      </c>
-      <c r="T11">
-        <v>-0.109</v>
+        <v>0.126</v>
+      </c>
+      <c r="S11">
+        <v>-0.152</v>
       </c>
       <c r="U11">
-        <v>0.16800000000000001</v>
+        <v>-0.107</v>
       </c>
       <c r="W11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="X11">
-        <v>0.11700000000000001</v>
+        <v>0.108</v>
       </c>
       <c r="Y11">
-        <v>0.501</v>
+        <v>0.70399999999999996</v>
       </c>
       <c r="Z11">
-        <v>-0.17399999999999999</v>
+        <v>0.125</v>
       </c>
       <c r="AA11">
-        <v>0.223</v>
-      </c>
-      <c r="AC11">
-        <v>-0.19400000000000001</v>
+        <v>0.191</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0.74099999999999999</v>
       </c>
       <c r="C12">
-        <v>1.0069999999999999</v>
+        <v>-0.104</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F12">
-        <v>0.35699999999999998</v>
+        <v>0.55400000000000005</v>
       </c>
       <c r="G12">
-        <v>0.126</v>
-      </c>
-      <c r="H12">
-        <v>0.13500000000000001</v>
+        <v>0.17</v>
       </c>
       <c r="J12" t="s">
-        <v>8</v>
-      </c>
-      <c r="K12">
-        <v>0.77200000000000002</v>
+        <v>16</v>
       </c>
       <c r="M12">
-        <v>-0.13500000000000001</v>
+        <v>0.96</v>
       </c>
       <c r="N12">
-        <v>0.191</v>
+        <v>0.11</v>
       </c>
       <c r="P12" t="s">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="Q12">
+        <v>0.40799999999999997</v>
       </c>
       <c r="R12">
-        <v>0.188</v>
-      </c>
-      <c r="T12">
-        <v>0.317</v>
-      </c>
-      <c r="U12">
-        <v>0.72699999999999998</v>
-      </c>
-      <c r="V12" t="s">
-        <v>25</v>
+        <v>-0.114</v>
+      </c>
+      <c r="S12">
+        <v>0.128</v>
       </c>
       <c r="W12" t="s">
-        <v>2</v>
-      </c>
-      <c r="X12">
-        <v>0.55500000000000005</v>
+        <v>12</v>
       </c>
       <c r="Y12">
-        <v>0.14499999999999999</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="Z12">
-        <v>-0.17599999999999999</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="AB12">
-        <v>0.23</v>
+        <v>0.53200000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>0.872</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="G13">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="H13">
+        <v>0.245</v>
+      </c>
+      <c r="J13" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>0.72799999999999998</v>
-      </c>
-      <c r="C13">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13">
-        <v>0.192</v>
-      </c>
-      <c r="G13">
-        <v>0.65800000000000003</v>
-      </c>
-      <c r="H13">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="J13" t="s">
-        <v>5</v>
-      </c>
-      <c r="K13">
-        <v>0.41</v>
-      </c>
       <c r="L13">
-        <v>0.40500000000000003</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="M13">
-        <v>0.311</v>
-      </c>
-      <c r="N13">
-        <v>-0.13100000000000001</v>
-      </c>
-      <c r="O13" t="s">
-        <v>19</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="P13" t="s">
-        <v>3</v>
-      </c>
-      <c r="R13">
-        <v>0.58499999999999996</v>
-      </c>
-      <c r="S13">
-        <v>0.224</v>
-      </c>
-      <c r="U13">
-        <v>-0.17299999999999999</v>
+        <v>7</v>
+      </c>
+      <c r="Q13">
+        <v>0.90200000000000002</v>
       </c>
       <c r="W13" t="s">
-        <v>7</v>
-      </c>
-      <c r="X13">
-        <v>0.85699999999999998</v>
+        <v>13</v>
+      </c>
+      <c r="Y13">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="AA13">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="AC13">
+        <v>0.75800000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B14">
-        <v>0.56499999999999995</v>
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="C14">
+        <v>0.105</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F14">
-        <v>0.188</v>
-      </c>
-      <c r="G14">
-        <v>0.34300000000000003</v>
-      </c>
-      <c r="H14">
-        <v>0.122</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="J14" t="s">
-        <v>4</v>
-      </c>
-      <c r="K14">
-        <v>0.49199999999999999</v>
+        <v>14</v>
       </c>
       <c r="L14">
-        <v>-0.107</v>
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="M14">
+        <v>-0.11</v>
+      </c>
+      <c r="N14">
+        <v>0.16600000000000001</v>
       </c>
       <c r="P14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q14">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="R14">
-        <v>0.503</v>
+        <v>0.70299999999999996</v>
       </c>
       <c r="S14">
-        <v>-0.17</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="T14">
-        <v>0.21199999999999999</v>
+        <v>-0.13200000000000001</v>
       </c>
       <c r="U14">
-        <v>-0.21</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="W14" t="s">
-        <v>8</v>
-      </c>
-      <c r="X14">
-        <v>0.77600000000000002</v>
-      </c>
-      <c r="Z14">
-        <v>0.111</v>
+        <v>14</v>
+      </c>
+      <c r="Y14">
+        <v>0.94599999999999995</v>
       </c>
       <c r="AA14">
-        <v>-0.107</v>
-      </c>
-      <c r="AB14">
-        <v>-0.13600000000000001</v>
+        <v>-0.114</v>
       </c>
       <c r="AC14">
-        <v>0.13500000000000001</v>
+        <v>0.193</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="C15">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <v>-0.13200000000000001</v>
+      </c>
+      <c r="G15">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="H15">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="J15" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="L15">
+        <v>0.105</v>
+      </c>
+      <c r="N15">
+        <v>-0.124</v>
+      </c>
+      <c r="P15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q15">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="W15" t="s">
         <v>15</v>
       </c>
-      <c r="B15">
-        <v>0.41499999999999998</v>
-      </c>
-      <c r="C15">
-        <v>0.17399999999999999</v>
-      </c>
-      <c r="E15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15">
-        <v>0.99199999999999999</v>
-      </c>
-      <c r="J15" t="s">
-        <v>6</v>
-      </c>
-      <c r="K15">
-        <v>0.46700000000000003</v>
-      </c>
-      <c r="L15">
-        <v>0.20300000000000001</v>
-      </c>
-      <c r="P15" t="s">
-        <v>11</v>
-      </c>
-      <c r="R15">
-        <v>0.71599999999999997</v>
-      </c>
-      <c r="S15">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="T15">
-        <v>0.17299999999999999</v>
-      </c>
-      <c r="W15" t="s">
-        <v>9</v>
-      </c>
       <c r="X15">
-        <v>0.76100000000000001</v>
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="Z15">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AA15">
+        <v>0.121</v>
       </c>
       <c r="AB15">
-        <v>0.111</v>
+        <v>-0.153</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B16">
-        <v>0.64700000000000002</v>
-      </c>
-      <c r="C16">
-        <v>0.27200000000000002</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>-0.13200000000000001</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="G16">
-        <v>0.42399999999999999</v>
-      </c>
-      <c r="H16">
-        <v>0.63700000000000001</v>
-      </c>
-      <c r="I16" t="s">
-        <v>19</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="J16" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="K16">
-        <v>0.59399999999999997</v>
+        <v>0.443</v>
       </c>
       <c r="L16">
-        <v>0.105</v>
+        <v>0.27300000000000002</v>
       </c>
       <c r="N16">
-        <v>-0.124</v>
+        <v>-0.13900000000000001</v>
       </c>
       <c r="P16" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="Q16">
-        <v>0.83099999999999996</v>
+        <v>0.248</v>
+      </c>
+      <c r="S16">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="T16">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="U16">
+        <v>0.111</v>
+      </c>
+      <c r="V16" t="s">
+        <v>25</v>
       </c>
       <c r="W16" t="s">
-        <v>15</v>
-      </c>
-      <c r="X16">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="Z16">
-        <v>0.28999999999999998</v>
+        <v>16</v>
       </c>
       <c r="AA16">
-        <v>0.121</v>
-      </c>
-      <c r="AB16">
-        <v>-0.153</v>
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="AC16">
+        <v>0.128</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.45">
@@ -2164,33 +3405,45 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC1" xr:uid="{99B320C6-A597-4E1B-B5FD-F0989543660C}">
+  <autoFilter ref="A1:AC16" xr:uid="{99B320C6-A597-4E1B-B5FD-F0989543660C}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC16">
-      <sortCondition sortBy="cellColor" ref="AC1" dxfId="38"/>
+      <sortCondition sortBy="cellColor" ref="U1:U16" dxfId="1"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="B2:C16">
-    <cfRule type="cellIs" dxfId="37" priority="5" operator="greaterThan">
+  <conditionalFormatting sqref="Q2:U16">
+    <cfRule type="cellIs" dxfId="109" priority="11" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X2:AC16">
+    <cfRule type="cellIs" dxfId="108" priority="10" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H16">
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="93" priority="7" operator="greaterThan">
+      <formula>0.499</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:N16">
-    <cfRule type="cellIs" dxfId="35" priority="3" operator="greaterThan">
+  <conditionalFormatting sqref="B2:C16">
+    <cfRule type="cellIs" dxfId="107" priority="6" operator="greaterThan">
+      <formula>0.499</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:U16">
-    <cfRule type="cellIs" dxfId="34" priority="2" operator="greaterThan">
-      <formula>0.299</formula>
+    <cfRule type="cellIs" dxfId="105" priority="3" operator="greaterThan">
+      <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2:AC16">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="K2:N16">
+    <cfRule type="cellIs" dxfId="104" priority="5" operator="greaterThan">
+      <formula>0.499</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="103" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2201,11 +3454,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D61808F-2A1D-4F74-9E35-43CB27586058}">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="164" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -2214,7 +3465,7 @@
     <col min="12" max="12" width="13.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>17</v>
       </c>
@@ -2252,48 +3503,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>0.70799999999999996</v>
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>0.26500000000000001</v>
       </c>
       <c r="D2">
-        <v>-0.11799999999999999</v>
+        <v>0.41599999999999998</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G2">
-        <v>0.17799999999999999</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="I2">
-        <v>0.33900000000000002</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="J2">
-        <v>0.50700000000000001</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="L2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2">
-        <v>0.504</v>
-      </c>
-      <c r="P2">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="Q2">
-        <v>-0.378</v>
-      </c>
-      <c r="R2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+      <c r="N2">
+        <v>0.85199999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2319,39 +3558,51 @@
         <v>0.98199999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0.20100000000000001</v>
       </c>
       <c r="C4">
-        <v>0.58199999999999996</v>
+        <v>-0.2</v>
       </c>
       <c r="D4">
-        <v>0.13100000000000001</v>
+        <v>0.53200000000000003</v>
       </c>
       <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>0.188</v>
+      </c>
+      <c r="H4">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="I4">
+        <v>-0.20300000000000001</v>
+      </c>
+      <c r="J4">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="L4" t="s">
         <v>6</v>
       </c>
-      <c r="I4">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="L4" t="s">
-        <v>4</v>
-      </c>
       <c r="M4">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="N4">
-        <v>-0.182</v>
+        <v>0.157</v>
       </c>
       <c r="O4">
-        <v>0.53600000000000003</v>
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="P4">
+        <v>0.151</v>
       </c>
       <c r="Q4">
-        <v>-0.16400000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2364,9 +3615,6 @@
       <c r="D5">
         <v>0.13900000000000001</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
       <c r="F5" t="s">
         <v>5</v>
       </c>
@@ -2398,271 +3646,262 @@
         <v>0.155</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>0.91</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>0.75</v>
+      </c>
+      <c r="I6">
+        <v>0.114</v>
+      </c>
+      <c r="J6">
+        <v>-0.217</v>
+      </c>
+      <c r="L6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6">
+        <v>0.74</v>
+      </c>
+      <c r="Q6">
+        <v>0.224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>0.109</v>
+      </c>
+      <c r="C7">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>0.85</v>
+      </c>
+      <c r="L7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7">
+        <v>0.82699999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="J8">
+        <v>0.105</v>
+      </c>
+      <c r="L8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8">
+        <v>0.83899999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="D9">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="L9" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="C6">
-        <v>-0.2</v>
-      </c>
-      <c r="D6">
-        <v>0.53200000000000003</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="M9">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="N9">
+        <v>-0.182</v>
+      </c>
+      <c r="O9">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="Q9">
+        <v>-0.16400000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.875</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="L10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="N10">
+        <v>0.158</v>
+      </c>
+      <c r="Q10">
+        <v>0.28199999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>0.36</v>
+      </c>
+      <c r="C11">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>0.106</v>
+      </c>
+      <c r="H11">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="I11">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="J11">
+        <v>-0.17899999999999999</v>
+      </c>
+      <c r="L11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N11">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="P11">
+        <v>-0.16700000000000001</v>
+      </c>
+      <c r="Q11">
+        <v>-0.26300000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="L12" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12">
+        <v>0.745</v>
+      </c>
+      <c r="P12">
+        <v>0.191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>2</v>
       </c>
-      <c r="G6">
-        <v>0.188</v>
-      </c>
-      <c r="H6">
-        <v>0.49099999999999999</v>
-      </c>
-      <c r="I6">
-        <v>-0.20300000000000001</v>
-      </c>
-      <c r="J6">
-        <v>0.29099999999999998</v>
-      </c>
-      <c r="L6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M6">
-        <v>0.157</v>
-      </c>
-      <c r="O6">
-        <v>0.42699999999999999</v>
-      </c>
-      <c r="P6">
-        <v>0.151</v>
-      </c>
-      <c r="Q6">
-        <v>0.44500000000000001</v>
-      </c>
-      <c r="R6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7">
-        <v>0.36</v>
-      </c>
-      <c r="C7">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7">
-        <v>0.106</v>
-      </c>
-      <c r="H7">
-        <v>0.39700000000000002</v>
-      </c>
-      <c r="I7">
-        <v>0.27300000000000002</v>
-      </c>
-      <c r="J7">
-        <v>-0.17899999999999999</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="B13">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="F13" t="s">
         <v>10</v>
       </c>
-      <c r="N7">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="P7">
-        <v>-0.16700000000000001</v>
-      </c>
-      <c r="Q7">
-        <v>-0.26300000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>0.109</v>
-      </c>
-      <c r="C8">
-        <v>0.48699999999999999</v>
-      </c>
-      <c r="F8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8">
-        <v>0.85</v>
-      </c>
-      <c r="L8" t="s">
-        <v>7</v>
-      </c>
-      <c r="M8">
-        <v>0.82699999999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>0.91</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="G13">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="I13">
+        <v>-0.24099999999999999</v>
+      </c>
+      <c r="J13">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="L13" t="s">
+        <v>12</v>
+      </c>
+      <c r="O13">
+        <v>0.90800000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="H9">
-        <v>0.75</v>
-      </c>
-      <c r="I9">
-        <v>0.114</v>
-      </c>
-      <c r="J9">
-        <v>-0.217</v>
-      </c>
-      <c r="L9" t="s">
-        <v>8</v>
-      </c>
-      <c r="M9">
-        <v>0.74</v>
-      </c>
-      <c r="Q9">
-        <v>0.224</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10">
-        <v>0.90500000000000003</v>
-      </c>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10">
-        <v>0.82099999999999995</v>
-      </c>
-      <c r="J10">
-        <v>0.105</v>
-      </c>
-      <c r="L10" t="s">
-        <v>9</v>
-      </c>
-      <c r="M10">
-        <v>0.83899999999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+      <c r="B14">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="D14">
+        <v>-0.11799999999999999</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="I14">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="J14">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="L14" t="s">
         <v>2</v>
       </c>
-      <c r="B11">
-        <v>0.58499999999999996</v>
-      </c>
-      <c r="F11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11">
-        <v>0.59699999999999998</v>
-      </c>
-      <c r="I11">
-        <v>-0.24099999999999999</v>
-      </c>
-      <c r="J11">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="L11" t="s">
-        <v>12</v>
-      </c>
-      <c r="O11">
-        <v>0.90800000000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12">
-        <v>0.26500000000000001</v>
-      </c>
-      <c r="D12">
-        <v>0.41599999999999998</v>
-      </c>
-      <c r="F12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <v>0.55500000000000005</v>
-      </c>
-      <c r="I12">
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="J12">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="L12" t="s">
-        <v>11</v>
-      </c>
-      <c r="N12">
-        <v>0.85199999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>0.89200000000000002</v>
-      </c>
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13">
-        <v>0.89400000000000002</v>
-      </c>
-      <c r="L13" t="s">
-        <v>14</v>
-      </c>
-      <c r="N13">
-        <v>0.745</v>
-      </c>
-      <c r="P13">
-        <v>0.191</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14">
-        <v>0.875</v>
-      </c>
-      <c r="F14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14">
-        <v>0.91900000000000004</v>
-      </c>
-      <c r="L14" t="s">
-        <v>15</v>
-      </c>
       <c r="M14">
-        <v>0.41499999999999998</v>
-      </c>
-      <c r="N14">
-        <v>0.158</v>
+        <v>0.504</v>
+      </c>
+      <c r="P14">
+        <v>0.14799999999999999</v>
       </c>
       <c r="Q14">
-        <v>0.28199999999999997</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+        <v>-0.378</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>17</v>
       </c>
@@ -2844,25 +4083,31 @@
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{85F09F99-28C1-4BB1-A75C-F2C0B1518057}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q14">
-      <sortCondition sortBy="cellColor" ref="J1" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="D1" dxfId="117"/>
     </sortState>
   </autoFilter>
+  <conditionalFormatting sqref="M2:Q14">
+    <cfRule type="cellIs" dxfId="169" priority="6" operator="lessThan">
+      <formula>-0.299</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="168" priority="7" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="167" priority="4" operator="greaterThan">
+      <formula>0.399</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="166" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="164" priority="3" operator="greaterThan">
+      <formula>0.399</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="165" priority="1" operator="greaterThan">
       <formula>0.299</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M2:Q14">
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="greaterThan">
-      <formula>0.299</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="lessThan">
-      <formula>-0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2874,9 +4119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8727E6E-4063-4F85-BAE5-AB6F095D427F}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -3305,21 +4548,21 @@
   </sheetData>
   <autoFilter ref="A1:F14" xr:uid="{F6EC43A2-0E96-4311-A986-12EE04542C46}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
-      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="32"/>
+      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="181"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:E1048576">
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="180" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:K1">
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="179" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K12">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="178" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3329,12 +4572,447 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC6BCC2-AE82-430A-9446-637AC6346772}">
+  <dimension ref="A1:E29"/>
+  <sheetViews>
+    <sheetView zoomScale="120" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="14.9296875" customWidth="1"/>
+    <col min="7" max="7" width="15.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="D2">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="E2">
+        <v>0.50700000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>-0.114</v>
+      </c>
+      <c r="C3">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="E3">
+        <v>0.64600000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="D4">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="E4">
+        <v>-0.191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>0.83099999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="C6">
+        <v>0.317</v>
+      </c>
+      <c r="D6">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="E6">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>0.223</v>
+      </c>
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>-0.23899999999999999</v>
+      </c>
+      <c r="E7">
+        <v>0.23899999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="E9">
+        <v>-0.193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0.86099999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="D11">
+        <v>0.223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0.624</v>
+      </c>
+      <c r="D12">
+        <v>-0.224</v>
+      </c>
+      <c r="E12">
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="E13">
+        <v>-0.106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0.89900000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>-0.01</v>
+      </c>
+      <c r="C17">
+        <v>0.08</v>
+      </c>
+      <c r="D17">
+        <v>0.27</v>
+      </c>
+      <c r="E17">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>0.12</v>
+      </c>
+      <c r="C18">
+        <v>0.05</v>
+      </c>
+      <c r="D18">
+        <v>-0.03</v>
+      </c>
+      <c r="E18">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>0.11</v>
+      </c>
+      <c r="C19">
+        <v>-0.1</v>
+      </c>
+      <c r="D19">
+        <v>0.36</v>
+      </c>
+      <c r="E19">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20">
+        <v>0.01</v>
+      </c>
+      <c r="C20">
+        <v>0.02</v>
+      </c>
+      <c r="D20">
+        <v>0.7</v>
+      </c>
+      <c r="E20">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>0.25</v>
+      </c>
+      <c r="C21">
+        <v>0.37</v>
+      </c>
+      <c r="D21">
+        <v>0.06</v>
+      </c>
+      <c r="E21">
+        <v>-0.09</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22">
+        <v>-0.02</v>
+      </c>
+      <c r="C22">
+        <v>0.71</v>
+      </c>
+      <c r="D22">
+        <v>-0.03</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <v>0.02</v>
+      </c>
+      <c r="C23">
+        <v>0.47</v>
+      </c>
+      <c r="D23">
+        <v>0.11</v>
+      </c>
+      <c r="E23">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>0.63</v>
+      </c>
+      <c r="C24">
+        <v>-0.03</v>
+      </c>
+      <c r="D24">
+        <v>0.01</v>
+      </c>
+      <c r="E24">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>0.31</v>
+      </c>
+      <c r="C25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D25">
+        <v>0.03</v>
+      </c>
+      <c r="E25">
+        <v>-0.12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>0.63</v>
+      </c>
+      <c r="C26">
+        <v>0.04</v>
+      </c>
+      <c r="D26">
+        <v>0.03</v>
+      </c>
+      <c r="E26">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>0.36</v>
+      </c>
+      <c r="C27">
+        <v>0.03</v>
+      </c>
+      <c r="D27">
+        <v>-0.08</v>
+      </c>
+      <c r="E27">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <v>0.05</v>
+      </c>
+      <c r="C28">
+        <v>0.24</v>
+      </c>
+      <c r="D28">
+        <v>0.04</v>
+      </c>
+      <c r="E28">
+        <v>-0.09</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>0.04</v>
+      </c>
+      <c r="C29">
+        <v>0.26</v>
+      </c>
+      <c r="D29">
+        <v>0.04</v>
+      </c>
+      <c r="E29">
+        <v>-0.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:K1" xr:uid="{2A2FF23C-A49F-4BBF-A172-E01688A2AD61}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K14">
+      <sortCondition sortBy="cellColor" ref="E1" dxfId="177"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="B2:E14">
+    <cfRule type="cellIs" dxfId="176" priority="2" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:E29">
+    <cfRule type="cellIs" dxfId="175" priority="1" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8FEE297-2283-4876-8A50-4A8E8DF46A81}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -3545,11 +5223,11 @@
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{20237AFA-AF5A-4959-9459-F55DA7A9A145}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H12">
-      <sortCondition sortBy="cellColor" ref="E1" dxfId="28"/>
+      <sortCondition sortBy="cellColor" ref="E1" dxfId="174"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E12">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="173" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3557,13 +5235,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C8C1A-CFC6-49AC-B896-635D55B44BA8}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -3809,16 +5485,16 @@
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{76B16ADE-8397-4523-89E6-FD43024CAE02}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J14">
-      <sortCondition sortBy="cellColor" ref="J1" dxfId="10"/>
+      <sortCondition sortBy="cellColor" ref="J1" dxfId="172"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="171" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="170" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Trying different factoring and rotation methods
</commit_message>
<xml_diff>
--- a/R/Factor analysis  - factor loadings.xlsx
+++ b/R/Factor analysis  - factor loadings.xlsx
@@ -8,25 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\git\AHL\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8CA316-B208-4423-9B00-4DFCD1BEE96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBBECE8-ACE1-4012-AA7A-6110DEF6A1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
   </bookViews>
   <sheets>
     <sheet name="All CAMs" sheetId="1" r:id="rId1"/>
-    <sheet name="All CAMs rotation comparisons" sheetId="7" r:id="rId2"/>
-    <sheet name="Drop prayer and spirit" sheetId="2" r:id="rId3"/>
-    <sheet name="Mysterious Perfect Model" sheetId="3" r:id="rId4"/>
-    <sheet name="Comparing MPM" sheetId="6" r:id="rId5"/>
-    <sheet name="Numeric" sheetId="5" r:id="rId6"/>
+    <sheet name="All ml rotation comparisons" sheetId="7" r:id="rId2"/>
+    <sheet name="Principal Axis Factoring" sheetId="9" r:id="rId3"/>
+    <sheet name="PCA" sheetId="8" r:id="rId4"/>
+    <sheet name="Drop prayer and spirit" sheetId="2" r:id="rId5"/>
+    <sheet name="Mysterious Perfect Model" sheetId="3" r:id="rId6"/>
+    <sheet name="Comparing MPM" sheetId="6" r:id="rId7"/>
+    <sheet name="Numeric" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All CAMs'!$A$1:$AC$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'All CAMs rotation comparisons'!$N$1:$Q$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Comparing MPM'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Drop prayer and spirit'!$A$1:$Q$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Mysterious Perfect Model'!$A$1:$F$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Numeric!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'All ml rotation comparisons'!$Z$1:$AB$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Comparing MPM'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Drop prayer and spirit'!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Mysterious Perfect Model'!$A$1:$F$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Numeric!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">PCA!$B$1:$E$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Principal Axis Factoring'!$H$1:$K$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,6 +58,7 @@
     <author>tc={A97113B4-F367-4C2B-8A94-DB864EFF74E6}</author>
     <author>tc={711727C3-1319-4CF5-ADB3-56CF05FBEC16}</author>
     <author>tc={AF829918-3431-40D2-AA62-05EC558A21CE}</author>
+    <author>tc={E5503793-8E22-4959-AFFA-CEEDA9328B3C}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{47AC028E-CB7A-47F7-9352-0CD18B9CF11D}">
@@ -96,11 +101,55 @@
     All CAMs, promax rotation</t>
       </text>
     </comment>
+    <comment ref="Y1" authorId="5" shapeId="0" xr:uid="{E5503793-8E22-4959-AFFA-CEEDA9328B3C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    All CAMs, maximum likelihood, promax</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={68C2D0A8-62BB-4214-AD84-976C7BE3AB2B}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{68C2D0A8-62BB-4214-AD84-976C7BE3AB2B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    All CAMs, principal axis factoring (pa) with promax rotation</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={F7A5C9D5-E716-4F51-8BD8-AA873D1AD48D}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{F7A5C9D5-E716-4F51-8BD8-AA873D1AD48D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Principal Components with Varimax Rotation</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -135,7 +184,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -195,7 +244,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -255,7 +304,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -291,7 +340,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="36">
   <si>
     <t>ML2</t>
   </si>
@@ -370,6 +419,36 @@
   <si>
     <t xml:space="preserve">bad </t>
   </si>
+  <si>
+    <t>RC4</t>
+  </si>
+  <si>
+    <t>RC1</t>
+  </si>
+  <si>
+    <t>RC2</t>
+  </si>
+  <si>
+    <t>RC3</t>
+  </si>
+  <si>
+    <t>PA1</t>
+  </si>
+  <si>
+    <t>PA3</t>
+  </si>
+  <si>
+    <t>PA2</t>
+  </si>
+  <si>
+    <t>PA4</t>
+  </si>
+  <si>
+    <t>Proportion Explained</t>
+  </si>
+  <si>
+    <t>Cumulative Proportion</t>
+  </si>
 </sst>
 </file>
 
@@ -430,7 +509,71 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="143">
+  <dxfs count="82">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -462,6 +605,118 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -622,6 +877,56 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
@@ -706,6 +1011,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -726,6 +1039,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -756,6 +1077,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -816,6 +1145,22 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -866,940 +1211,50 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
           <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2134,6 +1589,25 @@
   <threadedComment ref="S1" dT="2021-06-08T21:14:23.49" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{AF829918-3431-40D2-AA62-05EC558A21CE}">
     <text>All CAMs, promax rotation</text>
   </threadedComment>
+  <threadedComment ref="Y1" dT="2021-06-09T21:30:53.91" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{E5503793-8E22-4959-AFFA-CEEDA9328B3C}">
+    <text>All CAMs, maximum likelihood, promax</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2021-06-09T21:16:27.69" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{68C2D0A8-62BB-4214-AD84-976C7BE3AB2B}">
+    <text>All CAMs, principal axis factoring (pa) with promax rotation</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2021-06-09T18:37:26.45" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{F7A5C9D5-E716-4F51-8BD8-AA873D1AD48D}">
+    <text>Principal Components with Varimax Rotation</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2141,8 +1615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A59E54-D4A7-4C25-9D11-CD018EBC24D4}">
   <dimension ref="A1:AD21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:N21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3333,43 +2807,43 @@
   </sheetData>
   <autoFilter ref="A1:AC16" xr:uid="{99B320C6-A597-4E1B-B5FD-F0989543660C}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC16">
-      <sortCondition sortBy="cellColor" ref="N1:N16" dxfId="117"/>
+      <sortCondition sortBy="cellColor" ref="N1:N16" dxfId="81"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="Q2:U16">
-    <cfRule type="cellIs" dxfId="126" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="16" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:AC16">
-    <cfRule type="cellIs" dxfId="125" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="79" priority="15" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H16">
-    <cfRule type="cellIs" dxfId="124" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="12" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="6" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C16">
-    <cfRule type="cellIs" dxfId="122" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="11" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="9" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="8" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:N16">
-    <cfRule type="cellIs" dxfId="118" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="2" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3380,10 +2854,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39412BF1-7058-497E-BBA1-3DAA310B3CD4}">
-  <dimension ref="A1:W21"/>
+  <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3394,9 +2868,10 @@
     <col min="13" max="13" width="14.33203125" customWidth="1"/>
     <col min="14" max="14" width="9.06640625" customWidth="1"/>
     <col min="19" max="19" width="14" customWidth="1"/>
+    <col min="25" max="25" width="13.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -3439,8 +2914,17 @@
       <c r="W1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Z1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3489,8 +2973,20 @@
       <c r="W2">
         <v>0.317</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Y2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2">
+        <v>-0.22</v>
+      </c>
+      <c r="AA2">
+        <v>0.379</v>
+      </c>
+      <c r="AB2">
+        <v>0.67400000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3542,8 +3038,17 @@
       <c r="W3">
         <v>0.90700000000000003</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Y3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA3">
+        <v>-0.28699999999999998</v>
+      </c>
+      <c r="AB3">
+        <v>1.109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3595,8 +3100,20 @@
       <c r="W4">
         <v>-0.216</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Y4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z4">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="AA4">
+        <v>0.623</v>
+      </c>
+      <c r="AB4">
+        <v>-0.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -3642,8 +3159,20 @@
       <c r="W5">
         <v>0.22600000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Y5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z5">
+        <v>0.113</v>
+      </c>
+      <c r="AA5">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="AB5">
+        <v>0.107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -3689,8 +3218,17 @@
       <c r="U6">
         <v>0.33200000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Y6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA6">
+        <v>0.76</v>
+      </c>
+      <c r="AB6">
+        <v>0.104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -3733,8 +3271,20 @@
       <c r="U7">
         <v>0.71899999999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Y7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z7">
+        <v>-0.17799999999999999</v>
+      </c>
+      <c r="AA7">
+        <v>1.1850000000000001</v>
+      </c>
+      <c r="AB7">
+        <v>-0.115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -3786,8 +3336,14 @@
       <c r="W8">
         <v>0.13500000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Y8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z8">
+        <v>0.66400000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -3833,8 +3389,17 @@
       <c r="V9">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Y9" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z9">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="AA9">
+        <v>-0.157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -3883,8 +3448,20 @@
       <c r="V10">
         <v>-0.11</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Y10" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z10">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="AA10">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="AB10">
+        <v>0.24399999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -3918,8 +3495,17 @@
       <c r="T11">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Y11" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z11">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="AA11">
+        <v>0.26400000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3959,8 +3545,14 @@
       <c r="U12">
         <v>0.20300000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Y12" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z12">
+        <v>0.86599999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -4000,8 +3592,14 @@
       <c r="T13">
         <v>0.88700000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Y13" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z13">
+        <v>0.63400000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -4044,8 +3642,14 @@
       <c r="W14">
         <v>-0.125</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Y14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z14">
+        <v>0.86299999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -4088,8 +3692,17 @@
       <c r="T15">
         <v>0.86099999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Y15" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z15">
+        <v>0.51</v>
+      </c>
+      <c r="AA15">
+        <v>0.216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -4138,8 +3751,20 @@
       <c r="V16">
         <v>0.16400000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Y16" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z16">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="AA16">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="AB16">
+        <v>0.13600000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>1</v>
       </c>
@@ -4183,8 +3808,17 @@
       <c r="W18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Z18" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -4242,8 +3876,20 @@
       <c r="W19">
         <v>1.079</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Y19" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z19">
+        <v>3.5409999999999999</v>
+      </c>
+      <c r="AA19">
+        <v>3.0019999999999998</v>
+      </c>
+      <c r="AB19">
+        <v>1.8240000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -4301,8 +3947,20 @@
       <c r="W20">
         <v>7.1999999999999995E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="Y20" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z20">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="AA20">
+        <v>0.2</v>
+      </c>
+      <c r="AB20">
+        <v>0.122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.45">
       <c r="G21" t="s">
         <v>24</v>
       </c>
@@ -4348,43 +4006,60 @@
       <c r="W21">
         <v>0.56999999999999995</v>
       </c>
+      <c r="Y21" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z21">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="AA21">
+        <v>0.436</v>
+      </c>
+      <c r="AB21">
+        <v>0.55800000000000005</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="N1:Q16" xr:uid="{39412BF1-7058-497E-BBA1-3DAA310B3CD4}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N2:Q16">
-      <sortCondition sortBy="cellColor" ref="Q1:Q16" dxfId="20"/>
+  <autoFilter ref="Z1:AB16" xr:uid="{39412BF1-7058-497E-BBA1-3DAA310B3CD4}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Z2:AB16">
+      <sortCondition sortBy="cellColor" ref="AB1:AB16" dxfId="20"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:B16">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="8" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E16">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K16">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:P4 N2 P2 N3:O3 N6:Q6 N5:O5 Q5 N10:Q12 N7:N8 P7:Q8 O9:Q9 N14:Q16 N13 P13:Q13">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:W16 T2:V2 T3:U4 W3:W4">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:Q16">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="2" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z2:AB16">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4395,6 +4070,935 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5509DC-DB05-43E6-A45B-32E76BC27DEA}">
+  <dimension ref="A1:K23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="7" max="7" width="13.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>-0.02</v>
+      </c>
+      <c r="C2">
+        <v>0.51</v>
+      </c>
+      <c r="D2">
+        <v>-0.16</v>
+      </c>
+      <c r="E2">
+        <v>0.39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="I2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K2">
+        <v>0.59699999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0.39</v>
+      </c>
+      <c r="C3">
+        <v>0.18</v>
+      </c>
+      <c r="D3">
+        <v>-0.12</v>
+      </c>
+      <c r="E3">
+        <v>0.35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>0.86399999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0.03</v>
+      </c>
+      <c r="C4">
+        <v>0.04</v>
+      </c>
+      <c r="D4">
+        <v>-0.05</v>
+      </c>
+      <c r="E4">
+        <v>0.81</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>0.157</v>
+      </c>
+      <c r="J4">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="K4">
+        <v>-0.123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0.18</v>
+      </c>
+      <c r="C5">
+        <v>-0.04</v>
+      </c>
+      <c r="D5">
+        <v>0.26</v>
+      </c>
+      <c r="E5">
+        <v>0.31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="I5">
+        <v>0.495</v>
+      </c>
+      <c r="J5">
+        <v>0.13500000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>-0.2</v>
+      </c>
+      <c r="C6">
+        <v>0.09</v>
+      </c>
+      <c r="D6">
+        <v>0.92</v>
+      </c>
+      <c r="E6">
+        <v>0.06</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="J6">
+        <v>-0.153</v>
+      </c>
+      <c r="K6">
+        <v>0.182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0.06</v>
+      </c>
+      <c r="C7">
+        <v>0.1</v>
+      </c>
+      <c r="D7">
+        <v>0.8</v>
+      </c>
+      <c r="E7">
+        <v>-0.17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="I7">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="K7">
+        <v>-0.32200000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0.35</v>
+      </c>
+      <c r="C8">
+        <v>0.45</v>
+      </c>
+      <c r="D8">
+        <v>0.17</v>
+      </c>
+      <c r="E8">
+        <v>0.12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="J8">
+        <v>0.14099999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0.26</v>
+      </c>
+      <c r="C9">
+        <v>0.54</v>
+      </c>
+      <c r="D9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E9">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="J9">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>-0.06</v>
+      </c>
+      <c r="C10">
+        <v>0.71</v>
+      </c>
+      <c r="D10">
+        <v>0.17</v>
+      </c>
+      <c r="E10">
+        <v>0.2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>0.66</v>
+      </c>
+      <c r="I10">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="J10">
+        <v>-0.123</v>
+      </c>
+      <c r="K10">
+        <v>-0.221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>-0.17</v>
+      </c>
+      <c r="C11">
+        <v>0.81</v>
+      </c>
+      <c r="D11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E11">
+        <v>0.26</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="J11">
+        <v>-0.13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0.71</v>
+      </c>
+      <c r="C12">
+        <v>0.25</v>
+      </c>
+      <c r="D12">
+        <v>-0.09</v>
+      </c>
+      <c r="E12">
+        <v>-0.2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12">
+        <v>0.84899999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0.48</v>
+      </c>
+      <c r="C13">
+        <v>0.01</v>
+      </c>
+      <c r="D13">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0.08</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="J13">
+        <v>0.184</v>
+      </c>
+      <c r="K13">
+        <v>0.19600000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0.82</v>
+      </c>
+      <c r="C14">
+        <v>-0.02</v>
+      </c>
+      <c r="D14">
+        <v>0.1</v>
+      </c>
+      <c r="E14">
+        <v>0.02</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14">
+        <v>0.85499999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>0.46</v>
+      </c>
+      <c r="C15">
+        <v>-0.12</v>
+      </c>
+      <c r="D15">
+        <v>0.18</v>
+      </c>
+      <c r="E15">
+        <v>0.24</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="I15">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="J15">
+        <v>-0.107</v>
+      </c>
+      <c r="K15">
+        <v>0.20499999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>0.81</v>
+      </c>
+      <c r="C16">
+        <v>-0.1</v>
+      </c>
+      <c r="D16">
+        <v>0.09</v>
+      </c>
+      <c r="E16">
+        <v>0.13</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="J16">
+        <v>0.26</v>
+      </c>
+      <c r="K16">
+        <v>0.23899999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" t="s">
+        <v>32</v>
+      </c>
+      <c r="K18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>2.54</v>
+      </c>
+      <c r="D19">
+        <v>1.92</v>
+      </c>
+      <c r="E19">
+        <v>1.73</v>
+      </c>
+      <c r="G19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19">
+        <v>3.01</v>
+      </c>
+      <c r="I19">
+        <v>2.5329999999999999</v>
+      </c>
+      <c r="J19">
+        <v>1.51</v>
+      </c>
+      <c r="K19">
+        <v>0.71199999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>0.2</v>
+      </c>
+      <c r="C20">
+        <v>0.17</v>
+      </c>
+      <c r="D20">
+        <v>0.13</v>
+      </c>
+      <c r="E20">
+        <v>0.12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="I20">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="J20">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="K20">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>0.2</v>
+      </c>
+      <c r="C21">
+        <v>0.37</v>
+      </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+      <c r="E21">
+        <v>0.61</v>
+      </c>
+      <c r="G21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="I21">
+        <v>0.37</v>
+      </c>
+      <c r="J21">
+        <v>0.47</v>
+      </c>
+      <c r="K21">
+        <v>0.51800000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22">
+        <v>0.33</v>
+      </c>
+      <c r="C22">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D22">
+        <v>0.21</v>
+      </c>
+      <c r="E22">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23">
+        <v>0.33</v>
+      </c>
+      <c r="C23">
+        <v>0.6</v>
+      </c>
+      <c r="D23">
+        <v>0.81</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="H1:K16" xr:uid="{8B5509DC-DB05-43E6-A45B-32E76BC27DEA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:K16">
+      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="1"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="B2:E16">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:K16">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4883B1BD-E07A-48BB-9F66-A8C7003F2BEF}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.46484375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>0.21</v>
+      </c>
+      <c r="C2">
+        <v>0.62</v>
+      </c>
+      <c r="D2">
+        <v>0.31</v>
+      </c>
+      <c r="E2">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0.23</v>
+      </c>
+      <c r="C3">
+        <v>0.59</v>
+      </c>
+      <c r="D3">
+        <v>0.24</v>
+      </c>
+      <c r="E3">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0.63</v>
+      </c>
+      <c r="C4">
+        <v>0.12</v>
+      </c>
+      <c r="D4">
+        <v>-0.04</v>
+      </c>
+      <c r="E4">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0.12</v>
+      </c>
+      <c r="C5">
+        <v>0.3</v>
+      </c>
+      <c r="D5">
+        <v>0.22</v>
+      </c>
+      <c r="E5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0.2</v>
+      </c>
+      <c r="C6">
+        <v>0.05</v>
+      </c>
+      <c r="D6">
+        <v>0.27</v>
+      </c>
+      <c r="E6">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0.25</v>
+      </c>
+      <c r="C7">
+        <v>0.52</v>
+      </c>
+      <c r="D7">
+        <v>0.52</v>
+      </c>
+      <c r="E7">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0.66</v>
+      </c>
+      <c r="C8">
+        <v>0.26</v>
+      </c>
+      <c r="D8">
+        <v>0.51</v>
+      </c>
+      <c r="E8">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0.17</v>
+      </c>
+      <c r="C9">
+        <v>-0.04</v>
+      </c>
+      <c r="D9">
+        <v>0.78</v>
+      </c>
+      <c r="E9">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0.06</v>
+      </c>
+      <c r="C10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.81</v>
+      </c>
+      <c r="E10">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0.2</v>
+      </c>
+      <c r="C11">
+        <v>0.72</v>
+      </c>
+      <c r="D11">
+        <v>0.23</v>
+      </c>
+      <c r="E11">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0.11</v>
+      </c>
+      <c r="C12">
+        <v>0.71</v>
+      </c>
+      <c r="D12">
+        <v>-0.1</v>
+      </c>
+      <c r="E12">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0.49</v>
+      </c>
+      <c r="C13">
+        <v>0.54</v>
+      </c>
+      <c r="D13">
+        <v>0.04</v>
+      </c>
+      <c r="E13">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0.82</v>
+      </c>
+      <c r="C14">
+        <v>0.2</v>
+      </c>
+      <c r="D14">
+        <v>0.05</v>
+      </c>
+      <c r="E14">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>0.53</v>
+      </c>
+      <c r="C15">
+        <v>0.48</v>
+      </c>
+      <c r="D15">
+        <v>0.47</v>
+      </c>
+      <c r="E15">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>0.72</v>
+      </c>
+      <c r="C16">
+        <v>0.22</v>
+      </c>
+      <c r="D16">
+        <v>0.48</v>
+      </c>
+      <c r="E16">
+        <v>0.18</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E16" xr:uid="{4883B1BD-E07A-48BB-9F66-A8C7003F2BEF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E16">
+      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="47"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="B2:E16">
+    <cfRule type="cellIs" dxfId="40" priority="1" operator="greaterThan">
+      <formula>0.699</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D61808F-2A1D-4F74-9E35-43CB27586058}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
@@ -5027,30 +5631,30 @@
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{85F09F99-28C1-4BB1-A75C-F2C0B1518057}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q14">
-      <sortCondition sortBy="cellColor" ref="D1" dxfId="116"/>
+      <sortCondition sortBy="cellColor" ref="D1" dxfId="70"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="M2:Q14">
-    <cfRule type="cellIs" dxfId="142" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="69" priority="6" operator="lessThan">
       <formula>-0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="140" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="4" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="138" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="3" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5059,7 +5663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8727E6E-4063-4F85-BAE5-AB6F095D427F}">
   <dimension ref="A1:K14"/>
   <sheetViews>
@@ -5494,21 +6098,21 @@
   </sheetData>
   <autoFilter ref="A1:F14" xr:uid="{F6EC43A2-0E96-4311-A986-12EE04542C46}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
-      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="136"/>
+      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="63"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:E1048576">
-    <cfRule type="cellIs" dxfId="135" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:K1">
-    <cfRule type="cellIs" dxfId="134" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K12">
-    <cfRule type="cellIs" dxfId="133" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5517,7 +6121,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC6BCC2-AE82-430A-9446-637AC6346772}">
   <dimension ref="A1:E29"/>
   <sheetViews>
@@ -5936,16 +6540,16 @@
   </sheetData>
   <autoFilter ref="A1:K1" xr:uid="{2A2FF23C-A49F-4BBF-A172-E01688A2AD61}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K14">
-      <sortCondition sortBy="cellColor" ref="E1" dxfId="132"/>
+      <sortCondition sortBy="cellColor" ref="E1" dxfId="59"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E14">
-    <cfRule type="cellIs" dxfId="131" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:E29">
-    <cfRule type="cellIs" dxfId="130" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5954,7 +6558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C8C1A-CFC6-49AC-B896-635D55B44BA8}">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -6204,16 +6808,16 @@
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{76B16ADE-8397-4523-89E6-FD43024CAE02}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J14">
-      <sortCondition sortBy="cellColor" ref="J1" dxfId="129"/>
+      <sortCondition sortBy="cellColor" ref="J1" dxfId="56"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="128" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="127" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Comparing models - drop prayer, spirit, energy
Created data frame to compare models. Running factor solutions with different rotations.
</commit_message>
<xml_diff>
--- a/R/Factor analysis  - factor loadings.xlsx
+++ b/R/Factor analysis  - factor loadings.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\git\AHL\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBBECE8-ACE1-4012-AA7A-6110DEF6A1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654D0275-8DFC-4A0C-B2BB-D31100F54ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
   </bookViews>
   <sheets>
     <sheet name="All CAMs" sheetId="1" r:id="rId1"/>
-    <sheet name="All ml rotation comparisons" sheetId="7" r:id="rId2"/>
+    <sheet name="Drop energy, pray, spirit" sheetId="10" r:id="rId2"/>
     <sheet name="Principal Axis Factoring" sheetId="9" r:id="rId3"/>
     <sheet name="PCA" sheetId="8" r:id="rId4"/>
     <sheet name="Drop prayer and spirit" sheetId="2" r:id="rId5"/>
@@ -24,8 +24,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All CAMs'!$A$1:$AC$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'All ml rotation comparisons'!$Z$1:$AB$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Comparing MPM'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Drop energy, pray, spirit'!$A$15:$S$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Drop prayer and spirit'!$A$1:$Q$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Mysterious Perfect Model'!$A$1:$F$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Numeric!$A$1:$J$1</definedName>
@@ -53,60 +53,100 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={47AC028E-CB7A-47F7-9352-0CD18B9CF11D}</author>
-    <author>tc={DB44D446-E5BA-4494-881B-A3A0DA5D608C}</author>
-    <author>tc={A97113B4-F367-4C2B-8A94-DB864EFF74E6}</author>
-    <author>tc={711727C3-1319-4CF5-ADB3-56CF05FBEC16}</author>
-    <author>tc={AF829918-3431-40D2-AA62-05EC558A21CE}</author>
-    <author>tc={E5503793-8E22-4959-AFFA-CEEDA9328B3C}</author>
+    <author>tc={05F861C7-3F05-45BE-A842-A70399D00986}</author>
+    <author>tc={15ED4DD3-15BC-4E0F-AD77-76216B25453F}</author>
+    <author>hanna</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{47AC028E-CB7A-47F7-9352-0CD18B9CF11D}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{05F861C7-3F05-45BE-A842-A70399D00986}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    All vars with varimax rotation</t>
+    Maximum likelihood, varimax</t>
       </text>
     </comment>
-    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{DB44D446-E5BA-4494-881B-A3A0DA5D608C}">
+    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{15ED4DD3-15BC-4E0F-AD77-76216B25453F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    All vars oblique rotation (oblimin)</t>
+    Maximum Likelihood, Promax</t>
       </text>
     </comment>
-    <comment ref="G1" authorId="2" shapeId="0" xr:uid="{A97113B4-F367-4C2B-8A94-DB864EFF74E6}">
+    <comment ref="K1" authorId="2" shapeId="0" xr:uid="{18A6050E-C695-43D0-A03E-6E6657D76CB3}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    All CAMs, oblimin rotation</t>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Maximum likelihood, 
+oblimin</t>
+        </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="3" shapeId="0" xr:uid="{711727C3-1319-4CF5-ADB3-56CF05FBEC16}">
+    <comment ref="P1" authorId="2" shapeId="0" xr:uid="{4B4AE082-A14D-4714-A595-1E92FDAD6FAB}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    All CAMs, varimax rotation</t>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Maximum likelihood, cluster rotation
+</t>
+        </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="4" shapeId="0" xr:uid="{AF829918-3431-40D2-AA62-05EC558A21CE}">
+    <comment ref="A15" authorId="2" shapeId="0" xr:uid="{F41A4B08-9370-41CE-9CC4-CC0C2D2A73C7}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    All CAMs, promax rotation</t>
-      </text>
-    </comment>
-    <comment ref="Y1" authorId="5" shapeId="0" xr:uid="{E5503793-8E22-4959-AFFA-CEEDA9328B3C}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    All CAMs, maximum likelihood, promax</t>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Maximum likelihood, varimax
+</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -340,7 +380,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="36">
   <si>
     <t>ML2</t>
   </si>
@@ -476,10 +516,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -509,7 +549,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="82">
+  <dxfs count="70">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -605,6 +645,66 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
@@ -653,6 +753,36 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
@@ -717,6 +847,54 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -927,6 +1105,46 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
@@ -955,298 +1173,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
           <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1574,23 +1500,11 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A1" dT="2021-06-08T21:00:27.95" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{47AC028E-CB7A-47F7-9352-0CD18B9CF11D}">
-    <text>All vars with varimax rotation</text>
+  <threadedComment ref="A1" dT="2021-06-12T19:29:21.77" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{05F861C7-3F05-45BE-A842-A70399D00986}">
+    <text>Maximum likelihood, varimax</text>
   </threadedComment>
-  <threadedComment ref="D1" dT="2021-06-08T21:02:29.86" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{DB44D446-E5BA-4494-881B-A3A0DA5D608C}">
-    <text>All vars oblique rotation (oblimin)</text>
-  </threadedComment>
-  <threadedComment ref="G1" dT="2021-06-08T21:12:13.03" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{A97113B4-F367-4C2B-8A94-DB864EFF74E6}">
-    <text>All CAMs, oblimin rotation</text>
-  </threadedComment>
-  <threadedComment ref="M1" dT="2021-06-08T21:12:23.05" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{711727C3-1319-4CF5-ADB3-56CF05FBEC16}">
-    <text>All CAMs, varimax rotation</text>
-  </threadedComment>
-  <threadedComment ref="S1" dT="2021-06-08T21:14:23.49" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{AF829918-3431-40D2-AA62-05EC558A21CE}">
-    <text>All CAMs, promax rotation</text>
-  </threadedComment>
-  <threadedComment ref="Y1" dT="2021-06-09T21:30:53.91" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{E5503793-8E22-4959-AFFA-CEEDA9328B3C}">
-    <text>All CAMs, maximum likelihood, promax</text>
+  <threadedComment ref="F1" dT="2021-06-12T19:33:56.63" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{15ED4DD3-15BC-4E0F-AD77-76216B25453F}">
+    <text>Maximum Likelihood, Promax</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1615,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A59E54-D4A7-4C25-9D11-CD018EBC24D4}">
   <dimension ref="A1:AD21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2807,44 +2721,44 @@
   </sheetData>
   <autoFilter ref="A1:AC16" xr:uid="{99B320C6-A597-4E1B-B5FD-F0989543660C}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC16">
-      <sortCondition sortBy="cellColor" ref="N1:N16" dxfId="81"/>
+      <sortCondition sortBy="cellColor" ref="N1:N16" dxfId="38"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="Q2:U16">
-    <cfRule type="cellIs" dxfId="80" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="16" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:AC16">
-    <cfRule type="cellIs" dxfId="79" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="15" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H16">
-    <cfRule type="cellIs" dxfId="78" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="6" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="12" operator="greaterThan">
       <formula>0.499</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="6" operator="greaterThan">
-      <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C16">
-    <cfRule type="cellIs" dxfId="76" priority="11" operator="greaterThan">
-      <formula>0.499</formula>
+    <cfRule type="cellIs" dxfId="60" priority="8" operator="greaterThan">
+      <formula>0.399</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="9" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="8" operator="greaterThan">
-      <formula>0.399</formula>
+    <cfRule type="cellIs" dxfId="58" priority="11" operator="greaterThan">
+      <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:N16">
-    <cfRule type="cellIs" dxfId="73" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="1" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="2" operator="greaterThan">
       <formula>0.499</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="1" operator="greaterThan">
-      <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2853,1219 +2767,768 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39412BF1-7058-497E-BBA1-3DAA310B3CD4}">
-  <dimension ref="A1:AB21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DF5018-9911-4233-8E1E-CFEBD8577F16}">
+  <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.1328125" customWidth="1"/>
-    <col min="4" max="4" width="13.86328125" customWidth="1"/>
-    <col min="7" max="7" width="13.265625" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" customWidth="1"/>
-    <col min="14" max="14" width="9.06640625" customWidth="1"/>
-    <col min="19" max="19" width="14" customWidth="1"/>
-    <col min="25" max="25" width="13.46484375" customWidth="1"/>
+    <col min="1" max="1" width="13.86328125" customWidth="1"/>
+    <col min="6" max="6" width="13.265625" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="16" max="16" width="12.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
         <v>0</v>
       </c>
-      <c r="J1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
       <c r="N1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P1" t="s">
         <v>1</v>
       </c>
       <c r="Q1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
+      <c r="R1" t="s">
         <v>0</v>
       </c>
-      <c r="V1" t="s">
+      <c r="S1" t="s">
         <v>1</v>
       </c>
-      <c r="W1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.628</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>0.628</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="C2">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>0.317</v>
+      </c>
+      <c r="H2">
+        <v>0.13600000000000001</v>
       </c>
       <c r="I2">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="J2">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="K2">
-        <v>0.72899999999999998</v>
-      </c>
-      <c r="M2" t="s">
-        <v>2</v>
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="M2">
+        <v>0.16200000000000001</v>
       </c>
       <c r="N2">
-        <v>0.20599999999999999</v>
-      </c>
-      <c r="O2">
-        <v>0.20300000000000001</v>
-      </c>
-      <c r="P2">
-        <v>0.35699999999999998</v>
-      </c>
-      <c r="Q2">
-        <v>0.88500000000000001</v>
-      </c>
-      <c r="S2" t="s">
-        <v>2</v>
-      </c>
-      <c r="V2">
-        <v>0.89300000000000002</v>
-      </c>
-      <c r="W2">
-        <v>0.317</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z2">
-        <v>-0.22</v>
-      </c>
-      <c r="AA2">
-        <v>0.379</v>
-      </c>
-      <c r="AB2">
-        <v>0.67400000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.45">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="P2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2">
+        <v>1.048</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.60899999999999999</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>0.60899999999999999</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>0.41</v>
+        <v>0.192</v>
+      </c>
+      <c r="C3">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="D3">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
       </c>
       <c r="I3">
-        <v>0.40500000000000003</v>
-      </c>
-      <c r="J3">
-        <v>0.311</v>
-      </c>
-      <c r="K3">
-        <v>-0.13100000000000001</v>
-      </c>
-      <c r="M3" t="s">
-        <v>3</v>
+        <v>1.0640000000000001</v>
+      </c>
+      <c r="K3" t="s">
+        <v>6</v>
       </c>
       <c r="N3">
-        <v>0.56399999999999995</v>
-      </c>
-      <c r="O3">
-        <v>0.59899999999999998</v>
-      </c>
-      <c r="P3">
-        <v>0.13900000000000001</v>
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="P3" t="s">
+        <v>12</v>
       </c>
       <c r="Q3">
-        <v>0.34699999999999998</v>
-      </c>
-      <c r="S3" t="s">
-        <v>3</v>
-      </c>
-      <c r="V3">
-        <v>0.32600000000000001</v>
-      </c>
-      <c r="W3">
-        <v>0.90700000000000003</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA3">
-        <v>-0.28699999999999998</v>
-      </c>
-      <c r="AB3">
-        <v>1.109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.45">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="R3">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="S3">
+        <v>0.40899999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.38100000000000001</v>
-      </c>
-      <c r="D4" t="s">
+        <v>0.39</v>
+      </c>
+      <c r="D4">
+        <v>0.188</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="I4">
+        <v>0.21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="N4">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="P4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="S4">
+        <v>0.318</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="C5">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="D5">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="H5">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="I5">
+        <v>-0.23899999999999999</v>
+      </c>
+      <c r="K5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="M5">
+        <v>0.505</v>
+      </c>
+      <c r="N5">
+        <v>-0.19600000000000001</v>
+      </c>
+      <c r="P5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R5">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="S5">
+        <v>0.24099999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="C6">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.221</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <v>0.83</v>
+      </c>
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="P6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q6">
+        <v>0.161</v>
+      </c>
+      <c r="R6">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="S6">
+        <v>-0.16600000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="C7">
+        <v>0.255</v>
+      </c>
+      <c r="D7">
+        <v>0.246</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7">
+        <v>1.0389999999999999</v>
+      </c>
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="P7" t="s">
+        <v>11</v>
+      </c>
+      <c r="R7">
+        <v>0.82</v>
+      </c>
+      <c r="S7">
+        <v>0.11799999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="C8">
+        <v>0.308</v>
+      </c>
+      <c r="D8">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="I8">
+        <v>-0.218</v>
+      </c>
+      <c r="K8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="M8">
+        <v>0.109</v>
+      </c>
+      <c r="N8">
+        <v>-0.158</v>
+      </c>
+      <c r="P8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q8">
+        <v>-0.12</v>
+      </c>
+      <c r="R8">
+        <v>1.024</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="C9">
+        <v>0.501</v>
+      </c>
+      <c r="F9" t="s">
         <v>4</v>
       </c>
-      <c r="E4">
-        <v>0.38100000000000001</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4">
-        <v>0.96</v>
-      </c>
-      <c r="K4">
-        <v>0.11</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="G9">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="H9">
+        <v>-0.156</v>
+      </c>
+      <c r="I9">
+        <v>0.113</v>
+      </c>
+      <c r="K9" t="s">
         <v>4</v>
       </c>
-      <c r="N4">
-        <v>0.191</v>
-      </c>
-      <c r="O4">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="P4">
-        <v>0.874</v>
-      </c>
-      <c r="Q4">
-        <v>0.39200000000000002</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="L9">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="M9">
+        <v>-0.126</v>
+      </c>
+      <c r="N9">
+        <v>0.124</v>
+      </c>
+      <c r="P9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="R9">
+        <v>0.11700000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="K10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="P10" t="s">
         <v>4</v>
       </c>
-      <c r="T4">
-        <v>-0.13</v>
-      </c>
-      <c r="U4">
-        <v>0.999</v>
-      </c>
-      <c r="V4">
-        <v>0.316</v>
-      </c>
-      <c r="W4">
-        <v>-0.216</v>
-      </c>
-      <c r="Y4" t="s">
+      <c r="Q10">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="R10">
+        <v>-0.14499999999999999</v>
+      </c>
+      <c r="S10">
+        <v>0.17799999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="C11">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="D11">
+        <v>0.45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="K11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L11">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="N11">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="P11" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q11">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="S11">
+        <v>0.112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="C12">
+        <v>0.89</v>
+      </c>
+      <c r="D12">
+        <v>0.254</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="K12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12">
+        <v>0.875</v>
+      </c>
+      <c r="P12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q12">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="S12">
+        <v>0.17899999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="C13">
+        <v>0.253</v>
+      </c>
+      <c r="D13">
+        <v>0.35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="I13">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="K13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="M13">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="N13">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="P13" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q13">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="S13">
+        <v>0.13800000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="C16">
+        <v>0.24</v>
+      </c>
+      <c r="D16">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="E16">
+        <v>0.59699999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>0.312</v>
+      </c>
+      <c r="C17">
+        <v>0.498</v>
+      </c>
+      <c r="E17">
+        <v>0.40699999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>0.3</v>
+      </c>
+      <c r="C18">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="D18">
+        <v>0.154</v>
+      </c>
+      <c r="E18">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="C19">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="D19">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="E19">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>4</v>
       </c>
-      <c r="Z4">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="AA4">
-        <v>0.623</v>
-      </c>
-      <c r="AB4">
-        <v>-0.12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>0.90300000000000002</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>0.90300000000000002</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="C20">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="E20">
+        <v>0.66500000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="C21">
+        <v>0.42</v>
+      </c>
+      <c r="D21">
+        <v>0.33800000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
         <v>3</v>
       </c>
-      <c r="I5">
-        <v>0.63800000000000001</v>
-      </c>
-      <c r="K5">
-        <v>-0.16400000000000001</v>
-      </c>
-      <c r="M5" t="s">
-        <v>5</v>
-      </c>
-      <c r="N5">
-        <v>0.27700000000000002</v>
-      </c>
-      <c r="O5">
-        <v>0.85299999999999998</v>
-      </c>
-      <c r="P5">
-        <v>0.435</v>
-      </c>
-      <c r="S5" t="s">
-        <v>5</v>
-      </c>
-      <c r="T5">
-        <v>0.36499999999999999</v>
-      </c>
-      <c r="U5">
-        <v>0.47399999999999998</v>
-      </c>
-      <c r="W5">
-        <v>0.22600000000000001</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z5">
-        <v>0.113</v>
-      </c>
-      <c r="AA5">
-        <v>0.38900000000000001</v>
-      </c>
-      <c r="AB5">
+      <c r="B22">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="C22">
+        <v>0.153</v>
+      </c>
+      <c r="D22">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="E22">
+        <v>0.21299999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>0.214</v>
+      </c>
+      <c r="C23">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="D23">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="E23">
+        <v>0.224</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24">
+        <v>0.754</v>
+      </c>
+      <c r="C24">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="D24">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="E24">
         <v>0.107</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>0.61599999999999999</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6">
-        <v>0.61599999999999999</v>
-      </c>
-      <c r="G6" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>0.219</v>
+      </c>
+      <c r="C25">
+        <v>0.66</v>
+      </c>
+      <c r="D25">
+        <v>0.219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
         <v>10</v>
       </c>
-      <c r="I6">
-        <v>0.505</v>
-      </c>
-      <c r="J6">
-        <v>0.223</v>
-      </c>
-      <c r="K6">
-        <v>-0.22</v>
-      </c>
-      <c r="M6" t="s">
-        <v>6</v>
-      </c>
-      <c r="N6">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="O6">
-        <v>0.33</v>
-      </c>
-      <c r="P6">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="S6" t="s">
-        <v>6</v>
-      </c>
-      <c r="T6">
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="U6">
-        <v>0.33200000000000002</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA6">
-        <v>0.76</v>
-      </c>
-      <c r="AB6">
-        <v>0.104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>0.79500000000000004</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7">
-        <v>0.79500000000000004</v>
-      </c>
-      <c r="G7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7">
-        <v>0.75900000000000001</v>
-      </c>
-      <c r="J7">
-        <v>0.16300000000000001</v>
-      </c>
-      <c r="M7" t="s">
-        <v>7</v>
-      </c>
-      <c r="N7">
-        <v>0.80900000000000005</v>
-      </c>
-      <c r="O7">
-        <v>0.317</v>
-      </c>
-      <c r="P7">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="Q7">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="S7" t="s">
-        <v>7</v>
-      </c>
-      <c r="U7">
-        <v>0.71899999999999997</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z7">
-        <v>-0.17799999999999999</v>
-      </c>
-      <c r="AA7">
-        <v>1.1850000000000001</v>
-      </c>
-      <c r="AB7">
-        <v>-0.115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>0.61499999999999999</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <v>0.61499999999999999</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="B26">
+        <v>0.495</v>
+      </c>
+      <c r="C26">
+        <v>0.24</v>
+      </c>
+      <c r="E26">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>14</v>
       </c>
-      <c r="I8">
-        <v>0.99199999999999999</v>
-      </c>
-      <c r="J8">
-        <v>-0.11</v>
-      </c>
-      <c r="K8">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="M8" t="s">
-        <v>8</v>
-      </c>
-      <c r="N8">
-        <v>0.79300000000000004</v>
-      </c>
-      <c r="O8">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="P8">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="Q8">
-        <v>0.155</v>
-      </c>
-      <c r="S8" t="s">
-        <v>8</v>
-      </c>
-      <c r="U8">
-        <v>0.59799999999999998</v>
-      </c>
-      <c r="V8">
-        <v>-0.11</v>
-      </c>
-      <c r="W8">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z8">
-        <v>0.66400000000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>0.77800000000000002</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9">
-        <v>0.77800000000000002</v>
-      </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9">
-        <v>0.77200000000000002</v>
-      </c>
-      <c r="J9">
-        <v>-0.13500000000000001</v>
-      </c>
-      <c r="K9">
-        <v>0.191</v>
-      </c>
-      <c r="M9" t="s">
-        <v>9</v>
-      </c>
-      <c r="N9">
-        <v>0.505</v>
-      </c>
-      <c r="O9">
-        <v>0.435</v>
-      </c>
-      <c r="Q9">
-        <v>0.129</v>
-      </c>
-      <c r="S9" t="s">
-        <v>9</v>
-      </c>
-      <c r="U9">
-        <v>0.81699999999999995</v>
-      </c>
-      <c r="V9">
-        <v>0.11</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z9">
-        <v>0.55500000000000005</v>
-      </c>
-      <c r="AA9">
-        <v>-0.157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>0.53800000000000003</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10">
-        <v>0.53800000000000003</v>
-      </c>
-      <c r="G10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10">
-        <v>0.39200000000000002</v>
-      </c>
-      <c r="K10">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="M10" t="s">
-        <v>10</v>
-      </c>
-      <c r="N10">
-        <v>0.33100000000000002</v>
-      </c>
-      <c r="O10">
-        <v>0.753</v>
-      </c>
-      <c r="P10">
-        <v>0.24</v>
-      </c>
-      <c r="Q10">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="S10" t="s">
-        <v>10</v>
-      </c>
-      <c r="T10">
-        <v>0.59599999999999997</v>
-      </c>
-      <c r="U10">
-        <v>0.151</v>
-      </c>
-      <c r="V10">
-        <v>-0.11</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z10">
-        <v>0.48199999999999998</v>
-      </c>
-      <c r="AA10">
-        <v>0.29499999999999998</v>
-      </c>
-      <c r="AB10">
-        <v>0.24399999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>0.81899999999999995</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11">
-        <v>0.81899999999999995</v>
-      </c>
-      <c r="G11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11">
+      <c r="B27">
         <v>0.88600000000000001</v>
       </c>
-      <c r="M11" t="s">
-        <v>11</v>
-      </c>
-      <c r="N11">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="O11">
-        <v>0.62</v>
-      </c>
-      <c r="S11" t="s">
-        <v>11</v>
-      </c>
-      <c r="T11">
-        <v>0.51</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z11">
-        <v>0.42299999999999999</v>
-      </c>
-      <c r="AA11">
-        <v>0.26400000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>0.66900000000000004</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12">
-        <v>0.66900000000000004</v>
-      </c>
-      <c r="G12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12">
-        <v>0.85899999999999999</v>
-      </c>
-      <c r="M12" t="s">
-        <v>12</v>
-      </c>
-      <c r="N12">
-        <v>0.219</v>
-      </c>
-      <c r="O12">
-        <v>0.53500000000000003</v>
-      </c>
-      <c r="Q12">
-        <v>0.21</v>
-      </c>
-      <c r="S12" t="s">
-        <v>12</v>
-      </c>
-      <c r="T12">
-        <v>0.441</v>
-      </c>
-      <c r="U12">
-        <v>0.20300000000000001</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z12">
-        <v>0.86599999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13">
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="G13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13">
-        <v>0.46700000000000003</v>
-      </c>
-      <c r="I13">
-        <v>0.20300000000000001</v>
-      </c>
-      <c r="M13" t="s">
-        <v>13</v>
-      </c>
-      <c r="N13">
-        <v>0.58199999999999996</v>
-      </c>
-      <c r="O13">
-        <v>0.32700000000000001</v>
-      </c>
-      <c r="Q13">
-        <v>0.10299999999999999</v>
-      </c>
-      <c r="S13" t="s">
-        <v>13</v>
-      </c>
-      <c r="T13">
-        <v>0.88700000000000001</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z13">
-        <v>0.63400000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>0.80800000000000005</v>
-      </c>
-      <c r="D14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14">
-        <v>0.80800000000000005</v>
-      </c>
-      <c r="G14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14">
-        <v>0.49199999999999999</v>
-      </c>
-      <c r="I14">
-        <v>-0.107</v>
-      </c>
-      <c r="M14" t="s">
-        <v>14</v>
-      </c>
-      <c r="N14">
-        <v>0.42399999999999999</v>
-      </c>
-      <c r="S14" t="s">
-        <v>14</v>
-      </c>
-      <c r="T14">
-        <v>0.76400000000000001</v>
-      </c>
-      <c r="U14">
-        <v>-0.112</v>
-      </c>
-      <c r="V14">
-        <v>0.17100000000000001</v>
-      </c>
-      <c r="W14">
-        <v>-0.125</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z14">
-        <v>0.86299999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>0.51800000000000002</v>
-      </c>
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15">
-        <v>0.51800000000000002</v>
-      </c>
-      <c r="G15" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15">
-        <v>0.59399999999999997</v>
-      </c>
-      <c r="I15">
-        <v>0.105</v>
-      </c>
-      <c r="K15">
-        <v>-0.124</v>
-      </c>
-      <c r="M15" t="s">
-        <v>15</v>
-      </c>
-      <c r="N15">
-        <v>0.65400000000000003</v>
-      </c>
-      <c r="O15">
-        <v>0.17299999999999999</v>
-      </c>
-      <c r="P15">
-        <v>0.25700000000000001</v>
-      </c>
-      <c r="S15" t="s">
-        <v>15</v>
-      </c>
-      <c r="T15">
-        <v>0.86099999999999999</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z15">
-        <v>0.51</v>
-      </c>
-      <c r="AA15">
-        <v>0.216</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="D16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16">
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="G16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16">
-        <v>0.443</v>
-      </c>
-      <c r="I16">
-        <v>0.27300000000000002</v>
-      </c>
-      <c r="K16">
-        <v>-0.13900000000000001</v>
-      </c>
-      <c r="M16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N16">
-        <v>0.40100000000000002</v>
-      </c>
-      <c r="O16">
-        <v>0.23200000000000001</v>
-      </c>
-      <c r="P16">
-        <v>0.23</v>
-      </c>
-      <c r="Q16">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="S16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T16">
-        <v>0.36499999999999999</v>
-      </c>
-      <c r="V16">
-        <v>0.16400000000000001</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z16">
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="AA16">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="AB16">
-        <v>0.13600000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1"/>
-      <c r="H18" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" t="s">
-        <v>0</v>
-      </c>
-      <c r="J18" t="s">
-        <v>1</v>
-      </c>
-      <c r="K18" t="s">
-        <v>17</v>
-      </c>
-      <c r="N18" t="s">
-        <v>18</v>
-      </c>
-      <c r="O18" t="s">
-        <v>0</v>
-      </c>
-      <c r="P18" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>17</v>
-      </c>
-      <c r="T18" t="s">
-        <v>18</v>
-      </c>
-      <c r="U18" t="s">
-        <v>0</v>
-      </c>
-      <c r="V18" t="s">
-        <v>1</v>
-      </c>
-      <c r="W18" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19">
-        <v>6.6929999999999996</v>
-      </c>
-      <c r="D19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19">
-        <v>6.6929999999999996</v>
-      </c>
-      <c r="G19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19">
-        <v>3.47</v>
-      </c>
-      <c r="I19">
-        <v>2.5680000000000001</v>
-      </c>
-      <c r="J19">
-        <v>1.2509999999999999</v>
-      </c>
-      <c r="K19">
-        <v>0.75800000000000001</v>
-      </c>
-      <c r="M19" t="s">
-        <v>22</v>
-      </c>
-      <c r="N19">
-        <v>3.5720000000000001</v>
-      </c>
-      <c r="O19">
-        <v>3.109</v>
-      </c>
-      <c r="P19">
-        <v>1.3440000000000001</v>
-      </c>
-      <c r="Q19">
-        <v>1.24</v>
-      </c>
-      <c r="S19" t="s">
-        <v>22</v>
-      </c>
-      <c r="T19">
-        <v>3.39</v>
-      </c>
-      <c r="U19">
-        <v>2.968</v>
-      </c>
-      <c r="V19">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="W19">
-        <v>1.079</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z19">
-        <v>3.5409999999999999</v>
-      </c>
-      <c r="AA19">
-        <v>3.0019999999999998</v>
-      </c>
-      <c r="AB19">
-        <v>1.8240000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20">
-        <v>0.44600000000000001</v>
-      </c>
-      <c r="D20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20">
-        <v>0.44600000000000001</v>
-      </c>
-      <c r="G20" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="I20">
-        <v>0.17100000000000001</v>
-      </c>
-      <c r="J20">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="K20">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="M20" t="s">
-        <v>23</v>
-      </c>
-      <c r="N20">
-        <v>0.23799999999999999</v>
-      </c>
-      <c r="O20">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="P20">
-        <v>0.09</v>
-      </c>
-      <c r="Q20">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="S20" t="s">
-        <v>23</v>
-      </c>
-      <c r="T20">
-        <v>0.22600000000000001</v>
-      </c>
-      <c r="U20">
-        <v>0.19800000000000001</v>
-      </c>
-      <c r="V20">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="W20">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z20">
-        <v>0.23599999999999999</v>
-      </c>
-      <c r="AA20">
-        <v>0.2</v>
-      </c>
-      <c r="AB20">
-        <v>0.122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="G21" t="s">
-        <v>24</v>
-      </c>
-      <c r="H21">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="I21">
-        <v>0.40300000000000002</v>
-      </c>
-      <c r="J21">
-        <v>0.48599999999999999</v>
-      </c>
-      <c r="K21">
-        <v>0.53600000000000003</v>
-      </c>
-      <c r="M21" t="s">
-        <v>24</v>
-      </c>
-      <c r="N21">
-        <v>0.23799999999999999</v>
-      </c>
-      <c r="O21">
-        <v>0.44500000000000001</v>
-      </c>
-      <c r="P21">
-        <v>0.53500000000000003</v>
-      </c>
-      <c r="Q21">
-        <v>0.61799999999999999</v>
-      </c>
-      <c r="S21" t="s">
-        <v>24</v>
-      </c>
-      <c r="T21">
-        <v>0.22600000000000001</v>
-      </c>
-      <c r="U21">
-        <v>0.42399999999999999</v>
-      </c>
-      <c r="V21">
-        <v>0.499</v>
-      </c>
-      <c r="W21">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z21">
-        <v>0.23599999999999999</v>
-      </c>
-      <c r="AA21">
-        <v>0.436</v>
-      </c>
-      <c r="AB21">
-        <v>0.55800000000000005</v>
+      <c r="C27">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="D27">
+        <v>0.218</v>
+      </c>
+      <c r="E27">
+        <v>0.10100000000000001</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="Z1:AB16" xr:uid="{39412BF1-7058-497E-BBA1-3DAA310B3CD4}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Z2:AB16">
-      <sortCondition sortBy="cellColor" ref="AB1:AB16" dxfId="20"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="B2:B16">
-    <cfRule type="cellIs" dxfId="39" priority="8" operator="greaterThan">
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="B2:D13">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E16">
-    <cfRule type="cellIs" dxfId="38" priority="7" operator="greaterThan">
+  <conditionalFormatting sqref="G2:I13">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:K16">
-    <cfRule type="cellIs" dxfId="37" priority="5" operator="greaterThan">
-      <formula>0.299</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="6" operator="greaterThan">
-      <formula>0.499</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N4:P4 N2 P2 N3:O3 N6:Q6 N5:O5 Q5 N10:Q12 N7:N8 P7:Q8 O9:Q9 N14:Q16 N13 P13:Q13">
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="greaterThan">
+  <conditionalFormatting sqref="L2:N13">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T5:W16 T2:V2 T3:U4 W3:W4">
-    <cfRule type="cellIs" dxfId="34" priority="3" operator="greaterThan">
+  <conditionalFormatting sqref="Q2:S13">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:Q16">
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="greaterThan">
-      <formula>0.299</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z2:AB16">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="B16:E27">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4074,7 +3537,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="H2" sqref="H2:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4682,16 +4145,16 @@
   </sheetData>
   <autoFilter ref="H1:K16" xr:uid="{8B5509DC-DB05-43E6-A45B-32E76BC27DEA}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:K16">
-      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="39"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K16">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4985,11 +4448,11 @@
   </sheetData>
   <autoFilter ref="B1:E16" xr:uid="{4883B1BD-E07A-48BB-9F66-A8C7003F2BEF}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E16">
-      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="47"/>
+      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="69"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="40" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="1" operator="greaterThan">
       <formula>0.699</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5003,7 +4466,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A20" sqref="A3:B20"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5631,31 +5094,31 @@
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{85F09F99-28C1-4BB1-A75C-F2C0B1518057}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q14">
-      <sortCondition sortBy="cellColor" ref="D1" dxfId="70"/>
+      <sortCondition sortBy="cellColor" ref="D1" dxfId="68"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="M2:Q14">
-    <cfRule type="cellIs" dxfId="69" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="52" priority="6" operator="lessThan">
       <formula>-0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="67" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="2" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="4" operator="greaterThan">
       <formula>0.399</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="2" operator="greaterThan">
-      <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="65" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="1" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="3" operator="greaterThan">
       <formula>0.399</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="1" operator="greaterThan">
-      <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6098,21 +5561,21 @@
   </sheetData>
   <autoFilter ref="A1:F14" xr:uid="{F6EC43A2-0E96-4311-A986-12EE04542C46}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
-      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="63"/>
+      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="67"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:E1048576">
-    <cfRule type="cellIs" dxfId="62" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:K1">
-    <cfRule type="cellIs" dxfId="61" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K12">
-    <cfRule type="cellIs" dxfId="60" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6540,16 +6003,16 @@
   </sheetData>
   <autoFilter ref="A1:K1" xr:uid="{2A2FF23C-A49F-4BBF-A172-E01688A2AD61}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K14">
-      <sortCondition sortBy="cellColor" ref="E1" dxfId="59"/>
+      <sortCondition sortBy="cellColor" ref="E1" dxfId="66"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E14">
-    <cfRule type="cellIs" dxfId="58" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:E29">
-    <cfRule type="cellIs" dxfId="57" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6808,16 +6271,16 @@
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{76B16ADE-8397-4523-89E6-FD43024CAE02}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J14">
-      <sortCondition sortBy="cellColor" ref="J1" dxfId="56"/>
+      <sortCondition sortBy="cellColor" ref="J1" dxfId="65"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="55" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="54" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Finished models excluding prayer, spirit, and energy
</commit_message>
<xml_diff>
--- a/R/Factor analysis  - factor loadings.xlsx
+++ b/R/Factor analysis  - factor loadings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\git\AHL\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654D0275-8DFC-4A0C-B2BB-D31100F54ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF396E1-E547-4F9E-84C6-0539742CA5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All CAMs'!$A$1:$AC$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Comparing MPM'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Drop energy, pray, spirit'!$A$15:$S$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Drop energy, pray, spirit'!$A$15:$E$27</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Drop prayer and spirit'!$A$1:$Q$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Mysterious Perfect Model'!$A$1:$F$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Numeric!$A$1:$J$1</definedName>
@@ -145,6 +145,56 @@
           </rPr>
           <t xml:space="preserve">
 Maximum likelihood, varimax
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G15" authorId="2" shapeId="0" xr:uid="{AC596428-AC76-47DE-95A2-2E771234EF9E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Maximum Likelihood, promax
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M15" authorId="2" shapeId="0" xr:uid="{757BA119-28A5-497D-87CC-6A14CB24F0C7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Maximum likelhood, oblimin
 </t>
         </r>
       </text>
@@ -380,7 +430,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="36">
   <si>
     <t>ML2</t>
   </si>
@@ -549,7 +599,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="90">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -615,6 +665,70 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -705,6 +819,66 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
@@ -753,6 +927,22 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -783,6 +973,36 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
@@ -847,6 +1067,76 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
@@ -855,6 +1145,26 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
@@ -863,6 +1173,36 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
@@ -871,6 +1211,66 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
@@ -879,6 +1279,16 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
@@ -887,6 +1297,26 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
@@ -981,198 +1411,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2721,43 +2959,43 @@
   </sheetData>
   <autoFilter ref="A1:AC16" xr:uid="{99B320C6-A597-4E1B-B5FD-F0989543660C}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC16">
-      <sortCondition sortBy="cellColor" ref="N1:N16" dxfId="38"/>
+      <sortCondition sortBy="cellColor" ref="N1:N16" dxfId="89"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="Q2:U16">
-    <cfRule type="cellIs" dxfId="64" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="16" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:AC16">
-    <cfRule type="cellIs" dxfId="63" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="87" priority="15" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H16">
-    <cfRule type="cellIs" dxfId="62" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="6" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="85" priority="12" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C16">
-    <cfRule type="cellIs" dxfId="60" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="84" priority="8" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="9" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="11" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:N16">
-    <cfRule type="cellIs" dxfId="57" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="81" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="2" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2768,21 +3006,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DF5018-9911-4233-8E1E-CFEBD8577F16}">
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.86328125" customWidth="1"/>
     <col min="6" max="6" width="13.265625" customWidth="1"/>
+    <col min="7" max="7" width="12.06640625" customWidth="1"/>
     <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.59765625" customWidth="1"/>
     <col min="16" max="16" width="12.53125" customWidth="1"/>
+    <col min="19" max="19" width="14.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>17</v>
       </c>
@@ -2820,7 +3061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2861,7 +3102,7 @@
         <v>1.048</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2899,7 +3140,7 @@
         <v>0.40899999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2937,7 +3178,7 @@
         <v>0.318</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2984,7 +3225,7 @@
         <v>0.24099999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -3022,7 +3263,7 @@
         <v>-0.16600000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3057,7 +3298,7 @@
         <v>0.11799999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -3101,7 +3342,7 @@
         <v>1.024</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -3145,7 +3386,7 @@
         <v>0.11700000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -3183,7 +3424,7 @@
         <v>0.17799999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3221,7 +3462,7 @@
         <v>0.112</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -3256,7 +3497,7 @@
         <v>0.17899999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -3300,7 +3541,7 @@
         <v>0.13800000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>0</v>
       </c>
@@ -3313,8 +3554,44 @@
       <c r="E15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="H15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" t="s">
+        <v>17</v>
+      </c>
+      <c r="O15" t="s">
+        <v>0</v>
+      </c>
+      <c r="P15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>18</v>
+      </c>
+      <c r="T15" t="s">
+        <v>17</v>
+      </c>
+      <c r="U15" t="s">
+        <v>0</v>
+      </c>
+      <c r="V15" t="s">
+        <v>1</v>
+      </c>
+      <c r="W15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -3330,8 +3607,35 @@
       <c r="E16">
         <v>0.59699999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G16" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>0.505</v>
+      </c>
+      <c r="J16">
+        <v>-0.21199999999999999</v>
+      </c>
+      <c r="K16">
+        <v>0.307</v>
+      </c>
+      <c r="M16" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16">
+        <v>0.11</v>
+      </c>
+      <c r="Q16">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="S16" t="s">
+        <v>4</v>
+      </c>
+      <c r="W16">
+        <v>0.71399999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -3344,8 +3648,41 @@
       <c r="E17">
         <v>0.40699999999999997</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>-0.21199999999999999</v>
+      </c>
+      <c r="K17">
+        <v>0.755</v>
+      </c>
+      <c r="M17" t="s">
+        <v>12</v>
+      </c>
+      <c r="O17">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="P17">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="Q17">
+        <v>0.502</v>
+      </c>
+      <c r="S17" t="s">
+        <v>12</v>
+      </c>
+      <c r="U17">
+        <v>0.192</v>
+      </c>
+      <c r="V17">
+        <v>0.245</v>
+      </c>
+      <c r="W17">
+        <v>0.58299999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -3361,8 +3698,35 @@
       <c r="E18">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18">
+        <v>0.11</v>
+      </c>
+      <c r="J18">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="K18">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="M18" t="s">
+        <v>6</v>
+      </c>
+      <c r="P18">
+        <v>0.95</v>
+      </c>
+      <c r="S18" t="s">
+        <v>6</v>
+      </c>
+      <c r="V18">
+        <v>0.93</v>
+      </c>
+      <c r="W18">
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -3378,8 +3742,44 @@
       <c r="E19">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <v>0.95</v>
+      </c>
+      <c r="K19">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="M19" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="P19">
+        <v>0.19</v>
+      </c>
+      <c r="Q19">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="S19" t="s">
+        <v>3</v>
+      </c>
+      <c r="T19">
+        <v>-0.105</v>
+      </c>
+      <c r="U19">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="V19">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="W19">
+        <v>0.152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -3389,8 +3789,44 @@
       <c r="E20">
         <v>0.66500000000000004</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20">
+        <v>0.874</v>
+      </c>
+      <c r="K20">
+        <v>0.109</v>
+      </c>
+      <c r="M20" t="s">
+        <v>10</v>
+      </c>
+      <c r="N20">
+        <v>0.122</v>
+      </c>
+      <c r="O20">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="P20">
+        <v>-0.20499999999999999</v>
+      </c>
+      <c r="Q20">
+        <v>0.129</v>
+      </c>
+      <c r="S20" t="s">
+        <v>10</v>
+      </c>
+      <c r="T20">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="U20">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="V20">
+        <v>-0.23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -3403,8 +3839,32 @@
       <c r="D21">
         <v>0.33800000000000002</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G21" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="K21">
+        <v>-0.16500000000000001</v>
+      </c>
+      <c r="M21" t="s">
+        <v>11</v>
+      </c>
+      <c r="O21">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="S21" t="s">
+        <v>11</v>
+      </c>
+      <c r="T21">
+        <v>0.109</v>
+      </c>
+      <c r="U21">
+        <v>0.80500000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -3420,8 +3880,29 @@
       <c r="E22">
         <v>0.21299999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="K22">
+        <v>0.159</v>
+      </c>
+      <c r="M22" t="s">
+        <v>14</v>
+      </c>
+      <c r="O22">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="S22" t="s">
+        <v>14</v>
+      </c>
+      <c r="U22">
+        <v>1.0209999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -3437,8 +3918,53 @@
       <c r="E23">
         <v>0.224</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23">
+        <v>0.114</v>
+      </c>
+      <c r="I23">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="J23">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="K23">
+        <v>-0.156</v>
+      </c>
+      <c r="M23" t="s">
+        <v>2</v>
+      </c>
+      <c r="N23">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="O23">
+        <v>0.151</v>
+      </c>
+      <c r="P23">
+        <v>-0.17799999999999999</v>
+      </c>
+      <c r="Q23">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="S23" t="s">
+        <v>2</v>
+      </c>
+      <c r="T23">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="U23">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="V23">
+        <v>-0.214</v>
+      </c>
+      <c r="W23">
+        <v>0.246</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -3454,8 +3980,35 @@
       <c r="E24">
         <v>0.107</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G24" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="I24">
+        <v>-0.11899999999999999</v>
+      </c>
+      <c r="J24">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="K24">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="M24" t="s">
+        <v>7</v>
+      </c>
+      <c r="N24">
+        <v>0.871</v>
+      </c>
+      <c r="S24" t="s">
+        <v>7</v>
+      </c>
+      <c r="T24">
+        <v>0.91500000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -3468,8 +4021,44 @@
       <c r="D25">
         <v>0.219</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="I25">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="J25">
+        <v>-0.22700000000000001</v>
+      </c>
+      <c r="K25">
+        <v>0.111</v>
+      </c>
+      <c r="M25" t="s">
+        <v>8</v>
+      </c>
+      <c r="N25">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="P25">
+        <v>0.104</v>
+      </c>
+      <c r="Q25">
+        <v>-0.187</v>
+      </c>
+      <c r="S25" t="s">
+        <v>8</v>
+      </c>
+      <c r="T25">
+        <v>0.82</v>
+      </c>
+      <c r="W25">
+        <v>-0.20300000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -3482,8 +4071,26 @@
       <c r="E26">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26">
+        <v>0.84</v>
+      </c>
+      <c r="M26" t="s">
+        <v>9</v>
+      </c>
+      <c r="N26">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="S26" t="s">
+        <v>9</v>
+      </c>
+      <c r="T26">
+        <v>0.84699999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -3499,31 +4106,84 @@
       <c r="E27">
         <v>0.10100000000000001</v>
       </c>
+      <c r="G27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27">
+        <v>1.0529999999999999</v>
+      </c>
+      <c r="M27" t="s">
+        <v>15</v>
+      </c>
+      <c r="N27">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="O27">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="P27">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="Q27">
+        <v>-0.17</v>
+      </c>
+      <c r="S27" t="s">
+        <v>15</v>
+      </c>
+      <c r="T27">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="V27">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="W27">
+        <v>-0.159</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A15:E27" xr:uid="{00DF5018-9911-4233-8E1E-CFEBD8577F16}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:E27">
+      <sortCondition sortBy="cellColor" ref="E15:E27" dxfId="1"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B2:D13">
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="8" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:I13">
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:N13">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="6" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:S13">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:E27">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16:K27">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N16:Q27">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T16:W27">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4145,16 +4805,16 @@
   </sheetData>
   <autoFilter ref="H1:K16" xr:uid="{8B5509DC-DB05-43E6-A45B-32E76BC27DEA}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:K16">
-      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="39"/>
+      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="79"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="55" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K16">
-    <cfRule type="cellIs" dxfId="54" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4448,11 +5108,11 @@
   </sheetData>
   <autoFilter ref="B1:E16" xr:uid="{4883B1BD-E07A-48BB-9F66-A8C7003F2BEF}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E16">
-      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="69"/>
+      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="76"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="53" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="1" operator="greaterThan">
       <formula>0.699</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5094,30 +5754,30 @@
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{85F09F99-28C1-4BB1-A75C-F2C0B1518057}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q14">
-      <sortCondition sortBy="cellColor" ref="D1" dxfId="68"/>
+      <sortCondition sortBy="cellColor" ref="D1" dxfId="74"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="M2:Q14">
-    <cfRule type="cellIs" dxfId="52" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="73" priority="6" operator="lessThan">
       <formula>-0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="50" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="4" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="48" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="69" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="3" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5565,17 +6225,17 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:E1048576">
-    <cfRule type="cellIs" dxfId="46" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:K1">
-    <cfRule type="cellIs" dxfId="45" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K12">
-    <cfRule type="cellIs" dxfId="44" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6003,16 +6663,16 @@
   </sheetData>
   <autoFilter ref="A1:K1" xr:uid="{2A2FF23C-A49F-4BBF-A172-E01688A2AD61}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K14">
-      <sortCondition sortBy="cellColor" ref="E1" dxfId="66"/>
+      <sortCondition sortBy="cellColor" ref="E1" dxfId="63"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E14">
-    <cfRule type="cellIs" dxfId="43" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:E29">
-    <cfRule type="cellIs" dxfId="42" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6271,16 +6931,16 @@
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{76B16ADE-8397-4523-89E6-FD43024CAE02}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J14">
-      <sortCondition sortBy="cellColor" ref="J1" dxfId="65"/>
+      <sortCondition sortBy="cellColor" ref="J1" dxfId="60"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="41" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="40" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Created function for obtaining fit statistics and adding them to a tibble
Working on redoing all models with function
</commit_message>
<xml_diff>
--- a/R/Factor analysis  - factor loadings.xlsx
+++ b/R/Factor analysis  - factor loadings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\git\AHL\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF396E1-E547-4F9E-84C6-0539742CA5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1F96A7-AC54-4ACD-A23A-0D5A0B594CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
   </bookViews>
@@ -17,18 +17,20 @@
     <sheet name="Drop energy, pray, spirit" sheetId="10" r:id="rId2"/>
     <sheet name="Principal Axis Factoring" sheetId="9" r:id="rId3"/>
     <sheet name="PCA" sheetId="8" r:id="rId4"/>
-    <sheet name="Drop prayer and spirit" sheetId="2" r:id="rId5"/>
+    <sheet name="Drop prayer and spirit" sheetId="2" state="hidden" r:id="rId5"/>
     <sheet name="Mysterious Perfect Model" sheetId="3" r:id="rId6"/>
-    <sheet name="Comparing MPM" sheetId="6" r:id="rId7"/>
-    <sheet name="Numeric" sheetId="5" r:id="rId8"/>
+    <sheet name="Ex Pray Spirit Comparisons" sheetId="11" r:id="rId7"/>
+    <sheet name="Comparing MPM" sheetId="6" r:id="rId8"/>
+    <sheet name="Numeric" sheetId="5" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All CAMs'!$A$1:$AC$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Comparing MPM'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Comparing MPM'!$A$1:$K$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Drop energy, pray, spirit'!$A$15:$E$27</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Drop prayer and spirit'!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Ex Pray Spirit Comparisons'!$A$16:$C$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Mysterious Perfect Model'!$A$1:$F$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Numeric!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Numeric!$A$1:$J$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">PCA!$B$1:$E$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Principal Axis Factoring'!$H$1:$K$16</definedName>
   </definedNames>
@@ -340,6 +342,141 @@
     <author>hanna</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{BF07EF22-39DC-4119-8DF2-E0F29C3B0008}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Maximum likelihood, varimax rotation
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{FC0F7213-7285-4B2C-B961-AEEC5050BD1E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Maximum Likelihood, promax rotation
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{2510CC9D-8268-435A-8CB7-4E7BC12401C1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Maximum likelihood, oblimin rotation
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{5EA7F6F2-02E1-4A68-8922-3BBD5F6D467E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Maximum Likelihood, cluster rotation
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{E0824D5C-0A44-4F46-8A81-A476B5475001}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Principal Axis, varimax
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>hanna</author>
+  </authors>
+  <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{D5712E48-0578-4E7B-970F-9D684F744419}">
       <text>
         <r>
@@ -394,7 +531,7 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -430,7 +567,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="36">
   <si>
     <t>ML2</t>
   </si>
@@ -599,7 +736,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="90">
+  <dxfs count="76">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -629,162 +766,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
           <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -911,68 +892,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1035,6 +954,26 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
@@ -1077,42 +1016,34 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1293,6 +1224,94 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
           <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1767,7 +1786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A59E54-D4A7-4C25-9D11-CD018EBC24D4}">
   <dimension ref="A1:AD21"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -2959,43 +2978,43 @@
   </sheetData>
   <autoFilter ref="A1:AC16" xr:uid="{99B320C6-A597-4E1B-B5FD-F0989543660C}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC16">
-      <sortCondition sortBy="cellColor" ref="N1:N16" dxfId="89"/>
+      <sortCondition sortBy="cellColor" ref="N1:N16" dxfId="75"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="Q2:U16">
-    <cfRule type="cellIs" dxfId="88" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="16" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:AC16">
-    <cfRule type="cellIs" dxfId="87" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="15" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H16">
-    <cfRule type="cellIs" dxfId="86" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="6" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="12" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C16">
-    <cfRule type="cellIs" dxfId="84" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="8" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="69" priority="9" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="11" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:N16">
-    <cfRule type="cellIs" dxfId="81" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="2" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3008,8 +3027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DF5018-9911-4233-8E1E-CFEBD8577F16}">
   <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3019,7 +3038,7 @@
     <col min="7" max="7" width="12.06640625" customWidth="1"/>
     <col min="11" max="11" width="15.33203125" customWidth="1"/>
     <col min="13" max="13" width="12.59765625" customWidth="1"/>
-    <col min="16" max="16" width="12.53125" customWidth="1"/>
+    <col min="16" max="16" width="14.265625" customWidth="1"/>
     <col min="19" max="19" width="14.59765625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4143,47 +4162,47 @@
   </sheetData>
   <autoFilter ref="A15:E27" xr:uid="{00DF5018-9911-4233-8E1E-CFEBD8577F16}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:E27">
-      <sortCondition sortBy="cellColor" ref="E15:E27" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="E15:E27" dxfId="65"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B2:D13">
-    <cfRule type="cellIs" dxfId="30" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="8" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:I13">
-    <cfRule type="cellIs" dxfId="29" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:N13">
-    <cfRule type="cellIs" dxfId="28" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="6" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:S13">
-    <cfRule type="cellIs" dxfId="27" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="5" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:E27">
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:K27">
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16:Q27">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16:W27">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4196,9 +4215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5509DC-DB05-43E6-A45B-32E76BC27DEA}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:K16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -4805,16 +4822,16 @@
   </sheetData>
   <autoFilter ref="H1:K16" xr:uid="{8B5509DC-DB05-43E6-A45B-32E76BC27DEA}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:K16">
-      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="79"/>
+      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="56"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="78" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K16">
-    <cfRule type="cellIs" dxfId="77" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5108,11 +5125,11 @@
   </sheetData>
   <autoFilter ref="B1:E16" xr:uid="{4883B1BD-E07A-48BB-9F66-A8C7003F2BEF}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E16">
-      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="76"/>
+      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="53"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="75" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="1" operator="greaterThan">
       <formula>0.699</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5754,30 +5771,30 @@
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{85F09F99-28C1-4BB1-A75C-F2C0B1518057}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q14">
-      <sortCondition sortBy="cellColor" ref="D1" dxfId="74"/>
+      <sortCondition sortBy="cellColor" ref="D1" dxfId="51"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="M2:Q14">
-    <cfRule type="cellIs" dxfId="73" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="50" priority="6" operator="lessThan">
       <formula>-0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="71" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="4" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="69" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="3" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6221,21 +6238,21 @@
   </sheetData>
   <autoFilter ref="A1:F14" xr:uid="{F6EC43A2-0E96-4311-A986-12EE04542C46}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
-      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="67"/>
+      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="44"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:E1048576">
-    <cfRule type="cellIs" dxfId="66" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:K1">
-    <cfRule type="cellIs" dxfId="65" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K12">
-    <cfRule type="cellIs" dxfId="64" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6245,6 +6262,657 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498CC891-573B-427D-8528-B6E57CC0DFD4}">
+  <dimension ref="A1:O29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.86328125" customWidth="1"/>
+    <col min="9" max="9" width="13.53125" customWidth="1"/>
+    <col min="13" max="13" width="13.06640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="C2">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="G2">
+        <v>0.52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>0.436</v>
+      </c>
+      <c r="K2">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="M2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="O2">
+        <v>0.39300000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="C3">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="K3">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="M3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>0.60199999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="C4">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G4">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="M4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>0.53</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>0.502</v>
+      </c>
+      <c r="M5" t="s">
+        <v>7</v>
+      </c>
+      <c r="O5">
+        <v>0.873</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>0.98</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="M6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6">
+        <v>0.628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7">
+        <v>-0.12</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="M7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="C8">
+        <v>0.307</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="I8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="M8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="O8">
+        <v>0.42399999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0.434</v>
+      </c>
+      <c r="C9">
+        <v>0.504</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="G9">
+        <v>-0.125</v>
+      </c>
+      <c r="I9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="M9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9">
+        <v>0.214</v>
+      </c>
+      <c r="O9">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>0.33</v>
+      </c>
+      <c r="C10">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="I10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="M10" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>0.64900000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>0.12</v>
+      </c>
+      <c r="C11">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="I11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="M11" t="s">
+        <v>6</v>
+      </c>
+      <c r="N11">
+        <v>0.377</v>
+      </c>
+      <c r="O11">
+        <v>0.27600000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="C12">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <v>0.98</v>
+      </c>
+      <c r="G12">
+        <v>-0.11899999999999999</v>
+      </c>
+      <c r="I12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="M12" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12">
+        <v>0.52800000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>0.503</v>
+      </c>
+      <c r="C13">
+        <v>0.246</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>0.45</v>
+      </c>
+      <c r="G13">
+        <v>0.254</v>
+      </c>
+      <c r="I13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="K13">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="M13" t="s">
+        <v>11</v>
+      </c>
+      <c r="N13">
+        <v>0.96199999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="C14">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0.184</v>
+      </c>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14">
+        <v>0.36</v>
+      </c>
+      <c r="K14">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="M14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14">
+        <v>0.97899999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="C17">
+        <v>0.33100000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="C18">
+        <v>0.67200000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>0.437</v>
+      </c>
+      <c r="C19">
+        <v>0.44800000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>0.81</v>
+      </c>
+      <c r="C20">
+        <v>0.34799999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="C21">
+        <v>0.312</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="C22">
+        <v>0.84399999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="C23">
+        <v>0.42099999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="C24">
+        <v>0.32400000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="C25">
+        <v>0.57699999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="C26">
+        <v>0.44800000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="C27">
+        <v>0.88100000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>0.436</v>
+      </c>
+      <c r="C28">
+        <v>0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="C29">
+        <v>0.29199999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A16:C29" xr:uid="{498CC891-573B-427D-8528-B6E57CC0DFD4}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:C29">
+      <sortCondition sortBy="cellColor" ref="C16:C29" dxfId="1"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="B2:C14">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:G14">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:K14">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:O14">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:C29">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC6BCC2-AE82-430A-9446-637AC6346772}">
   <dimension ref="A1:E29"/>
   <sheetViews>
@@ -6663,16 +7331,16 @@
   </sheetData>
   <autoFilter ref="A1:K1" xr:uid="{2A2FF23C-A49F-4BBF-A172-E01688A2AD61}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K14">
-      <sortCondition sortBy="cellColor" ref="E1" dxfId="63"/>
+      <sortCondition sortBy="cellColor" ref="E1" dxfId="40"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E14">
-    <cfRule type="cellIs" dxfId="62" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:E29">
-    <cfRule type="cellIs" dxfId="61" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6681,7 +7349,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C8C1A-CFC6-49AC-B896-635D55B44BA8}">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -6931,16 +7599,16 @@
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{76B16ADE-8397-4523-89E6-FD43024CAE02}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J14">
-      <sortCondition sortBy="cellColor" ref="J1" dxfId="60"/>
+      <sortCondition sortBy="cellColor" ref="J1" dxfId="37"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="59" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="58" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Cleaned up factor analysis file, some analyses run with Terrence added at the end
</commit_message>
<xml_diff>
--- a/R/Factor analysis  - factor loadings.xlsx
+++ b/R/Factor analysis  - factor loadings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\git\AHL\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1F96A7-AC54-4ACD-A23A-0D5A0B594CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BAE0A9-BF62-4B7F-AF25-60C28C6703E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
   </bookViews>
   <sheets>
     <sheet name="All CAMs" sheetId="1" r:id="rId1"/>
@@ -736,7 +736,79 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="76">
+  <dxfs count="77">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -860,34 +932,172 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -930,18 +1140,22 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -974,104 +1188,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1252,104 +1374,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
           <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1786,8 +1810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A59E54-D4A7-4C25-9D11-CD018EBC24D4}">
   <dimension ref="A1:AD21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1864,232 +1888,202 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>0.872</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="G2">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="H2">
+        <v>0.245</v>
+      </c>
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="M2">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="P2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>0.81</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2">
-        <v>0.878</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="Q2">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="W2" t="s">
         <v>13</v>
       </c>
-      <c r="L2">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="M2">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="N2">
-        <v>0.72899999999999998</v>
-      </c>
-      <c r="P2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q2">
-        <v>0.68700000000000006</v>
-      </c>
-      <c r="R2">
-        <v>0.126</v>
-      </c>
-      <c r="S2">
-        <v>-0.152</v>
-      </c>
-      <c r="U2">
-        <v>-0.107</v>
-      </c>
-      <c r="W2" t="s">
-        <v>11</v>
-      </c>
-      <c r="X2">
-        <v>0.108</v>
-      </c>
       <c r="Y2">
-        <v>0.70399999999999996</v>
-      </c>
-      <c r="Z2">
-        <v>0.125</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="AA2">
-        <v>0.191</v>
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="AC2">
+        <v>0.75800000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3">
-        <v>0.72799999999999998</v>
+        <v>0.74099999999999999</v>
       </c>
       <c r="C3">
-        <v>0.14000000000000001</v>
+        <v>-0.104</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3">
-        <v>0.192</v>
+        <v>0.55400000000000005</v>
       </c>
       <c r="G3">
-        <v>0.65800000000000003</v>
-      </c>
-      <c r="H3">
-        <v>0.14000000000000001</v>
+        <v>0.17</v>
       </c>
       <c r="J3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3">
-        <v>0.41</v>
-      </c>
-      <c r="L3">
-        <v>0.40500000000000003</v>
+        <v>16</v>
       </c>
       <c r="M3">
-        <v>0.311</v>
+        <v>0.96</v>
       </c>
       <c r="N3">
-        <v>-0.13100000000000001</v>
-      </c>
-      <c r="O3" t="s">
-        <v>19</v>
+        <v>0.11</v>
       </c>
       <c r="P3" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="Q3">
+        <v>0.40799999999999997</v>
       </c>
       <c r="R3">
-        <v>0.58499999999999996</v>
+        <v>-0.114</v>
       </c>
       <c r="S3">
-        <v>0.224</v>
-      </c>
-      <c r="U3">
-        <v>-0.17299999999999999</v>
+        <v>0.128</v>
       </c>
       <c r="W3" t="s">
-        <v>7</v>
-      </c>
-      <c r="X3">
-        <v>0.85699999999999998</v>
+        <v>12</v>
+      </c>
+      <c r="Y3">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="Z3">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="AB3">
+        <v>0.53200000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>0.74099999999999999</v>
-      </c>
-      <c r="C4">
-        <v>-0.104</v>
+        <v>0.80400000000000005</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F4">
-        <v>0.55400000000000005</v>
-      </c>
-      <c r="G4">
-        <v>0.17</v>
+        <v>0.871</v>
       </c>
       <c r="J4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="N4">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="P4" t="s">
         <v>16</v>
       </c>
-      <c r="M4">
-        <v>0.96</v>
-      </c>
-      <c r="N4">
-        <v>0.11</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="T4">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="U4">
+        <v>0.106</v>
+      </c>
+      <c r="W4" t="s">
         <v>4</v>
       </c>
-      <c r="Q4">
-        <v>0.40799999999999997</v>
-      </c>
-      <c r="R4">
-        <v>-0.114</v>
-      </c>
-      <c r="S4">
-        <v>0.128</v>
-      </c>
-      <c r="W4" t="s">
-        <v>12</v>
+      <c r="X4">
+        <v>0.1</v>
       </c>
       <c r="Y4">
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="Z4">
-        <v>0.27800000000000002</v>
+        <v>-0.12</v>
       </c>
       <c r="AB4">
-        <v>0.53200000000000003</v>
+        <v>0.67200000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>0.67200000000000004</v>
-      </c>
-      <c r="C5">
-        <v>-0.106</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F5">
-        <v>0.22800000000000001</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="G5">
-        <v>0.50900000000000001</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="J5" t="s">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="K5">
+        <v>0.443</v>
       </c>
       <c r="L5">
-        <v>0.63800000000000001</v>
+        <v>0.27300000000000002</v>
       </c>
       <c r="N5">
-        <v>-0.16400000000000001</v>
+        <v>-0.13900000000000001</v>
       </c>
       <c r="P5" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="Q5">
-        <v>0.35099999999999998</v>
-      </c>
-      <c r="R5">
-        <v>0.36899999999999999</v>
+        <v>0.248</v>
       </c>
       <c r="S5">
-        <v>0.14599999999999999</v>
+        <v>0.27900000000000003</v>
       </c>
       <c r="T5">
-        <v>0.32400000000000001</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="U5">
-        <v>-0.13200000000000001</v>
+        <v>0.111</v>
       </c>
       <c r="V5" t="s">
         <v>25</v>
       </c>
       <c r="W5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y5">
-        <v>0.57799999999999996</v>
-      </c>
-      <c r="Z5">
-        <v>0.21199999999999999</v>
+        <v>16</v>
+      </c>
+      <c r="AA5">
+        <v>0.94899999999999995</v>
       </c>
       <c r="AC5">
-        <v>-0.14699999999999999</v>
+        <v>0.128</v>
       </c>
       <c r="AD5" t="s">
         <v>25</v>
@@ -2097,364 +2091,397 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B6">
-        <v>0.44800000000000001</v>
+        <v>0.185</v>
+      </c>
+      <c r="C6">
+        <v>0.64800000000000002</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>0.53200000000000003</v>
-      </c>
-      <c r="G6">
-        <v>-0.14399999999999999</v>
+        <v>16</v>
+      </c>
+      <c r="H6">
+        <v>0.998</v>
       </c>
       <c r="J6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L6">
-        <v>0.505</v>
-      </c>
-      <c r="M6">
-        <v>0.223</v>
-      </c>
-      <c r="N6">
-        <v>-0.22</v>
+        <v>7</v>
+      </c>
+      <c r="K6">
+        <v>0.88600000000000001</v>
       </c>
       <c r="P6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q6">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="R6">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="S6">
+        <v>0.35</v>
+      </c>
+      <c r="T6">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="U6">
+        <v>-0.15</v>
+      </c>
+      <c r="W6" t="s">
         <v>6</v>
       </c>
-      <c r="S6">
-        <v>0.98499999999999999</v>
-      </c>
-      <c r="W6" t="s">
-        <v>5</v>
-      </c>
-      <c r="X6">
-        <v>0.318</v>
-      </c>
-      <c r="Y6">
-        <v>0.375</v>
-      </c>
       <c r="Z6">
-        <v>0.13400000000000001</v>
-      </c>
-      <c r="AA6">
-        <v>0.33700000000000002</v>
-      </c>
-      <c r="AC6">
-        <v>-0.124</v>
+        <v>0.96099999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>0.872</v>
+        <v>0.81</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F7">
-        <v>0.54800000000000004</v>
-      </c>
-      <c r="G7">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="H7">
-        <v>0.245</v>
+        <v>0.878</v>
       </c>
       <c r="J7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="M7">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="N7">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="P7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q7">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="R7">
+        <v>0.126</v>
+      </c>
+      <c r="S7">
+        <v>-0.152</v>
+      </c>
+      <c r="U7">
+        <v>-0.107</v>
+      </c>
+      <c r="W7" t="s">
         <v>11</v>
       </c>
-      <c r="L7">
-        <v>0.75900000000000001</v>
-      </c>
-      <c r="M7">
-        <v>0.16300000000000001</v>
-      </c>
-      <c r="P7" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q7">
-        <v>0.90200000000000002</v>
-      </c>
-      <c r="W7" t="s">
-        <v>13</v>
+      <c r="X7">
+        <v>0.108</v>
       </c>
       <c r="Y7">
-        <v>0.16300000000000001</v>
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="Z7">
+        <v>0.125</v>
       </c>
       <c r="AA7">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="AC7">
-        <v>0.75800000000000001</v>
+        <v>0.191</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>0.55900000000000005</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="C8">
-        <v>0.105</v>
+        <v>-0.106</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F8">
-        <v>0.65300000000000002</v>
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="G8">
+        <v>0.50900000000000001</v>
       </c>
       <c r="J8" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="L8">
-        <v>0.99199999999999999</v>
-      </c>
-      <c r="M8">
-        <v>-0.11</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="N8">
-        <v>0.16600000000000001</v>
+        <v>-0.16400000000000001</v>
       </c>
       <c r="P8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="Q8">
-        <v>0.70299999999999996</v>
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="R8">
+        <v>0.36899999999999999</v>
       </c>
       <c r="S8">
-        <v>0.10100000000000001</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="T8">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="U8">
         <v>-0.13200000000000001</v>
       </c>
-      <c r="U8">
-        <v>0.19800000000000001</v>
+      <c r="V8" t="s">
+        <v>25</v>
       </c>
       <c r="W8" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="Y8">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="AA8">
-        <v>-0.114</v>
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="Z8">
+        <v>0.21199999999999999</v>
       </c>
       <c r="AC8">
-        <v>0.193</v>
+        <v>-0.14699999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.55900000000000005</v>
       </c>
       <c r="C9">
-        <v>1.0069999999999999</v>
+        <v>0.105</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F9">
-        <v>0.35699999999999998</v>
-      </c>
-      <c r="G9">
-        <v>0.126</v>
-      </c>
-      <c r="H9">
-        <v>0.13500000000000001</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="J9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="M9">
+        <v>-0.11</v>
+      </c>
+      <c r="N9">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="P9" t="s">
         <v>8</v>
       </c>
-      <c r="K9">
-        <v>0.77200000000000002</v>
-      </c>
-      <c r="M9">
-        <v>-0.13500000000000001</v>
-      </c>
-      <c r="N9">
-        <v>0.191</v>
-      </c>
-      <c r="P9" t="s">
-        <v>13</v>
-      </c>
-      <c r="R9">
-        <v>0.188</v>
+      <c r="Q9">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="S9">
+        <v>0.10100000000000001</v>
       </c>
       <c r="T9">
-        <v>0.317</v>
+        <v>-0.13200000000000001</v>
       </c>
       <c r="U9">
-        <v>0.72699999999999998</v>
-      </c>
-      <c r="V9" t="s">
-        <v>25</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="W9" t="s">
-        <v>2</v>
-      </c>
-      <c r="X9">
-        <v>0.55500000000000005</v>
+        <v>14</v>
       </c>
       <c r="Y9">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="Z9">
-        <v>-0.17599999999999999</v>
-      </c>
-      <c r="AB9">
-        <v>0.23</v>
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="AA9">
+        <v>-0.114</v>
+      </c>
+      <c r="AC9">
+        <v>0.193</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="C10">
+        <v>-0.13100000000000001</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="J10" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>0.80400000000000005</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10">
-        <v>0.871</v>
-      </c>
-      <c r="J10" t="s">
-        <v>15</v>
-      </c>
       <c r="K10">
-        <v>0.39200000000000002</v>
-      </c>
-      <c r="N10">
-        <v>0.11899999999999999</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="P10" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="R10">
+        <v>0.97099999999999997</v>
       </c>
       <c r="T10">
-        <v>0.96399999999999997</v>
+        <v>-0.109</v>
       </c>
       <c r="U10">
-        <v>0.106</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="W10" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="X10">
-        <v>0.1</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="Y10">
-        <v>-0.12</v>
-      </c>
-      <c r="AB10">
-        <v>0.67200000000000004</v>
+        <v>0.501</v>
+      </c>
+      <c r="Z10">
+        <v>-0.17399999999999999</v>
+      </c>
+      <c r="AA10">
+        <v>0.223</v>
+      </c>
+      <c r="AC10">
+        <v>-0.19400000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>0.185</v>
+        <v>0.72799999999999998</v>
       </c>
       <c r="C11">
-        <v>0.64800000000000002</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <v>0.192</v>
+      </c>
+      <c r="G11">
+        <v>0.65800000000000003</v>
       </c>
       <c r="H11">
-        <v>0.998</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>0.41</v>
+      </c>
+      <c r="L11">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="M11">
+        <v>0.311</v>
+      </c>
+      <c r="N11">
+        <v>-0.13100000000000001</v>
+      </c>
+      <c r="O11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P11" t="s">
+        <v>3</v>
+      </c>
+      <c r="R11">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="S11">
+        <v>0.224</v>
+      </c>
+      <c r="U11">
+        <v>-0.17299999999999999</v>
+      </c>
+      <c r="W11" t="s">
         <v>7</v>
       </c>
-      <c r="K11">
-        <v>0.88600000000000001</v>
-      </c>
-      <c r="P11" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q11">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="R11">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="S11">
-        <v>0.35</v>
-      </c>
-      <c r="T11">
-        <v>0.10299999999999999</v>
-      </c>
-      <c r="U11">
-        <v>-0.15</v>
-      </c>
-      <c r="W11" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z11">
-        <v>0.96099999999999997</v>
+      <c r="X11">
+        <v>0.85699999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>1.0069999999999999</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="G12">
+        <v>0.126</v>
+      </c>
+      <c r="H12">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="J12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="M12">
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="N12">
+        <v>0.191</v>
+      </c>
+      <c r="P12" t="s">
+        <v>13</v>
+      </c>
+      <c r="R12">
+        <v>0.188</v>
+      </c>
+      <c r="T12">
+        <v>0.317</v>
+      </c>
+      <c r="U12">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="V12" t="s">
+        <v>25</v>
+      </c>
+      <c r="W12" t="s">
         <v>2</v>
       </c>
-      <c r="B12">
-        <v>0.71899999999999997</v>
-      </c>
-      <c r="C12">
-        <v>-0.13100000000000001</v>
-      </c>
-      <c r="E12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12">
-        <v>0.67900000000000005</v>
-      </c>
-      <c r="J12" t="s">
-        <v>9</v>
-      </c>
-      <c r="K12">
-        <v>0.85899999999999999</v>
-      </c>
-      <c r="P12" t="s">
-        <v>14</v>
-      </c>
-      <c r="R12">
-        <v>0.97099999999999997</v>
-      </c>
-      <c r="T12">
-        <v>-0.109</v>
-      </c>
-      <c r="U12">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="W12" t="s">
-        <v>10</v>
-      </c>
       <c r="X12">
-        <v>0.11700000000000001</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="Y12">
-        <v>0.501</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="Z12">
-        <v>-0.17399999999999999</v>
-      </c>
-      <c r="AA12">
-        <v>0.223</v>
-      </c>
-      <c r="AC12">
-        <v>-0.19400000000000001</v>
+        <v>-0.17599999999999999</v>
+      </c>
+      <c r="AB12">
+        <v>0.23</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.45">
@@ -2571,114 +2598,111 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B15">
-        <v>0.64700000000000002</v>
-      </c>
-      <c r="C15">
-        <v>0.27200000000000002</v>
+        <v>0.44800000000000001</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F15">
-        <v>-0.13200000000000001</v>
+        <v>0.53200000000000003</v>
       </c>
       <c r="G15">
-        <v>0.42399999999999999</v>
-      </c>
-      <c r="H15">
-        <v>0.63700000000000001</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="J15" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15">
-        <v>0.59399999999999997</v>
+        <v>10</v>
       </c>
       <c r="L15">
-        <v>0.105</v>
+        <v>0.505</v>
+      </c>
+      <c r="M15">
+        <v>0.223</v>
       </c>
       <c r="N15">
+        <v>-0.22</v>
+      </c>
+      <c r="P15" t="s">
+        <v>6</v>
+      </c>
+      <c r="S15">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="W15" t="s">
+        <v>5</v>
+      </c>
+      <c r="X15">
+        <v>0.318</v>
+      </c>
+      <c r="Y15">
+        <v>0.375</v>
+      </c>
+      <c r="Z15">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="AA15">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="AC15">
         <v>-0.124</v>
-      </c>
-      <c r="P15" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q15">
-        <v>0.83099999999999996</v>
-      </c>
-      <c r="W15" t="s">
-        <v>15</v>
-      </c>
-      <c r="X15">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="Z15">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="AA15">
-        <v>0.121</v>
-      </c>
-      <c r="AB15">
-        <v>-0.153</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>0.61799999999999999</v>
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="C16">
+        <v>0.27200000000000002</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F16">
-        <v>0.47299999999999998</v>
+        <v>-0.13200000000000001</v>
       </c>
       <c r="G16">
-        <v>0.20399999999999999</v>
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="H16">
+        <v>0.63700000000000001</v>
       </c>
       <c r="J16" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="K16">
-        <v>0.443</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="L16">
-        <v>0.27300000000000002</v>
+        <v>0.105</v>
       </c>
       <c r="N16">
-        <v>-0.13900000000000001</v>
+        <v>-0.124</v>
       </c>
       <c r="P16" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q16">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="W16" t="s">
         <v>15</v>
       </c>
-      <c r="Q16">
-        <v>0.248</v>
-      </c>
-      <c r="S16">
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="T16">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="U16">
-        <v>0.111</v>
-      </c>
-      <c r="V16" t="s">
-        <v>25</v>
-      </c>
-      <c r="W16" t="s">
-        <v>16</v>
+      <c r="X16">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="Z16">
+        <v>0.28999999999999998</v>
       </c>
       <c r="AA16">
-        <v>0.94899999999999995</v>
-      </c>
-      <c r="AC16">
-        <v>0.128</v>
+        <v>0.121</v>
+      </c>
+      <c r="AB16">
+        <v>-0.153</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.45">
@@ -2978,43 +3002,43 @@
   </sheetData>
   <autoFilter ref="A1:AC16" xr:uid="{99B320C6-A597-4E1B-B5FD-F0989543660C}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC16">
-      <sortCondition sortBy="cellColor" ref="N1:N16" dxfId="75"/>
+      <sortCondition sortBy="cellColor" ref="AC1:AC16" dxfId="1"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="Q2:U16">
-    <cfRule type="cellIs" dxfId="74" priority="16" operator="greaterThan">
-      <formula>0.299</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X2:AC16">
-    <cfRule type="cellIs" dxfId="73" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="17" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H16">
-    <cfRule type="cellIs" dxfId="72" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="13" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C16">
-    <cfRule type="cellIs" dxfId="70" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="9" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="10" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="12" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:N16">
-    <cfRule type="cellIs" dxfId="67" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="greaterThan">
+      <formula>0.499</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X2:AC16">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3027,8 +3051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DF5018-9911-4233-8E1E-CFEBD8577F16}">
   <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView topLeftCell="F8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4162,47 +4186,47 @@
   </sheetData>
   <autoFilter ref="A15:E27" xr:uid="{00DF5018-9911-4233-8E1E-CFEBD8577F16}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:E27">
-      <sortCondition sortBy="cellColor" ref="E15:E27" dxfId="65"/>
+      <sortCondition sortBy="cellColor" ref="E15:E27" dxfId="76"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B2:D13">
-    <cfRule type="cellIs" dxfId="64" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="8" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:I13">
-    <cfRule type="cellIs" dxfId="63" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:N13">
-    <cfRule type="cellIs" dxfId="62" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="6" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:S13">
-    <cfRule type="cellIs" dxfId="61" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="5" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:E27">
-    <cfRule type="cellIs" dxfId="60" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:K27">
-    <cfRule type="cellIs" dxfId="59" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16:Q27">
-    <cfRule type="cellIs" dxfId="58" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="69" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16:W27">
-    <cfRule type="cellIs" dxfId="57" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4822,16 +4846,16 @@
   </sheetData>
   <autoFilter ref="H1:K16" xr:uid="{8B5509DC-DB05-43E6-A45B-32E76BC27DEA}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:K16">
-      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="56"/>
+      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="67"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="55" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K16">
-    <cfRule type="cellIs" dxfId="54" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5125,11 +5149,11 @@
   </sheetData>
   <autoFilter ref="B1:E16" xr:uid="{4883B1BD-E07A-48BB-9F66-A8C7003F2BEF}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E16">
-      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="53"/>
+      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="64"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="52" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="1" operator="greaterThan">
       <formula>0.699</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5771,30 +5795,30 @@
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{85F09F99-28C1-4BB1-A75C-F2C0B1518057}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q14">
-      <sortCondition sortBy="cellColor" ref="D1" dxfId="51"/>
+      <sortCondition sortBy="cellColor" ref="D1" dxfId="62"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="M2:Q14">
-    <cfRule type="cellIs" dxfId="50" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="6" operator="lessThan">
       <formula>-0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="48" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="4" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="46" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="3" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6238,21 +6262,21 @@
   </sheetData>
   <autoFilter ref="A1:F14" xr:uid="{F6EC43A2-0E96-4311-A986-12EE04542C46}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
-      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="44"/>
+      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="55"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:E1048576">
-    <cfRule type="cellIs" dxfId="43" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:K1">
-    <cfRule type="cellIs" dxfId="42" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K12">
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6265,8 +6289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498CC891-573B-427D-8528-B6E57CC0DFD4}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6879,31 +6903,31 @@
   </sheetData>
   <autoFilter ref="A16:C29" xr:uid="{498CC891-573B-427D-8528-B6E57CC0DFD4}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:C29">
-      <sortCondition sortBy="cellColor" ref="C16:C29" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="C16:C29" dxfId="51"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:C14">
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="5" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G14">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:K14">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:O14">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C29">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7331,16 +7355,16 @@
   </sheetData>
   <autoFilter ref="A1:K1" xr:uid="{2A2FF23C-A49F-4BBF-A172-E01688A2AD61}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K14">
-      <sortCondition sortBy="cellColor" ref="E1" dxfId="40"/>
+      <sortCondition sortBy="cellColor" ref="E1" dxfId="45"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E14">
-    <cfRule type="cellIs" dxfId="39" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:E29">
-    <cfRule type="cellIs" dxfId="38" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7599,16 +7623,16 @@
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{76B16ADE-8397-4523-89E6-FD43024CAE02}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J14">
-      <sortCondition sortBy="cellColor" ref="J1" dxfId="37"/>
+      <sortCondition sortBy="cellColor" ref="J1" dxfId="42"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="36" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="35" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Started analyses with prayer and spiritual healing combined
Found that biofeedback was consistently loading on its own factor. It has the fewest cases reporting yes. Dropped it and now working on analyses without biofeedback.
</commit_message>
<xml_diff>
--- a/R/Factor analysis  - factor loadings.xlsx
+++ b/R/Factor analysis  - factor loadings.xlsx
@@ -1,38 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\git\AHL\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BAE0A9-BF62-4B7F-AF25-60C28C6703E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04988D2-74E7-4C19-A64F-728B3E438E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
   </bookViews>
   <sheets>
     <sheet name="All CAMs" sheetId="1" r:id="rId1"/>
-    <sheet name="Drop energy, pray, spirit" sheetId="10" r:id="rId2"/>
-    <sheet name="Principal Axis Factoring" sheetId="9" r:id="rId3"/>
-    <sheet name="PCA" sheetId="8" r:id="rId4"/>
-    <sheet name="Drop prayer and spirit" sheetId="2" state="hidden" r:id="rId5"/>
-    <sheet name="Mysterious Perfect Model" sheetId="3" r:id="rId6"/>
-    <sheet name="Ex Pray Spirit Comparisons" sheetId="11" r:id="rId7"/>
-    <sheet name="Comparing MPM" sheetId="6" r:id="rId8"/>
-    <sheet name="Numeric" sheetId="5" r:id="rId9"/>
+    <sheet name="Combine Pray and Spirit" sheetId="12" r:id="rId2"/>
+    <sheet name="Drop energy, pray, spirit" sheetId="10" r:id="rId3"/>
+    <sheet name="Principal Axis Factoring" sheetId="9" r:id="rId4"/>
+    <sheet name="PCA" sheetId="8" r:id="rId5"/>
+    <sheet name="Drop prayer and spirit" sheetId="2" state="hidden" r:id="rId6"/>
+    <sheet name="Mysterious Perfect Model" sheetId="3" r:id="rId7"/>
+    <sheet name="Ex Pray Spirit Comparisons" sheetId="11" r:id="rId8"/>
+    <sheet name="Comparing MPM" sheetId="6" r:id="rId9"/>
+    <sheet name="Numeric" sheetId="5" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All CAMs'!$A$1:$AC$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Comparing MPM'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Drop energy, pray, spirit'!$A$15:$E$27</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Drop prayer and spirit'!$A$1:$Q$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Ex Pray Spirit Comparisons'!$A$16:$C$29</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Mysterious Perfect Model'!$A$1:$F$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Numeric!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">PCA!$B$1:$E$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Principal Axis Factoring'!$H$1:$K$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Combine Pray and Spirit'!$A$18:$G$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Comparing MPM'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Drop energy, pray, spirit'!$A$15:$E$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Drop prayer and spirit'!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Ex Pray Spirit Comparisons'!$A$16:$C$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Mysterious Perfect Model'!$A$1:$F$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Numeric!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">PCA!$B$1:$E$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Principal Axis Factoring'!$H$1:$K$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,6 +55,66 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>hanna</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{575DDA7A-1908-4B42-9961-2E4DA5AF87AF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ML varimax
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{1AD95E32-A93F-4250-8A65-83534243FA9D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ML promax
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={05F861C7-3F05-45BE-A842-A70399D00986}</author>
@@ -205,7 +267,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={68C2D0A8-62BB-4214-AD84-976C7BE3AB2B}</author>
@@ -223,7 +285,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={F7A5C9D5-E716-4F51-8BD8-AA873D1AD48D}</author>
@@ -241,7 +303,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -276,7 +338,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -336,7 +398,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -471,7 +533,7 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -531,7 +593,7 @@
 </comments>
 </file>
 
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -567,7 +629,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="50">
   <si>
     <t>ML2</t>
   </si>
@@ -676,6 +738,48 @@
   <si>
     <t>Cumulative Proportion</t>
   </si>
+  <si>
+    <t>Acupuncture</t>
+  </si>
+  <si>
+    <t>Biofeedback</t>
+  </si>
+  <si>
+    <t>Chiropractic</t>
+  </si>
+  <si>
+    <t>Energy Healing</t>
+  </si>
+  <si>
+    <t>Exercise</t>
+  </si>
+  <si>
+    <t>Herbal Therapy</t>
+  </si>
+  <si>
+    <t>Vitamins</t>
+  </si>
+  <si>
+    <t>Homeopathy</t>
+  </si>
+  <si>
+    <t>Hypnosis</t>
+  </si>
+  <si>
+    <t>Imagery</t>
+  </si>
+  <si>
+    <t>Massage</t>
+  </si>
+  <si>
+    <t>Relaxiation</t>
+  </si>
+  <si>
+    <t>Special Diet</t>
+  </si>
+  <si>
+    <t>Prayer/Spiritual</t>
+  </si>
 </sst>
 </file>
 
@@ -736,7 +840,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="77">
+  <dxfs count="119">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -834,6 +938,56 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
@@ -842,6 +996,94 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -852,6 +1094,110 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -892,6 +1238,94 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -912,6 +1346,102 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -932,6 +1462,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -952,6 +1490,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1002,6 +1548,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1032,6 +1586,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1092,6 +1654,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1102,6 +1672,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1122,6 +1700,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1132,6 +1718,76 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
@@ -1146,234 +1802,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1810,7 +2238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A59E54-D4A7-4C25-9D11-CD018EBC24D4}">
   <dimension ref="A1:AD21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -3002,43 +3430,43 @@
   </sheetData>
   <autoFilter ref="A1:AC16" xr:uid="{99B320C6-A597-4E1B-B5FD-F0989543660C}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC16">
-      <sortCondition sortBy="cellColor" ref="AC1:AC16" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="AC1:AC16" dxfId="118"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="Q2:U16">
-    <cfRule type="cellIs" dxfId="30" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="117" priority="17" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H16">
-    <cfRule type="cellIs" dxfId="29" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="116" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="115" priority="13" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C16">
-    <cfRule type="cellIs" dxfId="27" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="114" priority="9" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="113" priority="10" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="112" priority="12" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:N16">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="111" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="110" priority="3" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:AC16">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="109" priority="1" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3047,7 +3475,1027 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C8C1A-CFC6-49AC-B896-635D55B44BA8}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="14.265625" customWidth="1"/>
+    <col min="6" max="6" width="13.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="J2">
+        <v>0.35699999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="J3">
+        <v>0.374</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>-0.108</v>
+      </c>
+      <c r="D4">
+        <v>0.313</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>0.36199999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>0.70799999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="C6">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>0.26</v>
+      </c>
+      <c r="H6">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="J6">
+        <v>-0.11899999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>0.71099999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="D8">
+        <v>0.215</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8">
+        <v>0.49</v>
+      </c>
+      <c r="J8">
+        <v>0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>0.64700000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>0.39</v>
+      </c>
+      <c r="J10">
+        <v>0.23200000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>0.627</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>0.317</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="J12">
+        <v>-0.13600000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>0.23499999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>0.23799999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:J1" xr:uid="{76B16ADE-8397-4523-89E6-FD43024CAE02}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J14">
+      <sortCondition sortBy="cellColor" ref="J1" dxfId="74"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="B2:D14">
+    <cfRule type="cellIs" dxfId="73" priority="2" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:J14">
+    <cfRule type="cellIs" dxfId="72" priority="1" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F695CD81-3D97-4E1C-8866-BD773BF04255}">
+  <dimension ref="A1:O32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.265625" customWidth="1"/>
+    <col min="9" max="9" width="13.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="C2">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="G2">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2">
+        <v>-0.127</v>
+      </c>
+      <c r="L2">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="M2">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="O2">
+        <v>0.76300000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>0.157</v>
+      </c>
+      <c r="C3">
+        <v>0.22</v>
+      </c>
+      <c r="D3">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="E3">
+        <v>0.25</v>
+      </c>
+      <c r="G3">
+        <v>0.63</v>
+      </c>
+      <c r="I3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="O3">
+        <v>0.45600000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4">
+        <v>0.31</v>
+      </c>
+      <c r="C4">
+        <v>0.252</v>
+      </c>
+      <c r="G4">
+        <v>0.437</v>
+      </c>
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4">
+        <v>0.224</v>
+      </c>
+      <c r="L4">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="N4">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="O4">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>0.23</v>
+      </c>
+      <c r="C5">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="D5">
+        <v>0.153</v>
+      </c>
+      <c r="E5">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="F5">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="G5">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="I5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5">
+        <v>-0.159</v>
+      </c>
+      <c r="N5">
+        <v>0.86699999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>0.443</v>
+      </c>
+      <c r="C6">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="D6">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="E6">
+        <v>0.312</v>
+      </c>
+      <c r="F6">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="G6">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="I6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="L6">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="N6">
+        <v>0.443</v>
+      </c>
+      <c r="O6">
+        <v>0.23200000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7">
+        <v>0.185</v>
+      </c>
+      <c r="C7">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="D7">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="F7">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="K7">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="M7">
+        <v>0.45300000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="C8">
+        <v>0.189</v>
+      </c>
+      <c r="D8">
+        <v>0.193</v>
+      </c>
+      <c r="E8">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="F8">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="G8">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="I8" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8">
+        <v>0.221</v>
+      </c>
+      <c r="L8">
+        <v>-0.14899999999999999</v>
+      </c>
+      <c r="M8">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="O8">
+        <v>0.13600000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="C9">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="D9">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="E9">
+        <v>0.115</v>
+      </c>
+      <c r="F9">
+        <v>0.155</v>
+      </c>
+      <c r="G9">
+        <v>0.247</v>
+      </c>
+      <c r="I9" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="M9">
+        <v>-0.105</v>
+      </c>
+      <c r="N9">
+        <v>-0.193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="E10">
+        <v>0.115</v>
+      </c>
+      <c r="F10">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="I10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K10">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="L10">
+        <v>0.23</v>
+      </c>
+      <c r="M10">
+        <v>0.114</v>
+      </c>
+      <c r="O10">
+        <v>-0.18099999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11">
+        <v>0.24</v>
+      </c>
+      <c r="C11">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="F11">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="G11">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="I11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="K11">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="L11">
+        <v>-0.112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12">
+        <v>0.21</v>
+      </c>
+      <c r="C12">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="D12">
+        <v>0.183</v>
+      </c>
+      <c r="E12">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="F12">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="G12">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="I12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12">
+        <v>0.61</v>
+      </c>
+      <c r="L12">
+        <v>0.129</v>
+      </c>
+      <c r="N12">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="O12">
+        <v>-0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D13">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0.217</v>
+      </c>
+      <c r="F13">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="I13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13">
+        <v>0.77100000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="C14">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="D14">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="F14">
+        <v>0.26</v>
+      </c>
+      <c r="G14">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="I14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="M14">
+        <v>-0.113</v>
+      </c>
+      <c r="O14">
+        <v>0.36699999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="C15">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D15">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="E15">
+        <v>0.159</v>
+      </c>
+      <c r="F15">
+        <v>0.111</v>
+      </c>
+      <c r="G15">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="I15" t="s">
+        <v>43</v>
+      </c>
+      <c r="J15">
+        <v>0.873</v>
+      </c>
+      <c r="K15">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="N15">
+        <v>-0.20899999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="E19">
+        <v>0.129</v>
+      </c>
+      <c r="F19">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="G19">
+        <v>0.42599999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20">
+        <v>0.191</v>
+      </c>
+      <c r="E20">
+        <v>-0.17499999999999999</v>
+      </c>
+      <c r="G20">
+        <v>0.72799999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21">
+        <v>-0.13600000000000001</v>
+      </c>
+      <c r="D21">
+        <v>0.186</v>
+      </c>
+      <c r="E21">
+        <v>0.123</v>
+      </c>
+      <c r="F21">
+        <v>0.70799999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="C22">
+        <v>0.128</v>
+      </c>
+      <c r="D22">
+        <v>-0.104</v>
+      </c>
+      <c r="F22">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24">
+        <v>0.22</v>
+      </c>
+      <c r="C24">
+        <v>-0.252</v>
+      </c>
+      <c r="D24">
+        <v>0.49299999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25">
+        <v>0.999</v>
+      </c>
+      <c r="E25">
+        <v>-0.108</v>
+      </c>
+      <c r="F25">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="F26">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="G26">
+        <v>0.39100000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27">
+        <v>1.04</v>
+      </c>
+      <c r="E27">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F27">
+        <v>-0.16800000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C28">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="D28">
+        <v>-0.11799999999999999</v>
+      </c>
+      <c r="E28">
+        <v>-0.158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="D29">
+        <v>0.127</v>
+      </c>
+      <c r="E29">
+        <v>0.124</v>
+      </c>
+      <c r="F29">
+        <v>-0.27500000000000002</v>
+      </c>
+      <c r="G29">
+        <v>0.24099999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="G30">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="D31">
+        <v>-0.14699999999999999</v>
+      </c>
+      <c r="F31">
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="D32">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="G32">
+        <v>-0.13500000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A18:G32" xr:uid="{F695CD81-3D97-4E1C-8866-BD773BF04255}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A19:G32">
+      <sortCondition sortBy="cellColor" ref="G18:G32" dxfId="1"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="B2:G15">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="greaterThan">
+      <formula>0.399</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:O15">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
+      <formula>0.399</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:G32">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThan">
+      <formula>0.399</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DF5018-9911-4233-8E1E-CFEBD8577F16}">
   <dimension ref="A1:W27"/>
   <sheetViews>
@@ -4186,47 +5634,47 @@
   </sheetData>
   <autoFilter ref="A15:E27" xr:uid="{00DF5018-9911-4233-8E1E-CFEBD8577F16}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:E27">
-      <sortCondition sortBy="cellColor" ref="E15:E27" dxfId="76"/>
+      <sortCondition sortBy="cellColor" ref="E15:E27" dxfId="108"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B2:D13">
-    <cfRule type="cellIs" dxfId="75" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="8" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:I13">
-    <cfRule type="cellIs" dxfId="74" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:N13">
-    <cfRule type="cellIs" dxfId="73" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="6" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:S13">
-    <cfRule type="cellIs" dxfId="72" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="104" priority="5" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:E27">
-    <cfRule type="cellIs" dxfId="71" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="103" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:K27">
-    <cfRule type="cellIs" dxfId="70" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="102" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16:Q27">
-    <cfRule type="cellIs" dxfId="69" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16:W27">
-    <cfRule type="cellIs" dxfId="68" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="100" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4235,7 +5683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5509DC-DB05-43E6-A45B-32E76BC27DEA}">
   <dimension ref="A1:K23"/>
   <sheetViews>
@@ -4846,16 +6294,16 @@
   </sheetData>
   <autoFilter ref="H1:K16" xr:uid="{8B5509DC-DB05-43E6-A45B-32E76BC27DEA}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:K16">
-      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="67"/>
+      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="99"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="66" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="98" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K16">
-    <cfRule type="cellIs" dxfId="65" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="97" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4864,7 +6312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4883B1BD-E07A-48BB-9F66-A8C7003F2BEF}">
   <dimension ref="A1:E16"/>
   <sheetViews>
@@ -5149,11 +6597,11 @@
   </sheetData>
   <autoFilter ref="B1:E16" xr:uid="{4883B1BD-E07A-48BB-9F66-A8C7003F2BEF}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E16">
-      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="64"/>
+      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="96"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="63" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="95" priority="1" operator="greaterThan">
       <formula>0.699</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5162,7 +6610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D61808F-2A1D-4F74-9E35-43CB27586058}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
@@ -5795,30 +7243,30 @@
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{85F09F99-28C1-4BB1-A75C-F2C0B1518057}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q14">
-      <sortCondition sortBy="cellColor" ref="D1" dxfId="62"/>
+      <sortCondition sortBy="cellColor" ref="D1" dxfId="94"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="M2:Q14">
-    <cfRule type="cellIs" dxfId="61" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="93" priority="6" operator="lessThan">
       <formula>-0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="92" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="59" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="91" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="90" priority="4" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="57" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="3" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5827,7 +7275,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8727E6E-4063-4F85-BAE5-AB6F095D427F}">
   <dimension ref="A1:K14"/>
   <sheetViews>
@@ -6262,21 +7710,21 @@
   </sheetData>
   <autoFilter ref="A1:F14" xr:uid="{F6EC43A2-0E96-4311-A986-12EE04542C46}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
-      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="55"/>
+      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="87"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:E1048576">
-    <cfRule type="cellIs" dxfId="54" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:K1">
-    <cfRule type="cellIs" dxfId="53" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="85" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K12">
-    <cfRule type="cellIs" dxfId="52" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="84" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6285,7 +7733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498CC891-573B-427D-8528-B6E57CC0DFD4}">
   <dimension ref="A1:O29"/>
   <sheetViews>
@@ -6903,31 +8351,31 @@
   </sheetData>
   <autoFilter ref="A16:C29" xr:uid="{498CC891-573B-427D-8528-B6E57CC0DFD4}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:C29">
-      <sortCondition sortBy="cellColor" ref="C16:C29" dxfId="51"/>
+      <sortCondition sortBy="cellColor" ref="C16:C29" dxfId="83"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:C14">
-    <cfRule type="cellIs" dxfId="50" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="5" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G14">
-    <cfRule type="cellIs" dxfId="49" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="81" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:K14">
-    <cfRule type="cellIs" dxfId="48" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:O14">
-    <cfRule type="cellIs" dxfId="47" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="79" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C29">
-    <cfRule type="cellIs" dxfId="46" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6936,7 +8384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC6BCC2-AE82-430A-9446-637AC6346772}">
   <dimension ref="A1:E29"/>
   <sheetViews>
@@ -7355,284 +8803,16 @@
   </sheetData>
   <autoFilter ref="A1:K1" xr:uid="{2A2FF23C-A49F-4BBF-A172-E01688A2AD61}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K14">
-      <sortCondition sortBy="cellColor" ref="E1" dxfId="45"/>
+      <sortCondition sortBy="cellColor" ref="E1" dxfId="77"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E14">
-    <cfRule type="cellIs" dxfId="44" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:E29">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="greaterThan">
-      <formula>0.299</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C8C1A-CFC6-49AC-B896-635D55B44BA8}">
-  <dimension ref="A1:J14"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="14.265625" customWidth="1"/>
-    <col min="6" max="6" width="13.86328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>0.58099999999999996</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2">
-        <v>0.29299999999999998</v>
-      </c>
-      <c r="J2">
-        <v>0.35699999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3">
-        <v>0.24299999999999999</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="J3">
-        <v>0.374</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>-0.108</v>
-      </c>
-      <c r="D4">
-        <v>0.313</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4">
-        <v>0.36199999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>0.52700000000000002</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5">
-        <v>0.70799999999999996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>0.28699999999999998</v>
-      </c>
-      <c r="C6">
-        <v>0.34200000000000003</v>
-      </c>
-      <c r="F6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>0.26</v>
-      </c>
-      <c r="H6">
-        <v>0.36899999999999999</v>
-      </c>
-      <c r="J6">
-        <v>-0.11899999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>0.71199999999999997</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7">
-        <v>0.71099999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>0.45500000000000002</v>
-      </c>
-      <c r="D8">
-        <v>0.215</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8">
-        <v>0.49</v>
-      </c>
-      <c r="J8">
-        <v>0.13700000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>0.66100000000000003</v>
-      </c>
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9">
-        <v>0.64700000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>0.34699999999999998</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10">
-        <v>0.39</v>
-      </c>
-      <c r="J10">
-        <v>0.23200000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>0.63800000000000001</v>
-      </c>
-      <c r="F11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11">
-        <v>0.627</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>0.317</v>
-      </c>
-      <c r="F12" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="J12">
-        <v>-0.13600000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="F13" t="s">
-        <v>3</v>
-      </c>
-      <c r="H13">
-        <v>0.23499999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14">
-        <v>0.22800000000000001</v>
-      </c>
-      <c r="F14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14">
-        <v>0.23799999999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:J1" xr:uid="{76B16ADE-8397-4523-89E6-FD43024CAE02}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J14">
-      <sortCondition sortBy="cellColor" ref="J1" dxfId="42"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="41" priority="2" operator="greaterThan">
-      <formula>0.299</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="40" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Writing up EFA results
</commit_message>
<xml_diff>
--- a/R/Factor analysis  - factor loadings.xlsx
+++ b/R/Factor analysis  - factor loadings.xlsx
@@ -8,35 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\git\AHL\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D979F4D-66FA-4C39-BB33-7E58A1FDAD97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18694EE0-267A-4391-9BBE-1110E7EC3639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="3" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
   </bookViews>
   <sheets>
     <sheet name="All CAMs" sheetId="1" r:id="rId1"/>
     <sheet name="Combine Pray and Spirit" sheetId="12" r:id="rId2"/>
     <sheet name="Comb Pray Spirit Drop Bio" sheetId="13" r:id="rId3"/>
-    <sheet name="Drop energy, pray, spirit" sheetId="10" r:id="rId4"/>
-    <sheet name="Principal Axis Factoring" sheetId="9" r:id="rId5"/>
-    <sheet name="PCA" sheetId="8" r:id="rId6"/>
-    <sheet name="Drop prayer and spirit" sheetId="2" state="hidden" r:id="rId7"/>
-    <sheet name="Mysterious Perfect Model" sheetId="3" r:id="rId8"/>
-    <sheet name="Ex Pray Spirit Comparisons" sheetId="11" r:id="rId9"/>
-    <sheet name="Comparing MPM" sheetId="6" r:id="rId10"/>
-    <sheet name="Numeric" sheetId="5" r:id="rId11"/>
+    <sheet name="Final EFA" sheetId="14" r:id="rId4"/>
+    <sheet name="Drop energy, pray, spirit" sheetId="10" r:id="rId5"/>
+    <sheet name="Principal Axis Factoring" sheetId="9" r:id="rId6"/>
+    <sheet name="PCA" sheetId="8" r:id="rId7"/>
+    <sheet name="Drop prayer and spirit" sheetId="2" state="hidden" r:id="rId8"/>
+    <sheet name="Mysterious Perfect Model" sheetId="3" r:id="rId9"/>
+    <sheet name="Ex Pray Spirit Comparisons" sheetId="11" r:id="rId10"/>
+    <sheet name="Comparing MPM" sheetId="6" r:id="rId11"/>
+    <sheet name="Numeric" sheetId="5" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All CAMs'!$A$1:$AC$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Comb Pray Spirit Drop Bio'!$H$46:$L$59</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Combine Pray and Spirit'!$H$51:$M$65</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Comparing MPM'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Drop energy, pray, spirit'!$A$15:$E$27</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Drop prayer and spirit'!$A$1:$Q$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Ex Pray Spirit Comparisons'!$A$16:$C$29</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Mysterious Perfect Model'!$A$1:$F$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Numeric!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">PCA!$B$1:$E$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Principal Axis Factoring'!$H$1:$K$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Comparing MPM'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Drop energy, pray, spirit'!$A$15:$E$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Drop prayer and spirit'!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Ex Pray Spirit Comparisons'!$A$16:$C$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Mysterious Perfect Model'!$A$1:$F$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Numeric!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">PCA!$B$1:$E$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Principal Axis Factoring'!$H$1:$K$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -265,6 +266,66 @@
 </file>
 
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>hanna</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{D5712E48-0578-4E7B-970F-9D684F744419}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Four factor model excluding prayer and spiritual healing using MIDUS-complete data
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{6A9F4E1D-6D92-4062-8A79-2B5448FE1065}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Four factor model, prayer and spiritual healing dropped. 
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -508,6 +569,40 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>hanna</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{184B6EB6-15CF-40F7-A145-000C47DA5B99}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ML Cluster</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>tc={05F861C7-3F05-45BE-A842-A70399D00986}</author>
     <author>tc={15ED4DD3-15BC-4E0F-AD77-76216B25453F}</author>
     <author>hanna</author>
@@ -658,7 +753,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={68C2D0A8-62BB-4214-AD84-976C7BE3AB2B}</author>
@@ -676,7 +771,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={F7A5C9D5-E716-4F51-8BD8-AA873D1AD48D}</author>
@@ -694,7 +789,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -729,7 +824,7 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -789,7 +884,7 @@
 </comments>
 </file>
 
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -924,68 +1019,8 @@
 </comments>
 </file>
 
-<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>hanna</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{D5712E48-0578-4E7B-970F-9D684F744419}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>hanna:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Four factor model excluding prayer and spiritual healing using MIDUS-complete data
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{6A9F4E1D-6D92-4062-8A79-2B5448FE1065}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>hanna:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Four factor model, prayer and spiritual healing dropped. 
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="60">
   <si>
     <t>ML2</t>
   </si>
@@ -1139,6 +1174,33 @@
   <si>
     <t>aPraySpirit</t>
   </si>
+  <si>
+    <t>Exercise or Movement Therapy</t>
+  </si>
+  <si>
+    <t>Herbal</t>
+  </si>
+  <si>
+    <t>Imagery Techniques</t>
+  </si>
+  <si>
+    <t>Relaxation and Meditation</t>
+  </si>
+  <si>
+    <t>Prayer or Spiritual Healing</t>
+  </si>
+  <si>
+    <t>Mind-Body Practices</t>
+  </si>
+  <si>
+    <t>Alternative Systems</t>
+  </si>
+  <si>
+    <t>Physical and Nutritional Approaches</t>
+  </si>
+  <si>
+    <t>Manipulative Treatments</t>
+  </si>
 </sst>
 </file>
 
@@ -1199,71 +1261,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="161">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="70">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1271,940 +1269,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2471,6 +1535,222 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
           <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4197,43 +3477,43 @@
   </sheetData>
   <autoFilter ref="A1:AC16" xr:uid="{99B320C6-A597-4E1B-B5FD-F0989543660C}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC16">
-      <sortCondition sortBy="cellColor" ref="AC1:AC16" dxfId="160"/>
+      <sortCondition sortBy="cellColor" ref="AC1:AC16" dxfId="69"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="Q2:U16">
-    <cfRule type="cellIs" dxfId="159" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="17" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H16">
-    <cfRule type="cellIs" dxfId="158" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="13" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C16">
-    <cfRule type="cellIs" dxfId="156" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="9" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="10" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="12" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:N16">
-    <cfRule type="cellIs" dxfId="153" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="3" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:AC16">
-    <cfRule type="cellIs" dxfId="151" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="1" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4243,6 +3523,657 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498CC891-573B-427D-8528-B6E57CC0DFD4}">
+  <dimension ref="A1:O29"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.86328125" customWidth="1"/>
+    <col min="9" max="9" width="13.53125" customWidth="1"/>
+    <col min="13" max="13" width="13.06640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="C2">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="G2">
+        <v>0.52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>0.436</v>
+      </c>
+      <c r="K2">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="M2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="O2">
+        <v>0.39300000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="C3">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="K3">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="M3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>0.60199999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="C4">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G4">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="M4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>0.53</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>0.502</v>
+      </c>
+      <c r="M5" t="s">
+        <v>7</v>
+      </c>
+      <c r="O5">
+        <v>0.873</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>0.98</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="M6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6">
+        <v>0.628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7">
+        <v>-0.12</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="M7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="C8">
+        <v>0.307</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="I8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="M8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="O8">
+        <v>0.42399999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0.434</v>
+      </c>
+      <c r="C9">
+        <v>0.504</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="G9">
+        <v>-0.125</v>
+      </c>
+      <c r="I9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="M9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9">
+        <v>0.214</v>
+      </c>
+      <c r="O9">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>0.33</v>
+      </c>
+      <c r="C10">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="I10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="M10" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>0.64900000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>0.12</v>
+      </c>
+      <c r="C11">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="I11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="M11" t="s">
+        <v>6</v>
+      </c>
+      <c r="N11">
+        <v>0.377</v>
+      </c>
+      <c r="O11">
+        <v>0.27600000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="C12">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <v>0.98</v>
+      </c>
+      <c r="G12">
+        <v>-0.11899999999999999</v>
+      </c>
+      <c r="I12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="M12" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12">
+        <v>0.52800000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>0.503</v>
+      </c>
+      <c r="C13">
+        <v>0.246</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>0.45</v>
+      </c>
+      <c r="G13">
+        <v>0.254</v>
+      </c>
+      <c r="I13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="K13">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="M13" t="s">
+        <v>11</v>
+      </c>
+      <c r="N13">
+        <v>0.96199999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="C14">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0.184</v>
+      </c>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14">
+        <v>0.36</v>
+      </c>
+      <c r="K14">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="M14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14">
+        <v>0.97899999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="C17">
+        <v>0.33100000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="C18">
+        <v>0.67200000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>0.437</v>
+      </c>
+      <c r="C19">
+        <v>0.44800000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>0.81</v>
+      </c>
+      <c r="C20">
+        <v>0.34799999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="C21">
+        <v>0.312</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="C22">
+        <v>0.84399999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="C23">
+        <v>0.42099999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="C24">
+        <v>0.32400000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="C25">
+        <v>0.57699999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="C26">
+        <v>0.44800000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="C27">
+        <v>0.88100000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>0.436</v>
+      </c>
+      <c r="C28">
+        <v>0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="C29">
+        <v>0.29199999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A16:C29" xr:uid="{498CC891-573B-427D-8528-B6E57CC0DFD4}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:C29">
+      <sortCondition sortBy="cellColor" ref="C16:C29" dxfId="12"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="B2:C14">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:G14">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:K14">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:O14">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:C29">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC6BCC2-AE82-430A-9446-637AC6346772}">
   <dimension ref="A1:E29"/>
   <sheetViews>
@@ -4661,16 +4592,16 @@
   </sheetData>
   <autoFilter ref="A1:K1" xr:uid="{2A2FF23C-A49F-4BBF-A172-E01688A2AD61}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K14">
-      <sortCondition sortBy="cellColor" ref="E1" dxfId="119"/>
+      <sortCondition sortBy="cellColor" ref="E1" dxfId="6"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E14">
-    <cfRule type="cellIs" dxfId="118" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:E29">
-    <cfRule type="cellIs" dxfId="117" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4679,7 +4610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C8C1A-CFC6-49AC-B896-635D55B44BA8}">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -4929,16 +4860,16 @@
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{76B16ADE-8397-4523-89E6-FD43024CAE02}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J14">
-      <sortCondition sortBy="cellColor" ref="J1" dxfId="116"/>
+      <sortCondition sortBy="cellColor" ref="J1" dxfId="3"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="115" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="114" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6675,58 +6606,58 @@
   </sheetData>
   <autoFilter ref="H51:M65" xr:uid="{F695CD81-3D97-4E1C-8866-BD773BF04255}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H52:M65">
-      <sortCondition sortBy="cellColor" ref="L51:L65" dxfId="113"/>
+      <sortCondition sortBy="cellColor" ref="L51:L65" dxfId="59"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:G15">
-    <cfRule type="cellIs" dxfId="112" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="12" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:O15">
-    <cfRule type="cellIs" dxfId="111" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="11" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:G32">
-    <cfRule type="cellIs" dxfId="110" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="10" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:O32">
-    <cfRule type="cellIs" dxfId="109" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="9" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:F49">
-    <cfRule type="cellIs" dxfId="108" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="8" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:M49">
-    <cfRule type="cellIs" dxfId="107" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="7" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:F65">
-    <cfRule type="cellIs" dxfId="106" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="6" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I52:M65">
-    <cfRule type="cellIs" dxfId="101" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="5" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="4" operator="greaterThan">
       <formula>0.395</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="3" operator="greaterThan">
       <formula>0.39</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="2" operator="greaterThan">
       <formula>0.35</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="1" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6739,8 +6670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C42105-EFDA-4FA3-8AB1-E5E42D4D4CA4}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F46" zoomScale="140" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView topLeftCell="F46" zoomScale="140" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46:L59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8208,46 +8139,46 @@
   </sheetData>
   <autoFilter ref="H46:L59" xr:uid="{26C42105-EFDA-4FA3-8AB1-E5E42D4D4CA4}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H47:L59">
-      <sortCondition sortBy="cellColor" ref="L46:L59" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="L46:L59" dxfId="46"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:F14">
-    <cfRule type="cellIs" dxfId="22" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="8" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:M14">
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="7" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:F29">
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="6" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:M29">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="5" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:E44">
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="4" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32:L44">
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="3" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:E59">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="2" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47:L59">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="1" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8257,6 +8188,212 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984B0D20-5E48-4763-A83B-7B371039BA3E}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="26.06640625" customWidth="1"/>
+    <col min="2" max="2" width="17.1328125" customWidth="1"/>
+    <col min="3" max="3" width="16.19921875" customWidth="1"/>
+    <col min="4" max="4" width="29.19921875" customWidth="1"/>
+    <col min="5" max="5" width="21.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2">
+        <v>-0.16800000000000001</v>
+      </c>
+      <c r="C2">
+        <v>0.251</v>
+      </c>
+      <c r="E2">
+        <v>0.56499999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="E3">
+        <v>0.79200000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4">
+        <v>-0.20699999999999999</v>
+      </c>
+      <c r="D4">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="E4">
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="D5">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="E5">
+        <v>-0.18099999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6">
+        <v>0.104</v>
+      </c>
+      <c r="D6">
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7">
+        <v>0.214</v>
+      </c>
+      <c r="C7">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="D7">
+        <v>-0.26600000000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="D8">
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9">
+        <v>0.66</v>
+      </c>
+      <c r="D9">
+        <v>0.318</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="C10">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="E10">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="C11">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="D11">
+        <v>-0.37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="C13">
+        <v>-0.104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="D14">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="E14">
+        <v>-0.215</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:E14">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0.399</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DF5018-9911-4233-8E1E-CFEBD8577F16}">
   <dimension ref="A1:W27"/>
   <sheetViews>
@@ -9395,47 +9532,47 @@
   </sheetData>
   <autoFilter ref="A15:E27" xr:uid="{00DF5018-9911-4233-8E1E-CFEBD8577F16}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:E27">
-      <sortCondition sortBy="cellColor" ref="E15:E27" dxfId="150"/>
+      <sortCondition sortBy="cellColor" ref="E15:E27" dxfId="37"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B2:D13">
-    <cfRule type="cellIs" dxfId="149" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="8" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:I13">
-    <cfRule type="cellIs" dxfId="148" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:N13">
-    <cfRule type="cellIs" dxfId="147" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:S13">
-    <cfRule type="cellIs" dxfId="146" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:E27">
-    <cfRule type="cellIs" dxfId="145" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:K27">
-    <cfRule type="cellIs" dxfId="144" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16:Q27">
-    <cfRule type="cellIs" dxfId="143" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16:W27">
-    <cfRule type="cellIs" dxfId="142" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9444,7 +9581,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5509DC-DB05-43E6-A45B-32E76BC27DEA}">
   <dimension ref="A1:K23"/>
   <sheetViews>
@@ -10055,16 +10192,16 @@
   </sheetData>
   <autoFilter ref="H1:K16" xr:uid="{8B5509DC-DB05-43E6-A45B-32E76BC27DEA}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:K16">
-      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="141"/>
+      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="28"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="140" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K16">
-    <cfRule type="cellIs" dxfId="139" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10073,7 +10210,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4883B1BD-E07A-48BB-9F66-A8C7003F2BEF}">
   <dimension ref="A1:E16"/>
   <sheetViews>
@@ -10358,11 +10495,11 @@
   </sheetData>
   <autoFilter ref="B1:E16" xr:uid="{4883B1BD-E07A-48BB-9F66-A8C7003F2BEF}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E16">
-      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="138"/>
+      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="25"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="137" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="greaterThan">
       <formula>0.699</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10371,7 +10508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D61808F-2A1D-4F74-9E35-43CB27586058}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
@@ -11004,30 +11141,30 @@
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{85F09F99-28C1-4BB1-A75C-F2C0B1518057}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q14">
-      <sortCondition sortBy="cellColor" ref="D1" dxfId="136"/>
+      <sortCondition sortBy="cellColor" ref="D1" dxfId="23"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="M2:Q14">
-    <cfRule type="cellIs" dxfId="135" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="lessThan">
       <formula>-0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="133" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="131" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11036,7 +11173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8727E6E-4063-4F85-BAE5-AB6F095D427F}">
   <dimension ref="A1:K14"/>
   <sheetViews>
@@ -11471,672 +11608,21 @@
   </sheetData>
   <autoFilter ref="A1:F14" xr:uid="{F6EC43A2-0E96-4311-A986-12EE04542C46}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
-      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="129"/>
+      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="16"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:E1048576">
-    <cfRule type="cellIs" dxfId="128" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:K1">
-    <cfRule type="cellIs" dxfId="127" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K12">
-    <cfRule type="cellIs" dxfId="126" priority="1" operator="greaterThan">
-      <formula>0.299</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498CC891-573B-427D-8528-B6E57CC0DFD4}">
-  <dimension ref="A1:O29"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.86328125" customWidth="1"/>
-    <col min="9" max="9" width="13.53125" customWidth="1"/>
-    <col min="13" max="13" width="13.06640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>0.32200000000000001</v>
-      </c>
-      <c r="C2">
-        <v>0.59099999999999997</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>0.41299999999999998</v>
-      </c>
-      <c r="G2">
-        <v>0.52</v>
-      </c>
-      <c r="I2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2">
-        <v>0.436</v>
-      </c>
-      <c r="K2">
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="M2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2">
-        <v>0.55200000000000005</v>
-      </c>
-      <c r="O2">
-        <v>0.39300000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>0.66100000000000003</v>
-      </c>
-      <c r="C3">
-        <v>0.57699999999999996</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>0.65600000000000003</v>
-      </c>
-      <c r="I3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3">
-        <v>0.30599999999999999</v>
-      </c>
-      <c r="K3">
-        <v>0.35199999999999998</v>
-      </c>
-      <c r="M3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3">
-        <v>0.60199999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>0.45500000000000002</v>
-      </c>
-      <c r="C4">
-        <v>0.40200000000000002</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="G4">
-        <v>0.35499999999999998</v>
-      </c>
-      <c r="I4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4">
-        <v>0.61899999999999999</v>
-      </c>
-      <c r="M4" t="s">
-        <v>4</v>
-      </c>
-      <c r="O4">
-        <v>0.48799999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>0.36599999999999999</v>
-      </c>
-      <c r="C5">
-        <v>0.81399999999999995</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>0.53</v>
-      </c>
-      <c r="I5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5">
-        <v>0.502</v>
-      </c>
-      <c r="M5" t="s">
-        <v>7</v>
-      </c>
-      <c r="O5">
-        <v>0.873</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>0.30199999999999999</v>
-      </c>
-      <c r="C6">
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6">
-        <v>0.98</v>
-      </c>
-      <c r="I6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6">
-        <v>0.91900000000000004</v>
-      </c>
-      <c r="M6" t="s">
-        <v>8</v>
-      </c>
-      <c r="O6">
-        <v>0.628</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>0.32900000000000001</v>
-      </c>
-      <c r="C7">
-        <v>0.82899999999999996</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7">
-        <v>-0.12</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7">
-        <v>0.93600000000000005</v>
-      </c>
-      <c r="M7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O7">
-        <v>0.91400000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>0.85499999999999998</v>
-      </c>
-      <c r="C8">
-        <v>0.307</v>
-      </c>
-      <c r="E8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>0.64400000000000002</v>
-      </c>
-      <c r="I8" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8">
-        <v>0.61899999999999999</v>
-      </c>
-      <c r="M8" t="s">
-        <v>12</v>
-      </c>
-      <c r="N8">
-        <v>0.29099999999999998</v>
-      </c>
-      <c r="O8">
-        <v>0.42399999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>0.434</v>
-      </c>
-      <c r="C9">
-        <v>0.504</v>
-      </c>
-      <c r="E9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9">
-        <v>0.52400000000000002</v>
-      </c>
-      <c r="G9">
-        <v>-0.125</v>
-      </c>
-      <c r="I9" t="s">
-        <v>4</v>
-      </c>
-      <c r="J9">
-        <v>0.49199999999999999</v>
-      </c>
-      <c r="M9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N9">
-        <v>0.214</v>
-      </c>
-      <c r="O9">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>0.33</v>
-      </c>
-      <c r="C10">
-        <v>0.39700000000000002</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10">
-        <v>0.93600000000000005</v>
-      </c>
-      <c r="I10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10">
-        <v>0.89100000000000001</v>
-      </c>
-      <c r="M10" t="s">
-        <v>3</v>
-      </c>
-      <c r="N10">
-        <v>0.64900000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>0.12</v>
-      </c>
-      <c r="C11">
-        <v>0.41899999999999998</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11">
-        <v>0.67300000000000004</v>
-      </c>
-      <c r="I11" t="s">
-        <v>8</v>
-      </c>
-      <c r="J11">
-        <v>0.64400000000000002</v>
-      </c>
-      <c r="M11" t="s">
-        <v>6</v>
-      </c>
-      <c r="N11">
-        <v>0.377</v>
-      </c>
-      <c r="O11">
-        <v>0.27600000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>0.59799999999999998</v>
-      </c>
-      <c r="C12">
-        <v>0.25700000000000001</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12">
-        <v>0.98</v>
-      </c>
-      <c r="G12">
-        <v>-0.11899999999999999</v>
-      </c>
-      <c r="I12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="M12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N12">
-        <v>0.52800000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>0.503</v>
-      </c>
-      <c r="C13">
-        <v>0.246</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13">
-        <v>0.45</v>
-      </c>
-      <c r="G13">
-        <v>0.254</v>
-      </c>
-      <c r="I13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13">
-        <v>0.45100000000000001</v>
-      </c>
-      <c r="K13">
-        <v>0.26700000000000002</v>
-      </c>
-      <c r="M13" t="s">
-        <v>11</v>
-      </c>
-      <c r="N13">
-        <v>0.96199999999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>0.86299999999999999</v>
-      </c>
-      <c r="C14">
-        <v>0.29299999999999998</v>
-      </c>
-      <c r="E14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14">
-        <v>0.36099999999999999</v>
-      </c>
-      <c r="G14">
-        <v>0.184</v>
-      </c>
-      <c r="I14" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14">
-        <v>0.36</v>
-      </c>
-      <c r="K14">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="M14" t="s">
-        <v>14</v>
-      </c>
-      <c r="N14">
-        <v>0.97899999999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17">
-        <v>0.56200000000000006</v>
-      </c>
-      <c r="C17">
-        <v>0.33100000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18">
-        <v>0.58299999999999996</v>
-      </c>
-      <c r="C18">
-        <v>0.67200000000000004</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19">
-        <v>0.437</v>
-      </c>
-      <c r="C19">
-        <v>0.44800000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20">
-        <v>0.81</v>
-      </c>
-      <c r="C20">
-        <v>0.34799999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21">
-        <v>0.83399999999999996</v>
-      </c>
-      <c r="C21">
-        <v>0.312</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22">
-        <v>0.31900000000000001</v>
-      </c>
-      <c r="C22">
-        <v>0.84399999999999997</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23">
-        <v>0.54800000000000004</v>
-      </c>
-      <c r="C23">
-        <v>0.42099999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24">
-        <v>0.40899999999999997</v>
-      </c>
-      <c r="C24">
-        <v>0.32400000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25">
-        <v>0.28199999999999997</v>
-      </c>
-      <c r="C25">
-        <v>0.57699999999999996</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26">
-        <v>0.27800000000000002</v>
-      </c>
-      <c r="C26">
-        <v>0.44800000000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27">
-        <v>0.28499999999999998</v>
-      </c>
-      <c r="C27">
-        <v>0.88100000000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28">
-        <v>0.436</v>
-      </c>
-      <c r="C28">
-        <v>0.13700000000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29">
-        <v>0.58199999999999996</v>
-      </c>
-      <c r="C29">
-        <v>0.29199999999999998</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A16:C29" xr:uid="{498CC891-573B-427D-8528-B6E57CC0DFD4}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:C29">
-      <sortCondition sortBy="cellColor" ref="C16:C29" dxfId="125"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="B2:C14">
-    <cfRule type="cellIs" dxfId="124" priority="5" operator="greaterThan">
-      <formula>0.299</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:G14">
-    <cfRule type="cellIs" dxfId="123" priority="4" operator="greaterThan">
-      <formula>0.299</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2:K14">
-    <cfRule type="cellIs" dxfId="122" priority="3" operator="greaterThan">
-      <formula>0.299</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:O14">
-    <cfRule type="cellIs" dxfId="121" priority="2" operator="greaterThan">
-      <formula>0.299</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17:C29">
-    <cfRule type="cellIs" dxfId="120" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Created EFA loadings table
</commit_message>
<xml_diff>
--- a/R/Factor analysis  - factor loadings.xlsx
+++ b/R/Factor analysis  - factor loadings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\git\AHL\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18694EE0-267A-4391-9BBE-1110E7EC3639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5F4907-F4B0-4278-A3E5-D9990C356BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="3" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
   </bookViews>
@@ -1293,248 +1293,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1619,10 +1383,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1707,10 +1473,262 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1843,92 +1861,74 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3481,39 +3481,39 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="Q2:U16">
-    <cfRule type="cellIs" dxfId="68" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="17" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H16">
-    <cfRule type="cellIs" dxfId="67" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="13" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C16">
-    <cfRule type="cellIs" dxfId="65" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="9" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="10" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="12" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:N16">
-    <cfRule type="cellIs" dxfId="62" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="3" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:AC16">
-    <cfRule type="cellIs" dxfId="60" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="1" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4140,31 +4140,31 @@
   </sheetData>
   <autoFilter ref="A16:C29" xr:uid="{498CC891-573B-427D-8528-B6E57CC0DFD4}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:C29">
-      <sortCondition sortBy="cellColor" ref="C16:C29" dxfId="12"/>
+      <sortCondition sortBy="cellColor" ref="C16:C29" dxfId="61"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:C14">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G14">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:K14">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:O14">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C29">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4592,16 +4592,16 @@
   </sheetData>
   <autoFilter ref="A1:K1" xr:uid="{2A2FF23C-A49F-4BBF-A172-E01688A2AD61}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K14">
-      <sortCondition sortBy="cellColor" ref="E1" dxfId="6"/>
+      <sortCondition sortBy="cellColor" ref="E1" dxfId="60"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E14">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:E29">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4860,16 +4860,16 @@
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{76B16ADE-8397-4523-89E6-FD43024CAE02}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J14">
-      <sortCondition sortBy="cellColor" ref="J1" dxfId="3"/>
+      <sortCondition sortBy="cellColor" ref="J1" dxfId="59"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6606,58 +6606,58 @@
   </sheetData>
   <autoFilter ref="H51:M65" xr:uid="{F695CD81-3D97-4E1C-8866-BD773BF04255}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H52:M65">
-      <sortCondition sortBy="cellColor" ref="L51:L65" dxfId="59"/>
+      <sortCondition sortBy="cellColor" ref="L51:L65" dxfId="68"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:G15">
-    <cfRule type="cellIs" dxfId="58" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="12" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:O15">
-    <cfRule type="cellIs" dxfId="57" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="11" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:G32">
-    <cfRule type="cellIs" dxfId="56" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="10" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:O32">
-    <cfRule type="cellIs" dxfId="55" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="9" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:F49">
-    <cfRule type="cellIs" dxfId="54" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="8" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:M49">
-    <cfRule type="cellIs" dxfId="53" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="7" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:F65">
-    <cfRule type="cellIs" dxfId="52" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="6" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I52:M65">
-    <cfRule type="cellIs" dxfId="51" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="2" operator="greaterThan">
+      <formula>0.35</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="3" operator="greaterThan">
+      <formula>0.39</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="4" operator="greaterThan">
       <formula>0.395</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="3" operator="greaterThan">
-      <formula>0.39</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="2" operator="greaterThan">
-      <formula>0.35</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="5" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8139,46 +8139,46 @@
   </sheetData>
   <autoFilter ref="H46:L59" xr:uid="{26C42105-EFDA-4FA3-8AB1-E5E42D4D4CA4}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H47:L59">
-      <sortCondition sortBy="cellColor" ref="L46:L59" dxfId="46"/>
+      <sortCondition sortBy="cellColor" ref="L46:L59" dxfId="67"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:F14">
-    <cfRule type="cellIs" dxfId="45" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="8" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:M14">
-    <cfRule type="cellIs" dxfId="44" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="7" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:F29">
-    <cfRule type="cellIs" dxfId="43" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="6" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:M29">
-    <cfRule type="cellIs" dxfId="42" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="5" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:E44">
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="4" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32:L44">
-    <cfRule type="cellIs" dxfId="40" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:E59">
-    <cfRule type="cellIs" dxfId="39" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47:L59">
-    <cfRule type="cellIs" dxfId="38" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8192,7 +8192,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8384,7 +8384,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:E14">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9532,47 +9532,47 @@
   </sheetData>
   <autoFilter ref="A15:E27" xr:uid="{00DF5018-9911-4233-8E1E-CFEBD8577F16}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:E27">
-      <sortCondition sortBy="cellColor" ref="E15:E27" dxfId="37"/>
+      <sortCondition sortBy="cellColor" ref="E15:E27" dxfId="66"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B2:D13">
-    <cfRule type="cellIs" dxfId="36" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="8" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:I13">
-    <cfRule type="cellIs" dxfId="35" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:N13">
-    <cfRule type="cellIs" dxfId="34" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="6" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:S13">
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:E27">
-    <cfRule type="cellIs" dxfId="32" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:K27">
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16:Q27">
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16:W27">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10192,16 +10192,16 @@
   </sheetData>
   <autoFilter ref="H1:K16" xr:uid="{8B5509DC-DB05-43E6-A45B-32E76BC27DEA}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:K16">
-      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="28"/>
+      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="65"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K16">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10495,11 +10495,11 @@
   </sheetData>
   <autoFilter ref="B1:E16" xr:uid="{4883B1BD-E07A-48BB-9F66-A8C7003F2BEF}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E16">
-      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="25"/>
+      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="64"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="greaterThan">
       <formula>0.699</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11141,30 +11141,30 @@
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{85F09F99-28C1-4BB1-A75C-F2C0B1518057}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q14">
-      <sortCondition sortBy="cellColor" ref="D1" dxfId="23"/>
+      <sortCondition sortBy="cellColor" ref="D1" dxfId="63"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="M2:Q14">
-    <cfRule type="cellIs" dxfId="22" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="lessThan">
       <formula>-0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11608,21 +11608,21 @@
   </sheetData>
   <autoFilter ref="A1:F14" xr:uid="{F6EC43A2-0E96-4311-A986-12EE04542C46}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
-      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="16"/>
+      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="62"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:E1048576">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:K1">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K12">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added gooodness of fit table for all analysis, standardized loadings table for cfas
Wrote up efa factor loadings results as well.
</commit_message>
<xml_diff>
--- a/R/Factor analysis  - factor loadings.xlsx
+++ b/R/Factor analysis  - factor loadings.xlsx
@@ -1,43 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\git\AHL\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5F4907-F4B0-4278-A3E5-D9990C356BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45970B3F-DACE-4E45-9B15-C7B1414355CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="3" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" firstSheet="1" activeTab="5" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
   </bookViews>
   <sheets>
     <sheet name="All CAMs" sheetId="1" r:id="rId1"/>
     <sheet name="Combine Pray and Spirit" sheetId="12" r:id="rId2"/>
     <sheet name="Comb Pray Spirit Drop Bio" sheetId="13" r:id="rId3"/>
     <sheet name="Final EFA" sheetId="14" r:id="rId4"/>
-    <sheet name="Drop energy, pray, spirit" sheetId="10" r:id="rId5"/>
-    <sheet name="Principal Axis Factoring" sheetId="9" r:id="rId6"/>
-    <sheet name="PCA" sheetId="8" r:id="rId7"/>
-    <sheet name="Drop prayer and spirit" sheetId="2" state="hidden" r:id="rId8"/>
-    <sheet name="Mysterious Perfect Model" sheetId="3" r:id="rId9"/>
-    <sheet name="Ex Pray Spirit Comparisons" sheetId="11" r:id="rId10"/>
-    <sheet name="Comparing MPM" sheetId="6" r:id="rId11"/>
-    <sheet name="Numeric" sheetId="5" r:id="rId12"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId5"/>
+    <sheet name="CFA std loadings" sheetId="16" r:id="rId6"/>
+    <sheet name="Drop energy, pray, spirit" sheetId="10" r:id="rId7"/>
+    <sheet name="Principal Axis Factoring" sheetId="9" r:id="rId8"/>
+    <sheet name="PCA" sheetId="8" r:id="rId9"/>
+    <sheet name="Drop prayer and spirit" sheetId="2" state="hidden" r:id="rId10"/>
+    <sheet name="Mysterious Perfect Model" sheetId="3" r:id="rId11"/>
+    <sheet name="Ex Pray Spirit Comparisons" sheetId="11" r:id="rId12"/>
+    <sheet name="Comparing MPM" sheetId="6" r:id="rId13"/>
+    <sheet name="Numeric" sheetId="5" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All CAMs'!$A$1:$AC$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Comb Pray Spirit Drop Bio'!$H$46:$L$59</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Combine Pray and Spirit'!$H$51:$M$65</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Comparing MPM'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Drop energy, pray, spirit'!$A$15:$E$27</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Drop prayer and spirit'!$A$1:$Q$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Ex Pray Spirit Comparisons'!$A$16:$C$29</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Mysterious Perfect Model'!$A$1:$F$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Numeric!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">PCA!$B$1:$E$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Principal Axis Factoring'!$H$1:$K$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Comparing MPM'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Drop energy, pray, spirit'!$A$15:$E$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Drop prayer and spirit'!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Ex Pray Spirit Comparisons'!$A$16:$C$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Mysterious Perfect Model'!$A$1:$F$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">Numeric!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">PCA!$B$1:$E$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Principal Axis Factoring'!$H$1:$K$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet1!$A$1:$E$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1020,7 +1023,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="69">
   <si>
     <t>ML2</t>
   </si>
@@ -1201,6 +1204,33 @@
   <si>
     <t>Manipulative Treatments</t>
   </si>
+  <si>
+    <t>Factor 1 (Mind Body Practices)</t>
+  </si>
+  <si>
+    <t>Relaxation and Meditation Techniques</t>
+  </si>
+  <si>
+    <t>Factor 2 (Alternative Medical Systems)</t>
+  </si>
+  <si>
+    <t>Factor 3 (Physical and Nutritional Approaches)</t>
+  </si>
+  <si>
+    <t>Exercise and Movement</t>
+  </si>
+  <si>
+    <t>Factor 4 (Manipulative Treatments)</t>
+  </si>
+  <si>
+    <t>Wave 1</t>
+  </si>
+  <si>
+    <t>Wave 2</t>
+  </si>
+  <si>
+    <t>Wave 3</t>
+  </si>
 </sst>
 </file>
 
@@ -1261,7 +1291,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="72">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1269,6 +1299,368 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1363,372 +1755,10 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1861,74 +1891,92 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2294,7 +2342,7 @@
     <col min="1" max="1" width="13.3984375" customWidth="1"/>
     <col min="5" max="5" width="13.86328125" customWidth="1"/>
     <col min="6" max="6" width="10.265625" customWidth="1"/>
-    <col min="10" max="10" width="13.53125" customWidth="1"/>
+    <col min="10" max="10" width="13.59765625" customWidth="1"/>
     <col min="16" max="16" width="13.265625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="14.86328125" customWidth="1"/>
   </cols>
@@ -3477,43 +3525,43 @@
   </sheetData>
   <autoFilter ref="A1:AC16" xr:uid="{99B320C6-A597-4E1B-B5FD-F0989543660C}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC16">
-      <sortCondition sortBy="cellColor" ref="AC1:AC16" dxfId="69"/>
+      <sortCondition sortBy="cellColor" ref="AC1:AC16" dxfId="71"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="Q2:U16">
-    <cfRule type="cellIs" dxfId="58" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="17" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H16">
-    <cfRule type="cellIs" dxfId="57" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="69" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="13" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C16">
-    <cfRule type="cellIs" dxfId="55" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="9" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="10" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="12" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:N16">
-    <cfRule type="cellIs" dxfId="52" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="3" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:AC16">
-    <cfRule type="cellIs" dxfId="50" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="1" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3523,6 +3571,1129 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D61808F-2A1D-4F74-9E35-43CB27586058}">
+  <dimension ref="A1:Q19"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="14.3984375" customWidth="1"/>
+    <col min="6" max="6" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="D2">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="I2">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="J2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2">
+        <v>0.85199999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="I3">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="J3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="C4">
+        <v>-0.2</v>
+      </c>
+      <c r="D4">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>0.188</v>
+      </c>
+      <c r="H4">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="I4">
+        <v>-0.20300000000000001</v>
+      </c>
+      <c r="J4">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="L4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4">
+        <v>0.157</v>
+      </c>
+      <c r="O4">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="P4">
+        <v>0.151</v>
+      </c>
+      <c r="Q4">
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0.37</v>
+      </c>
+      <c r="C5">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="D5">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="H5">
+        <v>0.318</v>
+      </c>
+      <c r="J5">
+        <v>0.154</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="N5">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="O5">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="P5">
+        <v>0.155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>0.91</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>0.75</v>
+      </c>
+      <c r="I6">
+        <v>0.114</v>
+      </c>
+      <c r="J6">
+        <v>-0.217</v>
+      </c>
+      <c r="L6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6">
+        <v>0.74</v>
+      </c>
+      <c r="Q6">
+        <v>0.224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>0.109</v>
+      </c>
+      <c r="C7">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>0.85</v>
+      </c>
+      <c r="L7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7">
+        <v>0.82699999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="J8">
+        <v>0.105</v>
+      </c>
+      <c r="L8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8">
+        <v>0.83899999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="D9">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="L9" t="s">
+        <v>4</v>
+      </c>
+      <c r="M9">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="N9">
+        <v>-0.182</v>
+      </c>
+      <c r="O9">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="Q9">
+        <v>-0.16400000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.875</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="L10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="N10">
+        <v>0.158</v>
+      </c>
+      <c r="Q10">
+        <v>0.28199999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>0.36</v>
+      </c>
+      <c r="C11">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>0.106</v>
+      </c>
+      <c r="H11">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="I11">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="J11">
+        <v>-0.17899999999999999</v>
+      </c>
+      <c r="L11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N11">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="P11">
+        <v>-0.16700000000000001</v>
+      </c>
+      <c r="Q11">
+        <v>-0.26300000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="L12" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12">
+        <v>0.745</v>
+      </c>
+      <c r="P12">
+        <v>0.191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="I13">
+        <v>-0.24099999999999999</v>
+      </c>
+      <c r="J13">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="L13" t="s">
+        <v>12</v>
+      </c>
+      <c r="O13">
+        <v>0.90800000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="D14">
+        <v>-0.11799999999999999</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="I14">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="J14">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="L14" t="s">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <v>0.504</v>
+      </c>
+      <c r="P14">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="Q14">
+        <v>-0.378</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>18</v>
+      </c>
+      <c r="M16" t="s">
+        <v>0</v>
+      </c>
+      <c r="N16" t="s">
+        <v>17</v>
+      </c>
+      <c r="O16" t="s">
+        <v>18</v>
+      </c>
+      <c r="P16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>2.734</v>
+      </c>
+      <c r="C17">
+        <v>2.6259999999999999</v>
+      </c>
+      <c r="D17">
+        <v>1.367</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17">
+        <v>2.6680000000000001</v>
+      </c>
+      <c r="H17">
+        <v>2.5009999999999999</v>
+      </c>
+      <c r="I17">
+        <v>1.095</v>
+      </c>
+      <c r="J17">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="L17" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17">
+        <v>2.5289999999999999</v>
+      </c>
+      <c r="N17">
+        <v>1.9890000000000001</v>
+      </c>
+      <c r="O17">
+        <v>1.3540000000000001</v>
+      </c>
+      <c r="P17">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="Q17">
+        <v>0.58499999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>0.21</v>
+      </c>
+      <c r="C18">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="D18">
+        <v>0.105</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="H18">
+        <v>0.192</v>
+      </c>
+      <c r="I18">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="J18">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="L18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M18">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="N18">
+        <v>0.153</v>
+      </c>
+      <c r="O18">
+        <v>0.104</v>
+      </c>
+      <c r="P18">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="Q18">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>0.21</v>
+      </c>
+      <c r="C19">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="D19">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="H19">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="I19">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="J19">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="L19" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="N19">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="O19">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="P19">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="Q19">
+        <v>0.58299999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:Q1" xr:uid="{85F09F99-28C1-4BB1-A75C-F2C0B1518057}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q14">
+      <sortCondition sortBy="cellColor" ref="D1" dxfId="22"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="M2:Q14">
+    <cfRule type="cellIs" dxfId="21" priority="6" operator="lessThan">
+      <formula>-0.299</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:D14">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="4" operator="greaterThan">
+      <formula>0.399</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:J14">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="greaterThan">
+      <formula>0.399</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8727E6E-4063-4F85-BAE5-AB6F095D427F}">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.59765625" customWidth="1"/>
+    <col min="7" max="7" width="15.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>-0.01</v>
+      </c>
+      <c r="C2">
+        <v>0.08</v>
+      </c>
+      <c r="D2">
+        <v>0.27</v>
+      </c>
+      <c r="E2">
+        <v>0.37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>-0.03</v>
+      </c>
+      <c r="I2">
+        <v>0.05</v>
+      </c>
+      <c r="J2">
+        <v>0.25</v>
+      </c>
+      <c r="K2">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>0.12</v>
+      </c>
+      <c r="C3">
+        <v>0.05</v>
+      </c>
+      <c r="D3">
+        <v>-0.03</v>
+      </c>
+      <c r="E3">
+        <v>0.44</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3">
+        <v>0.06</v>
+      </c>
+      <c r="I3">
+        <v>0.01</v>
+      </c>
+      <c r="J3">
+        <v>-0.05</v>
+      </c>
+      <c r="K3">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0.11</v>
+      </c>
+      <c r="C4">
+        <v>-0.1</v>
+      </c>
+      <c r="D4">
+        <v>0.36</v>
+      </c>
+      <c r="E4">
+        <v>-0.06</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>0.11</v>
+      </c>
+      <c r="I4">
+        <v>-0.08</v>
+      </c>
+      <c r="J4">
+        <v>0.33</v>
+      </c>
+      <c r="K4">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>0.01</v>
+      </c>
+      <c r="C5">
+        <v>0.02</v>
+      </c>
+      <c r="D5">
+        <v>0.7</v>
+      </c>
+      <c r="E5">
+        <v>0.01</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>0.01</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0.75</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.25</v>
+      </c>
+      <c r="C6">
+        <v>0.37</v>
+      </c>
+      <c r="D6">
+        <v>0.06</v>
+      </c>
+      <c r="E6">
+        <v>-0.09</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <v>-0.01</v>
+      </c>
+      <c r="I6">
+        <v>0.81</v>
+      </c>
+      <c r="J6">
+        <v>-0.01</v>
+      </c>
+      <c r="K6">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>-0.02</v>
+      </c>
+      <c r="C7">
+        <v>0.71</v>
+      </c>
+      <c r="D7">
+        <v>-0.03</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I7">
+        <v>0.37</v>
+      </c>
+      <c r="J7">
+        <v>0.13</v>
+      </c>
+      <c r="K7">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.47</v>
+      </c>
+      <c r="D8">
+        <v>0.11</v>
+      </c>
+      <c r="E8">
+        <v>0.13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>0.33</v>
+      </c>
+      <c r="I8">
+        <v>0.04</v>
+      </c>
+      <c r="J8">
+        <v>0.02</v>
+      </c>
+      <c r="K8">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>0.31</v>
+      </c>
+      <c r="C9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.03</v>
+      </c>
+      <c r="E9">
+        <v>-0.12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>0.3</v>
+      </c>
+      <c r="I9">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K9">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>0.63</v>
+      </c>
+      <c r="C10">
+        <v>0.04</v>
+      </c>
+      <c r="D10">
+        <v>0.03</v>
+      </c>
+      <c r="E10">
+        <v>0.02</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>0.65</v>
+      </c>
+      <c r="I10">
+        <v>0.02</v>
+      </c>
+      <c r="J10">
+        <v>0.02</v>
+      </c>
+      <c r="K10">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0.36</v>
+      </c>
+      <c r="C11">
+        <v>0.03</v>
+      </c>
+      <c r="D11">
+        <v>-0.08</v>
+      </c>
+      <c r="E11">
+        <v>0.21</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <v>0.33</v>
+      </c>
+      <c r="I11">
+        <v>0.03</v>
+      </c>
+      <c r="J11">
+        <v>-0.08</v>
+      </c>
+      <c r="K11">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>0.63</v>
+      </c>
+      <c r="C12">
+        <v>-0.03</v>
+      </c>
+      <c r="D12">
+        <v>0.01</v>
+      </c>
+      <c r="E12">
+        <v>0.01</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <v>0.63</v>
+      </c>
+      <c r="I12">
+        <v>-0.03</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>0.04</v>
+      </c>
+      <c r="C13">
+        <v>0.26</v>
+      </c>
+      <c r="D13">
+        <v>0.04</v>
+      </c>
+      <c r="E13">
+        <v>-0.02</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>0.05</v>
+      </c>
+      <c r="C14">
+        <v>0.24</v>
+      </c>
+      <c r="D14">
+        <v>0.04</v>
+      </c>
+      <c r="E14">
+        <v>-0.09</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F14" xr:uid="{F6EC43A2-0E96-4311-A986-12EE04542C46}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
+      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="15"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="B1:E1048576">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:K1">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:K12">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThan">
+      <formula>0.299</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498CC891-573B-427D-8528-B6E57CC0DFD4}">
   <dimension ref="A1:O29"/>
   <sheetViews>
@@ -3532,10 +4703,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.265625" customWidth="1"/>
     <col min="5" max="5" width="12.86328125" customWidth="1"/>
-    <col min="9" max="9" width="13.53125" customWidth="1"/>
-    <col min="13" max="13" width="13.06640625" customWidth="1"/>
+    <col min="9" max="9" width="13.59765625" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.45">
@@ -4140,31 +5311,31 @@
   </sheetData>
   <autoFilter ref="A16:C29" xr:uid="{498CC891-573B-427D-8528-B6E57CC0DFD4}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:C29">
-      <sortCondition sortBy="cellColor" ref="C16:C29" dxfId="61"/>
+      <sortCondition sortBy="cellColor" ref="C16:C29" dxfId="11"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:C14">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G14">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:K14">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:O14">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C29">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4173,7 +5344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC6BCC2-AE82-430A-9446-637AC6346772}">
   <dimension ref="A1:E29"/>
   <sheetViews>
@@ -4181,7 +5352,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.9296875" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
     <col min="7" max="7" width="15.59765625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4592,16 +5763,16 @@
   </sheetData>
   <autoFilter ref="A1:K1" xr:uid="{2A2FF23C-A49F-4BBF-A172-E01688A2AD61}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K14">
-      <sortCondition sortBy="cellColor" ref="E1" dxfId="60"/>
+      <sortCondition sortBy="cellColor" ref="E1" dxfId="5"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E14">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:E29">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4610,7 +5781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C8C1A-CFC6-49AC-B896-635D55B44BA8}">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -4860,7 +6031,7 @@
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{76B16ADE-8397-4523-89E6-FD43024CAE02}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J14">
-      <sortCondition sortBy="cellColor" ref="J1" dxfId="59"/>
+      <sortCondition sortBy="cellColor" ref="J1" dxfId="2"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:D14">
@@ -4890,7 +6061,7 @@
   <cols>
     <col min="1" max="1" width="15.59765625" customWidth="1"/>
     <col min="2" max="2" width="10.265625" customWidth="1"/>
-    <col min="8" max="9" width="13.19921875" customWidth="1"/>
+    <col min="8" max="9" width="13.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.45">
@@ -6606,58 +7777,58 @@
   </sheetData>
   <autoFilter ref="H51:M65" xr:uid="{F695CD81-3D97-4E1C-8866-BD773BF04255}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H52:M65">
-      <sortCondition sortBy="cellColor" ref="L51:L65" dxfId="68"/>
+      <sortCondition sortBy="cellColor" ref="L51:L65" dxfId="61"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:G15">
-    <cfRule type="cellIs" dxfId="49" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="12" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:O15">
-    <cfRule type="cellIs" dxfId="48" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="11" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:G32">
-    <cfRule type="cellIs" dxfId="47" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="10" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:O32">
-    <cfRule type="cellIs" dxfId="46" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="9" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:F49">
-    <cfRule type="cellIs" dxfId="45" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="8" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:M49">
-    <cfRule type="cellIs" dxfId="44" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="7" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:F65">
-    <cfRule type="cellIs" dxfId="43" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="6" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I52:M65">
-    <cfRule type="cellIs" dxfId="42" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="1" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="2" operator="greaterThan">
       <formula>0.35</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="3" operator="greaterThan">
       <formula>0.39</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="4" operator="greaterThan">
       <formula>0.395</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="5" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8139,46 +9310,46 @@
   </sheetData>
   <autoFilter ref="H46:L59" xr:uid="{26C42105-EFDA-4FA3-8AB1-E5E42D4D4CA4}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H47:L59">
-      <sortCondition sortBy="cellColor" ref="L46:L59" dxfId="67"/>
+      <sortCondition sortBy="cellColor" ref="L46:L59" dxfId="48"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:F14">
-    <cfRule type="cellIs" dxfId="37" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="8" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:M14">
-    <cfRule type="cellIs" dxfId="36" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="7" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:F29">
-    <cfRule type="cellIs" dxfId="35" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="6" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:M29">
-    <cfRule type="cellIs" dxfId="34" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="5" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:E44">
-    <cfRule type="cellIs" dxfId="33" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="4" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32:L44">
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="3" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:E59">
-    <cfRule type="cellIs" dxfId="31" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="2" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47:L59">
-    <cfRule type="cellIs" dxfId="30" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="1" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8191,16 +9362,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984B0D20-5E48-4763-A83B-7B371039BA3E}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.06640625" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="17.1328125" customWidth="1"/>
-    <col min="3" max="3" width="16.19921875" customWidth="1"/>
-    <col min="4" max="4" width="29.19921875" customWidth="1"/>
+    <col min="3" max="3" width="16.1328125" customWidth="1"/>
+    <col min="4" max="4" width="29.1328125" customWidth="1"/>
     <col min="5" max="5" width="21.1328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8384,7 +9555,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:E14">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="1" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8394,6 +9565,498 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87DCAE64-8530-4592-A838-A6CB5F75441C}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="15.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>0.52</v>
+      </c>
+      <c r="C2">
+        <v>0.26</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0.68</v>
+      </c>
+      <c r="C3">
+        <v>0.2</v>
+      </c>
+      <c r="D3">
+        <v>-0.37</v>
+      </c>
+      <c r="E3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>0.93</v>
+      </c>
+      <c r="C4">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="D4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E4">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>0.95</v>
+      </c>
+      <c r="C5">
+        <v>-0.1</v>
+      </c>
+      <c r="D5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E5">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>0.52</v>
+      </c>
+      <c r="C6">
+        <v>-0.03</v>
+      </c>
+      <c r="D6">
+        <v>0.3</v>
+      </c>
+      <c r="E6">
+        <v>-0.21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>0.21</v>
+      </c>
+      <c r="C7">
+        <v>0.67</v>
+      </c>
+      <c r="D7">
+        <v>-0.27</v>
+      </c>
+      <c r="E7">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.06</v>
+      </c>
+      <c r="C8">
+        <v>0.7</v>
+      </c>
+      <c r="D8">
+        <v>0.22</v>
+      </c>
+      <c r="E8">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>-0.04</v>
+      </c>
+      <c r="C9">
+        <v>0.66</v>
+      </c>
+      <c r="D9">
+        <v>0.32</v>
+      </c>
+      <c r="E9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>0.06</v>
+      </c>
+      <c r="C10">
+        <v>-0.21</v>
+      </c>
+      <c r="D10">
+        <v>0.64</v>
+      </c>
+      <c r="E10">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>-0.01</v>
+      </c>
+      <c r="C11">
+        <v>0.4</v>
+      </c>
+      <c r="D11">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E11">
+        <v>-0.18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>0.1</v>
+      </c>
+      <c r="C12">
+        <v>0.09</v>
+      </c>
+      <c r="D12">
+        <v>0.52</v>
+      </c>
+      <c r="E12">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>-0.17</v>
+      </c>
+      <c r="C13">
+        <v>0.25</v>
+      </c>
+      <c r="D13">
+        <v>-0.05</v>
+      </c>
+      <c r="E13">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0.06</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0.13</v>
+      </c>
+      <c r="E14">
+        <v>0.79</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E14" xr:uid="{87DCAE64-8530-4592-A838-A6CB5F75441C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E14">
+      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="38"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="B2:E14">
+    <cfRule type="cellIs" dxfId="37" priority="1" operator="greaterThan">
+      <formula>0.499</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D6D6342-FAB0-45B3-B96B-783C62CCE1DB}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3">
+        <v>0.61</v>
+      </c>
+      <c r="C3">
+        <v>0.75</v>
+      </c>
+      <c r="D3">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C4">
+        <v>0.88</v>
+      </c>
+      <c r="D4">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5">
+        <v>0.89</v>
+      </c>
+      <c r="C5">
+        <v>0.77</v>
+      </c>
+      <c r="D5">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6">
+        <v>0.89</v>
+      </c>
+      <c r="C6">
+        <v>0.89</v>
+      </c>
+      <c r="D6">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C7">
+        <v>0.68</v>
+      </c>
+      <c r="D7">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9">
+        <v>0.89</v>
+      </c>
+      <c r="C9">
+        <v>0.91</v>
+      </c>
+      <c r="D9">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10">
+        <v>0.9</v>
+      </c>
+      <c r="C10">
+        <v>0.91</v>
+      </c>
+      <c r="D10">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11">
+        <v>0.67</v>
+      </c>
+      <c r="C11">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D11">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13">
+        <v>0.71</v>
+      </c>
+      <c r="C13">
+        <v>0.74</v>
+      </c>
+      <c r="D13">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14">
+        <v>0.71</v>
+      </c>
+      <c r="C14">
+        <v>0.68</v>
+      </c>
+      <c r="D14">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15">
+        <v>0.6</v>
+      </c>
+      <c r="C15">
+        <v>0.42</v>
+      </c>
+      <c r="D15">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0.94</v>
+      </c>
+      <c r="D17">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18">
+        <v>0.51</v>
+      </c>
+      <c r="C18">
+        <v>0.52</v>
+      </c>
+      <c r="D18">
+        <v>0.53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DF5018-9911-4233-8E1E-CFEBD8577F16}">
   <dimension ref="A1:W27"/>
   <sheetViews>
@@ -8405,8 +10068,8 @@
   <cols>
     <col min="1" max="1" width="13.86328125" customWidth="1"/>
     <col min="6" max="6" width="13.265625" customWidth="1"/>
-    <col min="7" max="7" width="12.06640625" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="11" max="11" width="15.265625" customWidth="1"/>
     <col min="13" max="13" width="12.59765625" customWidth="1"/>
     <col min="16" max="16" width="14.265625" customWidth="1"/>
     <col min="19" max="19" width="14.59765625" customWidth="1"/>
@@ -9532,47 +11195,47 @@
   </sheetData>
   <autoFilter ref="A15:E27" xr:uid="{00DF5018-9911-4233-8E1E-CFEBD8577F16}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:E27">
-      <sortCondition sortBy="cellColor" ref="E15:E27" dxfId="66"/>
+      <sortCondition sortBy="cellColor" ref="E15:E27" dxfId="36"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B2:D13">
-    <cfRule type="cellIs" dxfId="28" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="8" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:I13">
-    <cfRule type="cellIs" dxfId="27" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:N13">
-    <cfRule type="cellIs" dxfId="26" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="6" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:S13">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="5" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:E27">
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:K27">
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16:Q27">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16:W27">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9581,7 +11244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5509DC-DB05-43E6-A45B-32E76BC27DEA}">
   <dimension ref="A1:K23"/>
   <sheetViews>
@@ -9590,7 +11253,7 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="7" max="7" width="13.19921875" customWidth="1"/>
+    <col min="7" max="7" width="13.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
@@ -10192,16 +11855,16 @@
   </sheetData>
   <autoFilter ref="H1:K16" xr:uid="{8B5509DC-DB05-43E6-A45B-32E76BC27DEA}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:K16">
-      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="65"/>
+      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="27"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K16">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10210,7 +11873,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4883B1BD-E07A-48BB-9F66-A8C7003F2BEF}">
   <dimension ref="A1:E16"/>
   <sheetViews>
@@ -10220,7 +11883,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.46484375" customWidth="1"/>
+    <col min="1" max="1" width="13.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
@@ -10495,1138 +12158,15 @@
   </sheetData>
   <autoFilter ref="B1:E16" xr:uid="{4883B1BD-E07A-48BB-9F66-A8C7003F2BEF}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E16">
-      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="64"/>
+      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="24"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
       <formula>0.699</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D61808F-2A1D-4F74-9E35-43CB27586058}">
-  <dimension ref="A1:Q19"/>
-  <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="14.3984375" customWidth="1"/>
-    <col min="6" max="6" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>0.26500000000000001</v>
-      </c>
-      <c r="D2">
-        <v>0.41599999999999998</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>0.55500000000000005</v>
-      </c>
-      <c r="I2">
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="J2">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="L2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2">
-        <v>0.85199999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="I3">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="J3">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="L3" t="s">
-        <v>3</v>
-      </c>
-      <c r="P3">
-        <v>0.98199999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="C4">
-        <v>-0.2</v>
-      </c>
-      <c r="D4">
-        <v>0.53200000000000003</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>0.188</v>
-      </c>
-      <c r="H4">
-        <v>0.49099999999999999</v>
-      </c>
-      <c r="I4">
-        <v>-0.20300000000000001</v>
-      </c>
-      <c r="J4">
-        <v>0.29099999999999998</v>
-      </c>
-      <c r="L4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4">
-        <v>0.157</v>
-      </c>
-      <c r="O4">
-        <v>0.42699999999999999</v>
-      </c>
-      <c r="P4">
-        <v>0.151</v>
-      </c>
-      <c r="Q4">
-        <v>0.44500000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>0.37</v>
-      </c>
-      <c r="C5">
-        <v>0.48399999999999999</v>
-      </c>
-      <c r="D5">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5">
-        <v>0.51400000000000001</v>
-      </c>
-      <c r="H5">
-        <v>0.318</v>
-      </c>
-      <c r="J5">
-        <v>0.154</v>
-      </c>
-      <c r="K5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" t="s">
-        <v>5</v>
-      </c>
-      <c r="M5">
-        <v>0.34499999999999997</v>
-      </c>
-      <c r="N5">
-        <v>0.41099999999999998</v>
-      </c>
-      <c r="O5">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="P5">
-        <v>0.155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>0.91</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>0.75</v>
-      </c>
-      <c r="I6">
-        <v>0.114</v>
-      </c>
-      <c r="J6">
-        <v>-0.217</v>
-      </c>
-      <c r="L6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M6">
-        <v>0.74</v>
-      </c>
-      <c r="Q6">
-        <v>0.224</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>0.109</v>
-      </c>
-      <c r="C7">
-        <v>0.48699999999999999</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7">
-        <v>0.85</v>
-      </c>
-      <c r="L7" t="s">
-        <v>7</v>
-      </c>
-      <c r="M7">
-        <v>0.82699999999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>0.90500000000000003</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8">
-        <v>0.82099999999999995</v>
-      </c>
-      <c r="J8">
-        <v>0.105</v>
-      </c>
-      <c r="L8" t="s">
-        <v>9</v>
-      </c>
-      <c r="M8">
-        <v>0.83899999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>0.58199999999999996</v>
-      </c>
-      <c r="D9">
-        <v>0.13100000000000001</v>
-      </c>
-      <c r="F9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="L9" t="s">
-        <v>4</v>
-      </c>
-      <c r="M9">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="N9">
-        <v>-0.182</v>
-      </c>
-      <c r="O9">
-        <v>0.53600000000000003</v>
-      </c>
-      <c r="Q9">
-        <v>-0.16400000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>0.875</v>
-      </c>
-      <c r="F10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10">
-        <v>0.91900000000000004</v>
-      </c>
-      <c r="L10" t="s">
-        <v>15</v>
-      </c>
-      <c r="M10">
-        <v>0.41499999999999998</v>
-      </c>
-      <c r="N10">
-        <v>0.158</v>
-      </c>
-      <c r="Q10">
-        <v>0.28199999999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>0.36</v>
-      </c>
-      <c r="C11">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="F11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11">
-        <v>0.106</v>
-      </c>
-      <c r="H11">
-        <v>0.39700000000000002</v>
-      </c>
-      <c r="I11">
-        <v>0.27300000000000002</v>
-      </c>
-      <c r="J11">
-        <v>-0.17899999999999999</v>
-      </c>
-      <c r="L11" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="P11">
-        <v>-0.16700000000000001</v>
-      </c>
-      <c r="Q11">
-        <v>-0.26300000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>0.89200000000000002</v>
-      </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12">
-        <v>0.89400000000000002</v>
-      </c>
-      <c r="L12" t="s">
-        <v>14</v>
-      </c>
-      <c r="N12">
-        <v>0.745</v>
-      </c>
-      <c r="P12">
-        <v>0.191</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13">
-        <v>0.58499999999999996</v>
-      </c>
-      <c r="F13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13">
-        <v>0.59699999999999998</v>
-      </c>
-      <c r="I13">
-        <v>-0.24099999999999999</v>
-      </c>
-      <c r="J13">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="L13" t="s">
-        <v>12</v>
-      </c>
-      <c r="O13">
-        <v>0.90800000000000003</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14">
-        <v>0.70799999999999996</v>
-      </c>
-      <c r="D14">
-        <v>-0.11799999999999999</v>
-      </c>
-      <c r="F14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="I14">
-        <v>0.33900000000000002</v>
-      </c>
-      <c r="J14">
-        <v>0.50700000000000001</v>
-      </c>
-      <c r="L14" t="s">
-        <v>2</v>
-      </c>
-      <c r="M14">
-        <v>0.504</v>
-      </c>
-      <c r="P14">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="Q14">
-        <v>-0.378</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>0</v>
-      </c>
-      <c r="G16" t="s">
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" t="s">
-        <v>0</v>
-      </c>
-      <c r="J16" t="s">
-        <v>18</v>
-      </c>
-      <c r="M16" t="s">
-        <v>0</v>
-      </c>
-      <c r="N16" t="s">
-        <v>17</v>
-      </c>
-      <c r="O16" t="s">
-        <v>18</v>
-      </c>
-      <c r="P16" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17">
-        <v>2.734</v>
-      </c>
-      <c r="C17">
-        <v>2.6259999999999999</v>
-      </c>
-      <c r="D17">
-        <v>1.367</v>
-      </c>
-      <c r="F17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17">
-        <v>2.6680000000000001</v>
-      </c>
-      <c r="H17">
-        <v>2.5009999999999999</v>
-      </c>
-      <c r="I17">
-        <v>1.095</v>
-      </c>
-      <c r="J17">
-        <v>0.84399999999999997</v>
-      </c>
-      <c r="L17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17">
-        <v>2.5289999999999999</v>
-      </c>
-      <c r="N17">
-        <v>1.9890000000000001</v>
-      </c>
-      <c r="O17">
-        <v>1.3540000000000001</v>
-      </c>
-      <c r="P17">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="Q17">
-        <v>0.58499999999999996</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18">
-        <v>0.21</v>
-      </c>
-      <c r="C18">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="D18">
-        <v>0.105</v>
-      </c>
-      <c r="F18" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="H18">
-        <v>0.192</v>
-      </c>
-      <c r="I18">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="J18">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="L18" t="s">
-        <v>23</v>
-      </c>
-      <c r="M18">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="N18">
-        <v>0.153</v>
-      </c>
-      <c r="O18">
-        <v>0.104</v>
-      </c>
-      <c r="P18">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="Q18">
-        <v>4.4999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19">
-        <v>0.21</v>
-      </c>
-      <c r="C19">
-        <v>0.41199999999999998</v>
-      </c>
-      <c r="D19">
-        <v>0.51700000000000002</v>
-      </c>
-      <c r="F19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="H19">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="I19">
-        <v>0.48199999999999998</v>
-      </c>
-      <c r="J19">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="L19" t="s">
-        <v>24</v>
-      </c>
-      <c r="M19">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="N19">
-        <v>0.34799999999999998</v>
-      </c>
-      <c r="O19">
-        <v>0.45200000000000001</v>
-      </c>
-      <c r="P19">
-        <v>0.53800000000000003</v>
-      </c>
-      <c r="Q19">
-        <v>0.58299999999999996</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:Q1" xr:uid="{85F09F99-28C1-4BB1-A75C-F2C0B1518057}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q14">
-      <sortCondition sortBy="cellColor" ref="D1" dxfId="63"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="M2:Q14">
-    <cfRule type="cellIs" dxfId="17" priority="6" operator="lessThan">
-      <formula>-0.299</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="7" operator="greaterThan">
-      <formula>0.299</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
-      <formula>0.299</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="greaterThan">
-      <formula>0.399</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
-      <formula>0.299</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
-      <formula>0.399</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8727E6E-4063-4F85-BAE5-AB6F095D427F}">
-  <dimension ref="A1:K14"/>
-  <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="13.59765625" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>-0.01</v>
-      </c>
-      <c r="C2">
-        <v>0.08</v>
-      </c>
-      <c r="D2">
-        <v>0.27</v>
-      </c>
-      <c r="E2">
-        <v>0.37</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2">
-        <v>-0.03</v>
-      </c>
-      <c r="I2">
-        <v>0.05</v>
-      </c>
-      <c r="J2">
-        <v>0.25</v>
-      </c>
-      <c r="K2">
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3">
-        <v>0.12</v>
-      </c>
-      <c r="C3">
-        <v>0.05</v>
-      </c>
-      <c r="D3">
-        <v>-0.03</v>
-      </c>
-      <c r="E3">
-        <v>0.44</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3">
-        <v>0.06</v>
-      </c>
-      <c r="I3">
-        <v>0.01</v>
-      </c>
-      <c r="J3">
-        <v>-0.05</v>
-      </c>
-      <c r="K3">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>0.11</v>
-      </c>
-      <c r="C4">
-        <v>-0.1</v>
-      </c>
-      <c r="D4">
-        <v>0.36</v>
-      </c>
-      <c r="E4">
-        <v>-0.06</v>
-      </c>
-      <c r="G4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <v>0.11</v>
-      </c>
-      <c r="I4">
-        <v>-0.08</v>
-      </c>
-      <c r="J4">
-        <v>0.33</v>
-      </c>
-      <c r="K4">
-        <v>-0.05</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>0.01</v>
-      </c>
-      <c r="C5">
-        <v>0.02</v>
-      </c>
-      <c r="D5">
-        <v>0.7</v>
-      </c>
-      <c r="E5">
-        <v>0.01</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5">
-        <v>0.01</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0.75</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>0.25</v>
-      </c>
-      <c r="C6">
-        <v>0.37</v>
-      </c>
-      <c r="D6">
-        <v>0.06</v>
-      </c>
-      <c r="E6">
-        <v>-0.09</v>
-      </c>
-      <c r="G6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6">
-        <v>-0.01</v>
-      </c>
-      <c r="I6">
-        <v>0.81</v>
-      </c>
-      <c r="J6">
-        <v>-0.01</v>
-      </c>
-      <c r="K6">
-        <v>-0.01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>-0.02</v>
-      </c>
-      <c r="C7">
-        <v>0.71</v>
-      </c>
-      <c r="D7">
-        <v>-0.03</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="I7">
-        <v>0.37</v>
-      </c>
-      <c r="J7">
-        <v>0.13</v>
-      </c>
-      <c r="K7">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <v>0.02</v>
-      </c>
-      <c r="C8">
-        <v>0.47</v>
-      </c>
-      <c r="D8">
-        <v>0.11</v>
-      </c>
-      <c r="E8">
-        <v>0.13</v>
-      </c>
-      <c r="G8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8">
-        <v>0.33</v>
-      </c>
-      <c r="I8">
-        <v>0.04</v>
-      </c>
-      <c r="J8">
-        <v>0.02</v>
-      </c>
-      <c r="K8">
-        <v>-0.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>0.31</v>
-      </c>
-      <c r="C9">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D9">
-        <v>0.03</v>
-      </c>
-      <c r="E9">
-        <v>-0.12</v>
-      </c>
-      <c r="G9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9">
-        <v>0.3</v>
-      </c>
-      <c r="I9">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="J9">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="K9">
-        <v>-0.04</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>0.63</v>
-      </c>
-      <c r="C10">
-        <v>0.04</v>
-      </c>
-      <c r="D10">
-        <v>0.03</v>
-      </c>
-      <c r="E10">
-        <v>0.02</v>
-      </c>
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10">
-        <v>0.65</v>
-      </c>
-      <c r="I10">
-        <v>0.02</v>
-      </c>
-      <c r="J10">
-        <v>0.02</v>
-      </c>
-      <c r="K10">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>0.36</v>
-      </c>
-      <c r="C11">
-        <v>0.03</v>
-      </c>
-      <c r="D11">
-        <v>-0.08</v>
-      </c>
-      <c r="E11">
-        <v>0.21</v>
-      </c>
-      <c r="G11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11">
-        <v>0.33</v>
-      </c>
-      <c r="I11">
-        <v>0.03</v>
-      </c>
-      <c r="J11">
-        <v>-0.08</v>
-      </c>
-      <c r="K11">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>0.63</v>
-      </c>
-      <c r="C12">
-        <v>-0.03</v>
-      </c>
-      <c r="D12">
-        <v>0.01</v>
-      </c>
-      <c r="E12">
-        <v>0.01</v>
-      </c>
-      <c r="G12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12">
-        <v>0.63</v>
-      </c>
-      <c r="I12">
-        <v>-0.03</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13">
-        <v>0.04</v>
-      </c>
-      <c r="C13">
-        <v>0.26</v>
-      </c>
-      <c r="D13">
-        <v>0.04</v>
-      </c>
-      <c r="E13">
-        <v>-0.02</v>
-      </c>
-      <c r="F13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>0.05</v>
-      </c>
-      <c r="C14">
-        <v>0.24</v>
-      </c>
-      <c r="D14">
-        <v>0.04</v>
-      </c>
-      <c r="E14">
-        <v>-0.09</v>
-      </c>
-      <c r="F14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:F14" xr:uid="{F6EC43A2-0E96-4311-A986-12EE04542C46}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
-      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="62"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="B1:E1048576">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
-      <formula>0.299</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:K1">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
-      <formula>0.299</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:K12">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
-      <formula>0.299</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Merged panel data for LTA
And other stuff.. haven't saved in awhile
</commit_message>
<xml_diff>
--- a/R/Factor analysis  - factor loadings.xlsx
+++ b/R/Factor analysis  - factor loadings.xlsx
@@ -1,46 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\git\AHL\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45970B3F-DACE-4E45-9B15-C7B1414355CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9098BF8C-1A77-40FE-8543-A4D10A9EC66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" firstSheet="1" activeTab="5" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="4" xr2:uid="{1DD09E13-5243-4F1E-B7D4-320B301DF208}"/>
   </bookViews>
   <sheets>
     <sheet name="All CAMs" sheetId="1" r:id="rId1"/>
     <sheet name="Combine Pray and Spirit" sheetId="12" r:id="rId2"/>
-    <sheet name="Comb Pray Spirit Drop Bio" sheetId="13" r:id="rId3"/>
-    <sheet name="Final EFA" sheetId="14" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="15" r:id="rId5"/>
-    <sheet name="CFA std loadings" sheetId="16" r:id="rId6"/>
-    <sheet name="Drop energy, pray, spirit" sheetId="10" r:id="rId7"/>
-    <sheet name="Principal Axis Factoring" sheetId="9" r:id="rId8"/>
-    <sheet name="PCA" sheetId="8" r:id="rId9"/>
-    <sheet name="Drop prayer and spirit" sheetId="2" state="hidden" r:id="rId10"/>
-    <sheet name="Mysterious Perfect Model" sheetId="3" r:id="rId11"/>
-    <sheet name="Ex Pray Spirit Comparisons" sheetId="11" r:id="rId12"/>
-    <sheet name="Comparing MPM" sheetId="6" r:id="rId13"/>
-    <sheet name="Numeric" sheetId="5" r:id="rId14"/>
+    <sheet name="Sheet2" sheetId="17" r:id="rId3"/>
+    <sheet name="Comb Pray Spirit Drop Bio" sheetId="13" r:id="rId4"/>
+    <sheet name="Final EFA" sheetId="14" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId6"/>
+    <sheet name="CFA std loadings" sheetId="16" r:id="rId7"/>
+    <sheet name="Drop energy, pray, spirit" sheetId="10" r:id="rId8"/>
+    <sheet name="Principal Axis Factoring" sheetId="9" r:id="rId9"/>
+    <sheet name="PCA" sheetId="8" r:id="rId10"/>
+    <sheet name="Drop prayer and spirit" sheetId="2" state="hidden" r:id="rId11"/>
+    <sheet name="Mysterious Perfect Model" sheetId="3" r:id="rId12"/>
+    <sheet name="Ex Pray Spirit Comparisons" sheetId="11" r:id="rId13"/>
+    <sheet name="Comparing MPM" sheetId="6" r:id="rId14"/>
+    <sheet name="Numeric" sheetId="5" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All CAMs'!$A$1:$AC$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Comb Pray Spirit Drop Bio'!$H$46:$L$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Comb Pray Spirit Drop Bio'!$H$46:$L$59</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Combine Pray and Spirit'!$H$51:$M$65</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Comparing MPM'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Drop energy, pray, spirit'!$A$15:$E$27</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Drop prayer and spirit'!$A$1:$Q$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Ex Pray Spirit Comparisons'!$A$16:$C$29</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Mysterious Perfect Model'!$A$1:$F$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">Numeric!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">PCA!$B$1:$E$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Principal Axis Factoring'!$H$1:$K$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet1!$A$1:$E$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'Comparing MPM'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Drop energy, pray, spirit'!$A$15:$E$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Drop prayer and spirit'!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Ex Pray Spirit Comparisons'!$A$16:$C$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Mysterious Perfect Model'!$A$1:$F$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Numeric!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">PCA!$B$1:$E$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Principal Axis Factoring'!$H$1:$K$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet1!$A$1:$E$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet2!$A$66:$E$79</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -274,6 +276,141 @@
     <author>hanna</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{BF07EF22-39DC-4119-8DF2-E0F29C3B0008}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Maximum likelihood, varimax rotation
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{FC0F7213-7285-4B2C-B961-AEEC5050BD1E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Maximum Likelihood, promax rotation
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{2510CC9D-8268-435A-8CB7-4E7BC12401C1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Maximum likelihood, oblimin rotation
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{5EA7F6F2-02E1-4A68-8922-3BBD5F6D467E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Maximum Likelihood, cluster rotation
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{E0824D5C-0A44-4F46-8A81-A476B5475001}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hanna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Principal Axis, varimax
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>hanna</author>
+  </authors>
+  <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{D5712E48-0578-4E7B-970F-9D684F744419}">
       <text>
         <r>
@@ -328,7 +465,7 @@
 </comments>
 </file>
 
-<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -364,6 +501,87 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={62140F1E-E015-4347-8CCB-0F6A2B60F321}</author>
+    <author>tc={1280B8E6-9065-4846-BB3B-846E86FE89C6}</author>
+    <author>tc={73416874-87C4-4DFB-9577-EA58B86D3239}</author>
+    <author>tc={AB8C3CC9-E867-4720-B57C-DA6CD63F12C3}</author>
+    <author>tc={04C3A851-58E3-4C88-A504-E6D4A6DC7F89}</author>
+    <author>tc={E4E30268-700A-40A4-BE94-C8A501AFE0C9}</author>
+    <author>tc={21726126-81A9-419D-8B18-99E0332C5D44}</author>
+    <author>tc={A7233670-12F4-4AC7-B8B8-DBA2FA7AD68F}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{62140F1E-E015-4347-8CCB-0F6A2B60F321}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    all 6 ml varimax</t>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{1280B8E6-9065-4846-BB3B-846E86FE89C6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    all 6 ml promax</t>
+      </text>
+    </comment>
+    <comment ref="A17" authorId="2" shapeId="0" xr:uid="{73416874-87C4-4DFB-9577-EA58B86D3239}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    all 6 ml cluster</t>
+      </text>
+    </comment>
+    <comment ref="I17" authorId="3" shapeId="0" xr:uid="{AB8C3CC9-E867-4720-B57C-DA6CD63F12C3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    all 6 ml oblimin</t>
+      </text>
+    </comment>
+    <comment ref="A33" authorId="4" shapeId="0" xr:uid="{04C3A851-58E3-4C88-A504-E6D4A6DC7F89}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    all 5 ml varimax</t>
+      </text>
+    </comment>
+    <comment ref="H33" authorId="5" shapeId="0" xr:uid="{E4E30268-700A-40A4-BE94-C8A501AFE0C9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    all 5 ml promax</t>
+      </text>
+    </comment>
+    <comment ref="A49" authorId="6" shapeId="0" xr:uid="{21726126-81A9-419D-8B18-99E0332C5D44}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    all 5 ml cluster</t>
+      </text>
+    </comment>
+    <comment ref="H49" authorId="7" shapeId="0" xr:uid="{A7233670-12F4-4AC7-B8B8-DBA2FA7AD68F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    all 5 ml oblimin</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -569,7 +787,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -603,7 +821,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={05F861C7-3F05-45BE-A842-A70399D00986}</author>
@@ -756,7 +974,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={68C2D0A8-62BB-4214-AD84-976C7BE3AB2B}</author>
@@ -774,7 +992,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={F7A5C9D5-E716-4F51-8BD8-AA873D1AD48D}</author>
@@ -792,7 +1010,7 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -827,7 +1045,7 @@
 </comments>
 </file>
 
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hanna</author>
@@ -887,143 +1105,8 @@
 </comments>
 </file>
 
-<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>hanna</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{BF07EF22-39DC-4119-8DF2-E0F29C3B0008}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>hanna:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Maximum likelihood, varimax rotation
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{FC0F7213-7285-4B2C-B961-AEEC5050BD1E}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>hanna:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Maximum Likelihood, promax rotation
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{2510CC9D-8268-435A-8CB7-4E7BC12401C1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>hanna:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Maximum likelihood, oblimin rotation
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{5EA7F6F2-02E1-4A68-8922-3BBD5F6D467E}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>hanna:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Maximum Likelihood, cluster rotation
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{E0824D5C-0A44-4F46-8A81-A476B5475001}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>hanna:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Principal Axis, varimax
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="69">
   <si>
     <t>ML2</t>
   </si>
@@ -1291,7 +1374,1073 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="72">
+  <dxfs count="194">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2304,6 +3453,35 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2021-09-27T18:45:37.55" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{62140F1E-E015-4347-8CCB-0F6A2B60F321}">
+    <text>all 6 ml varimax</text>
+  </threadedComment>
+  <threadedComment ref="I1" dT="2021-09-27T18:49:06.33" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{1280B8E6-9065-4846-BB3B-846E86FE89C6}">
+    <text>all 6 ml promax</text>
+  </threadedComment>
+  <threadedComment ref="A17" dT="2021-09-27T18:58:54.84" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{73416874-87C4-4DFB-9577-EA58B86D3239}">
+    <text>all 6 ml cluster</text>
+  </threadedComment>
+  <threadedComment ref="I17" dT="2021-09-27T19:00:25.74" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{AB8C3CC9-E867-4720-B57C-DA6CD63F12C3}">
+    <text>all 6 ml oblimin</text>
+  </threadedComment>
+  <threadedComment ref="A33" dT="2021-09-27T19:40:01.02" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{04C3A851-58E3-4C88-A504-E6D4A6DC7F89}">
+    <text>all 5 ml varimax</text>
+  </threadedComment>
+  <threadedComment ref="H33" dT="2021-09-27T19:41:15.34" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{E4E30268-700A-40A4-BE94-C8A501AFE0C9}">
+    <text>all 5 ml promax</text>
+  </threadedComment>
+  <threadedComment ref="A49" dT="2021-09-27T19:43:10.34" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{21726126-81A9-419D-8B18-99E0332C5D44}">
+    <text>all 5 ml cluster</text>
+  </threadedComment>
+  <threadedComment ref="H49" dT="2021-09-27T19:44:05.99" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{A7233670-12F4-4AC7-B8B8-DBA2FA7AD68F}">
+    <text>all 5 ml oblimin</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A1" dT="2021-06-12T19:29:21.77" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{05F861C7-3F05-45BE-A842-A70399D00986}">
     <text>Maximum likelihood, varimax</text>
   </threadedComment>
@@ -2313,7 +3491,7 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A1" dT="2021-06-09T21:16:27.69" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{68C2D0A8-62BB-4214-AD84-976C7BE3AB2B}">
     <text>All CAMs, principal axis factoring (pa) with promax rotation</text>
@@ -2321,7 +3499,7 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A1" dT="2021-06-09T18:37:26.45" personId="{A5CA6894-FBDA-4D6C-B5C3-EC266C72EF46}" id="{F7A5C9D5-E716-4F51-8BD8-AA873D1AD48D}">
     <text>Principal Components with Varimax Rotation</text>
@@ -3525,43 +4703,43 @@
   </sheetData>
   <autoFilter ref="A1:AC16" xr:uid="{99B320C6-A597-4E1B-B5FD-F0989543660C}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC16">
-      <sortCondition sortBy="cellColor" ref="AC1:AC16" dxfId="71"/>
+      <sortCondition sortBy="cellColor" ref="AC1:AC16" dxfId="193"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="Q2:U16">
-    <cfRule type="cellIs" dxfId="70" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="192" priority="17" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H16">
-    <cfRule type="cellIs" dxfId="69" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="191" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="190" priority="13" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C16">
-    <cfRule type="cellIs" dxfId="67" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="189" priority="9" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="188" priority="10" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="187" priority="12" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:N16">
-    <cfRule type="cellIs" dxfId="64" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="186" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="185" priority="3" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:AC16">
-    <cfRule type="cellIs" dxfId="62" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="184" priority="1" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3571,6 +4749,304 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4883B1BD-E07A-48BB-9F66-A8C7003F2BEF}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>0.21</v>
+      </c>
+      <c r="C2">
+        <v>0.62</v>
+      </c>
+      <c r="D2">
+        <v>0.31</v>
+      </c>
+      <c r="E2">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0.23</v>
+      </c>
+      <c r="C3">
+        <v>0.59</v>
+      </c>
+      <c r="D3">
+        <v>0.24</v>
+      </c>
+      <c r="E3">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0.63</v>
+      </c>
+      <c r="C4">
+        <v>0.12</v>
+      </c>
+      <c r="D4">
+        <v>-0.04</v>
+      </c>
+      <c r="E4">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0.12</v>
+      </c>
+      <c r="C5">
+        <v>0.3</v>
+      </c>
+      <c r="D5">
+        <v>0.22</v>
+      </c>
+      <c r="E5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0.2</v>
+      </c>
+      <c r="C6">
+        <v>0.05</v>
+      </c>
+      <c r="D6">
+        <v>0.27</v>
+      </c>
+      <c r="E6">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0.25</v>
+      </c>
+      <c r="C7">
+        <v>0.52</v>
+      </c>
+      <c r="D7">
+        <v>0.52</v>
+      </c>
+      <c r="E7">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0.66</v>
+      </c>
+      <c r="C8">
+        <v>0.26</v>
+      </c>
+      <c r="D8">
+        <v>0.51</v>
+      </c>
+      <c r="E8">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0.17</v>
+      </c>
+      <c r="C9">
+        <v>-0.04</v>
+      </c>
+      <c r="D9">
+        <v>0.78</v>
+      </c>
+      <c r="E9">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0.06</v>
+      </c>
+      <c r="C10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.81</v>
+      </c>
+      <c r="E10">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0.2</v>
+      </c>
+      <c r="C11">
+        <v>0.72</v>
+      </c>
+      <c r="D11">
+        <v>0.23</v>
+      </c>
+      <c r="E11">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0.11</v>
+      </c>
+      <c r="C12">
+        <v>0.71</v>
+      </c>
+      <c r="D12">
+        <v>-0.1</v>
+      </c>
+      <c r="E12">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0.49</v>
+      </c>
+      <c r="C13">
+        <v>0.54</v>
+      </c>
+      <c r="D13">
+        <v>0.04</v>
+      </c>
+      <c r="E13">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0.82</v>
+      </c>
+      <c r="C14">
+        <v>0.2</v>
+      </c>
+      <c r="D14">
+        <v>0.05</v>
+      </c>
+      <c r="E14">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>0.53</v>
+      </c>
+      <c r="C15">
+        <v>0.48</v>
+      </c>
+      <c r="D15">
+        <v>0.47</v>
+      </c>
+      <c r="E15">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>0.72</v>
+      </c>
+      <c r="C16">
+        <v>0.22</v>
+      </c>
+      <c r="D16">
+        <v>0.48</v>
+      </c>
+      <c r="E16">
+        <v>0.18</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E16" xr:uid="{4883B1BD-E07A-48BB-9F66-A8C7003F2BEF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E16">
+      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="146"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="B2:E16">
+    <cfRule type="cellIs" dxfId="145" priority="1" operator="greaterThan">
+      <formula>0.699</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D61808F-2A1D-4F74-9E35-43CB27586058}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
@@ -4203,30 +5679,30 @@
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{85F09F99-28C1-4BB1-A75C-F2C0B1518057}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q14">
-      <sortCondition sortBy="cellColor" ref="D1" dxfId="22"/>
+      <sortCondition sortBy="cellColor" ref="D1" dxfId="144"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="M2:Q14">
-    <cfRule type="cellIs" dxfId="21" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="143" priority="6" operator="lessThan">
       <formula>-0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="142" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="141" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="140" priority="4" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="139" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="138" priority="3" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4235,7 +5711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8727E6E-4063-4F85-BAE5-AB6F095D427F}">
   <dimension ref="A1:K14"/>
   <sheetViews>
@@ -4670,21 +6146,21 @@
   </sheetData>
   <autoFilter ref="A1:F14" xr:uid="{F6EC43A2-0E96-4311-A986-12EE04542C46}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
-      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="15"/>
+      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="137"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:E1048576">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="136" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:K1">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="135" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K12">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="134" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4693,7 +6169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498CC891-573B-427D-8528-B6E57CC0DFD4}">
   <dimension ref="A1:O29"/>
   <sheetViews>
@@ -5311,31 +6787,31 @@
   </sheetData>
   <autoFilter ref="A16:C29" xr:uid="{498CC891-573B-427D-8528-B6E57CC0DFD4}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:C29">
-      <sortCondition sortBy="cellColor" ref="C16:C29" dxfId="11"/>
+      <sortCondition sortBy="cellColor" ref="C16:C29" dxfId="133"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:C14">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="132" priority="5" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G14">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="131" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:K14">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="130" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:O14">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="129" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C29">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="128" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5344,7 +6820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC6BCC2-AE82-430A-9446-637AC6346772}">
   <dimension ref="A1:E29"/>
   <sheetViews>
@@ -5763,16 +7239,16 @@
   </sheetData>
   <autoFilter ref="A1:K1" xr:uid="{2A2FF23C-A49F-4BBF-A172-E01688A2AD61}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K14">
-      <sortCondition sortBy="cellColor" ref="E1" dxfId="5"/>
+      <sortCondition sortBy="cellColor" ref="E1" dxfId="127"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E14">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="126" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:E29">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="125" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5781,7 +7257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C8C1A-CFC6-49AC-B896-635D55B44BA8}">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -6031,16 +7507,16 @@
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{76B16ADE-8397-4523-89E6-FD43024CAE02}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J14">
-      <sortCondition sortBy="cellColor" ref="J1" dxfId="2"/>
+      <sortCondition sortBy="cellColor" ref="J1" dxfId="124"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:D14">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="123" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J14">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="122" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6053,7 +7529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F695CD81-3D97-4E1C-8866-BD773BF04255}">
   <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
@@ -7777,58 +9253,58 @@
   </sheetData>
   <autoFilter ref="H51:M65" xr:uid="{F695CD81-3D97-4E1C-8866-BD773BF04255}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H52:M65">
-      <sortCondition sortBy="cellColor" ref="L51:L65" dxfId="61"/>
+      <sortCondition sortBy="cellColor" ref="L51:L65" dxfId="183"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:G15">
-    <cfRule type="cellIs" dxfId="60" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="182" priority="12" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:O15">
-    <cfRule type="cellIs" dxfId="59" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="181" priority="11" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:G32">
-    <cfRule type="cellIs" dxfId="58" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="180" priority="10" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:O32">
-    <cfRule type="cellIs" dxfId="57" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="179" priority="9" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:F49">
-    <cfRule type="cellIs" dxfId="56" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="178" priority="8" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:M49">
-    <cfRule type="cellIs" dxfId="55" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="177" priority="7" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:F65">
-    <cfRule type="cellIs" dxfId="54" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="176" priority="6" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I52:M65">
-    <cfRule type="cellIs" dxfId="53" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="175" priority="1" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="174" priority="2" operator="greaterThan">
       <formula>0.35</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="173" priority="3" operator="greaterThan">
       <formula>0.39</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="172" priority="4" operator="greaterThan">
       <formula>0.395</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="171" priority="5" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7838,10 +9314,1968 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC876D89-A98F-4B75-B9D9-2CB804013531}">
+  <dimension ref="A1:O79"/>
+  <sheetViews>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.9296875" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="C2">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="G2">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2">
+        <v>-0.127</v>
+      </c>
+      <c r="L2">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="M2">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="O2">
+        <v>0.76300000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>0.157</v>
+      </c>
+      <c r="C3">
+        <v>0.22</v>
+      </c>
+      <c r="D3">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="E3">
+        <v>0.25</v>
+      </c>
+      <c r="G3">
+        <v>0.63</v>
+      </c>
+      <c r="I3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="O3">
+        <v>0.45600000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4">
+        <v>0.31</v>
+      </c>
+      <c r="C4">
+        <v>0.252</v>
+      </c>
+      <c r="G4">
+        <v>0.437</v>
+      </c>
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4">
+        <v>0.224</v>
+      </c>
+      <c r="L4">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="N4">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="O4">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>0.23</v>
+      </c>
+      <c r="C5">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="D5">
+        <v>0.153</v>
+      </c>
+      <c r="E5">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="F5">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="G5">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="I5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5">
+        <v>-0.159</v>
+      </c>
+      <c r="N5">
+        <v>0.86699999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>0.443</v>
+      </c>
+      <c r="C6">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="D6">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="E6">
+        <v>0.312</v>
+      </c>
+      <c r="F6">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="G6">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="I6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="L6">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="N6">
+        <v>0.443</v>
+      </c>
+      <c r="O6">
+        <v>0.23200000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7">
+        <v>0.185</v>
+      </c>
+      <c r="C7">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="D7">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="F7">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="K7">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="M7">
+        <v>0.45300000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="C8">
+        <v>0.189</v>
+      </c>
+      <c r="D8">
+        <v>0.193</v>
+      </c>
+      <c r="E8">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="F8">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="G8">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="I8" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8">
+        <v>0.221</v>
+      </c>
+      <c r="L8">
+        <v>-0.14899999999999999</v>
+      </c>
+      <c r="M8">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="O8">
+        <v>0.13600000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="D9">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="E9">
+        <v>0.115</v>
+      </c>
+      <c r="F9">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="I9" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="M9">
+        <v>-0.105</v>
+      </c>
+      <c r="N9">
+        <v>-0.193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="E10">
+        <v>0.115</v>
+      </c>
+      <c r="F10">
+        <v>0.155</v>
+      </c>
+      <c r="G10">
+        <v>0.247</v>
+      </c>
+      <c r="I10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K10">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="L10">
+        <v>0.23</v>
+      </c>
+      <c r="M10">
+        <v>0.114</v>
+      </c>
+      <c r="O10">
+        <v>-0.18099999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11">
+        <v>0.21</v>
+      </c>
+      <c r="C11">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="D11">
+        <v>0.183</v>
+      </c>
+      <c r="E11">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="F11">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="G11">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="I11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="K11">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="L11">
+        <v>-0.112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12">
+        <v>0.24</v>
+      </c>
+      <c r="C12">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="F12">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="G12">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="I12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12">
+        <v>0.61</v>
+      </c>
+      <c r="L12">
+        <v>0.129</v>
+      </c>
+      <c r="N12">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="O12">
+        <v>-0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D13">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0.217</v>
+      </c>
+      <c r="F13">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="I13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13">
+        <v>0.77100000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="C14">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="D14">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="F14">
+        <v>0.26</v>
+      </c>
+      <c r="G14">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="I14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="M14">
+        <v>-0.113</v>
+      </c>
+      <c r="O14">
+        <v>0.36699999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="C15">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D15">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="E15">
+        <v>0.159</v>
+      </c>
+      <c r="F15">
+        <v>0.111</v>
+      </c>
+      <c r="G15">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="I15" t="s">
+        <v>43</v>
+      </c>
+      <c r="J15">
+        <v>0.873</v>
+      </c>
+      <c r="K15">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="N15">
+        <v>-0.20899999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" t="s">
+        <v>17</v>
+      </c>
+      <c r="M17" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17" t="s">
+        <v>21</v>
+      </c>
+      <c r="O17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="E18">
+        <v>0.129</v>
+      </c>
+      <c r="F18">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="G18">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="I18" t="s">
+        <v>40</v>
+      </c>
+      <c r="K18">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="M18">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="O18">
+        <v>0.52500000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19">
+        <v>0.191</v>
+      </c>
+      <c r="E19">
+        <v>-0.17499999999999999</v>
+      </c>
+      <c r="G19">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="I19" t="s">
+        <v>44</v>
+      </c>
+      <c r="L19">
+        <v>0.115</v>
+      </c>
+      <c r="N19">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20">
+        <v>-0.13600000000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.186</v>
+      </c>
+      <c r="E20">
+        <v>0.123</v>
+      </c>
+      <c r="F20">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="I20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M20">
+        <v>0.98699999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="C21">
+        <v>0.128</v>
+      </c>
+      <c r="D21">
+        <v>-0.104</v>
+      </c>
+      <c r="F21">
+        <v>0.42</v>
+      </c>
+      <c r="I21" t="s">
+        <v>45</v>
+      </c>
+      <c r="L21">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="M21">
+        <v>0.155</v>
+      </c>
+      <c r="N21">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="O21">
+        <v>0.19600000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22">
+        <v>0.99</v>
+      </c>
+      <c r="I22" t="s">
+        <v>47</v>
+      </c>
+      <c r="L22">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="M22">
+        <v>0.14299999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23">
+        <v>0.22</v>
+      </c>
+      <c r="C23">
+        <v>-0.252</v>
+      </c>
+      <c r="D23">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="I23" t="s">
+        <v>49</v>
+      </c>
+      <c r="J23">
+        <v>0.214</v>
+      </c>
+      <c r="L23">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="M23">
+        <v>-0.14899999999999999</v>
+      </c>
+      <c r="O23">
+        <v>0.13400000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24">
+        <v>0.999</v>
+      </c>
+      <c r="E24">
+        <v>-0.108</v>
+      </c>
+      <c r="F24">
+        <v>0.106</v>
+      </c>
+      <c r="I24" t="s">
+        <v>38</v>
+      </c>
+      <c r="J24">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="K24">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="L24">
+        <v>-0.21299999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C25">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="D25">
+        <v>-0.11799999999999999</v>
+      </c>
+      <c r="E25">
+        <v>-0.158</v>
+      </c>
+      <c r="I25" t="s">
+        <v>46</v>
+      </c>
+      <c r="K25">
+        <v>0.98399999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="F26">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="G26">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="I26" t="s">
+        <v>36</v>
+      </c>
+      <c r="J26">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="M26">
+        <v>0.157</v>
+      </c>
+      <c r="N26">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="O26">
+        <v>-0.23499999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27">
+        <v>1.04</v>
+      </c>
+      <c r="E27">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F27">
+        <v>-0.16800000000000001</v>
+      </c>
+      <c r="I27" t="s">
+        <v>41</v>
+      </c>
+      <c r="J27">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="N27">
+        <v>0.11899999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="D28">
+        <v>0.127</v>
+      </c>
+      <c r="E28">
+        <v>0.124</v>
+      </c>
+      <c r="F28">
+        <v>-0.27500000000000002</v>
+      </c>
+      <c r="G28">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="I28" t="s">
+        <v>42</v>
+      </c>
+      <c r="J28">
+        <v>0.63</v>
+      </c>
+      <c r="O28">
+        <v>0.26100000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="G29">
+        <v>0.1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>43</v>
+      </c>
+      <c r="J29">
+        <v>0.85899999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="D30">
+        <v>-0.14699999999999999</v>
+      </c>
+      <c r="F30">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="I30" t="s">
+        <v>39</v>
+      </c>
+      <c r="J30">
+        <v>0.311</v>
+      </c>
+      <c r="K30">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="M30">
+        <v>0.221</v>
+      </c>
+      <c r="N30">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="O30">
+        <v>0.17199999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="D31">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="G31">
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="I31" t="s">
+        <v>48</v>
+      </c>
+      <c r="J31">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="L31">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="O31">
+        <v>0.33800000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" t="s">
+        <v>20</v>
+      </c>
+      <c r="K33" t="s">
+        <v>1</v>
+      </c>
+      <c r="L33" t="s">
+        <v>0</v>
+      </c>
+      <c r="M33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34">
+        <v>0.156</v>
+      </c>
+      <c r="C34">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="D34">
+        <v>0.191</v>
+      </c>
+      <c r="E34">
+        <v>0.192</v>
+      </c>
+      <c r="F34">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="H34" t="s">
+        <v>41</v>
+      </c>
+      <c r="I34">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="M34">
+        <v>0.54600000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="C35">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="E35">
+        <v>0.436</v>
+      </c>
+      <c r="F35">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="H35" t="s">
+        <v>43</v>
+      </c>
+      <c r="I35">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="M35">
+        <v>0.50700000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36">
+        <v>0.312</v>
+      </c>
+      <c r="E36">
+        <v>0.46</v>
+      </c>
+      <c r="H36" t="s">
+        <v>36</v>
+      </c>
+      <c r="J36">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="L36">
+        <v>0.121</v>
+      </c>
+      <c r="M36">
+        <v>0.66600000000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="C37">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="D37">
+        <v>0.18</v>
+      </c>
+      <c r="E37">
+        <v>0.91</v>
+      </c>
+      <c r="F37">
+        <v>0.123</v>
+      </c>
+      <c r="H37" t="s">
+        <v>37</v>
+      </c>
+      <c r="I37">
+        <v>-0.14699999999999999</v>
+      </c>
+      <c r="K37">
+        <v>-0.124</v>
+      </c>
+      <c r="L37">
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="M37">
+        <v>0.13200000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="C38">
+        <v>0.49</v>
+      </c>
+      <c r="D38">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="E38">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="F38">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="H38" t="s">
+        <v>38</v>
+      </c>
+      <c r="K38">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="M38">
+        <v>0.248</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C39">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="D39">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="E39">
+        <v>0.254</v>
+      </c>
+      <c r="H39" t="s">
+        <v>46</v>
+      </c>
+      <c r="J39">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="K39">
+        <v>1.06</v>
+      </c>
+      <c r="L39">
+        <v>-0.159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="C40">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D40">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="E40">
+        <v>0.27</v>
+      </c>
+      <c r="F40">
+        <v>0.157</v>
+      </c>
+      <c r="H40" t="s">
+        <v>49</v>
+      </c>
+      <c r="I40">
+        <v>0.501</v>
+      </c>
+      <c r="J40">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="L40">
+        <v>-0.121</v>
+      </c>
+      <c r="M40">
+        <v>-0.121</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="C41">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="D41">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="E41">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="F41">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="H41" t="s">
+        <v>44</v>
+      </c>
+      <c r="I41">
+        <v>-0.18</v>
+      </c>
+      <c r="J41">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="L41">
+        <v>-0.153</v>
+      </c>
+      <c r="M41">
+        <v>0.26700000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="C42">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="D42">
+        <v>0.17</v>
+      </c>
+      <c r="E42">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="F42">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="H42" t="s">
+        <v>45</v>
+      </c>
+      <c r="I42">
+        <v>0.191</v>
+      </c>
+      <c r="J42">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="L42">
+        <v>0.151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43">
+        <v>0.497</v>
+      </c>
+      <c r="C43">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="H43" t="s">
+        <v>47</v>
+      </c>
+      <c r="I43">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="J43">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="L43">
+        <v>0.24299999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="D44">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="E44">
+        <v>0.111</v>
+      </c>
+      <c r="H44" t="s">
+        <v>40</v>
+      </c>
+      <c r="I44">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="K44">
+        <v>0.374</v>
+      </c>
+      <c r="L44">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="M44">
+        <v>-0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="C45">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="D45">
+        <v>0.124</v>
+      </c>
+      <c r="E45">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="F45">
+        <v>0.378</v>
+      </c>
+      <c r="H45" t="s">
+        <v>42</v>
+      </c>
+      <c r="I45">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="K45">
+        <v>-0.105</v>
+      </c>
+      <c r="M45">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="C46">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="D46">
+        <v>0.307</v>
+      </c>
+      <c r="E46">
+        <v>0.1</v>
+      </c>
+      <c r="H46" t="s">
+        <v>48</v>
+      </c>
+      <c r="I46">
+        <v>0.59699999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="C47">
+        <v>0.184</v>
+      </c>
+      <c r="D47">
+        <v>0.115</v>
+      </c>
+      <c r="E47">
+        <v>0.124</v>
+      </c>
+      <c r="H47" t="s">
+        <v>39</v>
+      </c>
+      <c r="I47">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="J47">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="K47">
+        <v>0.107</v>
+      </c>
+      <c r="L47">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="M47">
+        <v>0.27800000000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B49" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" t="s">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
+        <v>0</v>
+      </c>
+      <c r="I49" t="s">
+        <v>17</v>
+      </c>
+      <c r="J49" t="s">
+        <v>18</v>
+      </c>
+      <c r="K49" t="s">
+        <v>1</v>
+      </c>
+      <c r="L49" t="s">
+        <v>0</v>
+      </c>
+      <c r="M49" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>37</v>
+      </c>
+      <c r="B50">
+        <v>0.129</v>
+      </c>
+      <c r="F50">
+        <v>0.99</v>
+      </c>
+      <c r="H50" t="s">
+        <v>36</v>
+      </c>
+      <c r="I50">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="L50">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M50">
+        <v>-0.40100000000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="E51">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="F51">
+        <v>-0.11600000000000001</v>
+      </c>
+      <c r="H51" t="s">
+        <v>37</v>
+      </c>
+      <c r="L51">
+        <v>0.97599999999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52">
+        <v>-0.14499999999999999</v>
+      </c>
+      <c r="D52">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="E52">
+        <v>0.49</v>
+      </c>
+      <c r="H52" t="s">
+        <v>38</v>
+      </c>
+      <c r="I52">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="J52">
+        <v>-0.19600000000000001</v>
+      </c>
+      <c r="K52">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="M52">
+        <v>-0.14199999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>36</v>
+      </c>
+      <c r="B53">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="C53">
+        <v>-0.34300000000000003</v>
+      </c>
+      <c r="D53">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="E53">
+        <v>0.107</v>
+      </c>
+      <c r="F53">
+        <v>0.112</v>
+      </c>
+      <c r="H53" t="s">
+        <v>39</v>
+      </c>
+      <c r="I53">
+        <v>0.37</v>
+      </c>
+      <c r="J53">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="K53">
+        <v>0.154</v>
+      </c>
+      <c r="L53">
+        <v>0.17399999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54">
+        <v>0.252</v>
+      </c>
+      <c r="D54">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="H54" t="s">
+        <v>40</v>
+      </c>
+      <c r="I54">
+        <v>0.186</v>
+      </c>
+      <c r="K54">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="L54">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="M54">
+        <v>0.35399999999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>43</v>
+      </c>
+      <c r="C55">
+        <v>0.317</v>
+      </c>
+      <c r="D55">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="H55" t="s">
+        <v>41</v>
+      </c>
+      <c r="I55">
+        <v>0.83099999999999996</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>49</v>
+      </c>
+      <c r="B56">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="C56">
+        <v>0.54</v>
+      </c>
+      <c r="E56">
+        <v>-0.16500000000000001</v>
+      </c>
+      <c r="F56">
+        <v>-0.16200000000000001</v>
+      </c>
+      <c r="H56" t="s">
+        <v>42</v>
+      </c>
+      <c r="I56">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="M56">
+        <v>0.23200000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>40</v>
+      </c>
+      <c r="C57">
+        <v>0.59</v>
+      </c>
+      <c r="D57">
+        <v>-0.123</v>
+      </c>
+      <c r="E57">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="F57">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="H57" t="s">
+        <v>43</v>
+      </c>
+      <c r="I57">
+        <v>0.83699999999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>42</v>
+      </c>
+      <c r="C58">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="D58">
+        <v>0.371</v>
+      </c>
+      <c r="E58">
+        <v>-0.13700000000000001</v>
+      </c>
+      <c r="H58" t="s">
+        <v>44</v>
+      </c>
+      <c r="J58">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="L58">
+        <v>-0.14499999999999999</v>
+      </c>
+      <c r="M58">
+        <v>-0.34300000000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>48</v>
+      </c>
+      <c r="C59">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="H59" t="s">
+        <v>45</v>
+      </c>
+      <c r="J59">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="L59">
+        <v>0.114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>47</v>
+      </c>
+      <c r="B60">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="C60">
+        <v>0.217</v>
+      </c>
+      <c r="D60">
+        <v>-0.13200000000000001</v>
+      </c>
+      <c r="F60">
+        <v>0.157</v>
+      </c>
+      <c r="H60" t="s">
+        <v>46</v>
+      </c>
+      <c r="K60">
+        <v>1.0029999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>44</v>
+      </c>
+      <c r="B61">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="C61">
+        <v>-0.28799999999999998</v>
+      </c>
+      <c r="D61">
+        <v>0.193</v>
+      </c>
+      <c r="F61">
+        <v>-0.17899999999999999</v>
+      </c>
+      <c r="H61" t="s">
+        <v>47</v>
+      </c>
+      <c r="J61">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="L61">
+        <v>0.19500000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>45</v>
+      </c>
+      <c r="B62">
+        <v>0.755</v>
+      </c>
+      <c r="C62">
+        <v>0.224</v>
+      </c>
+      <c r="H62" t="s">
+        <v>48</v>
+      </c>
+      <c r="I62">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="J62">
+        <v>0.186</v>
+      </c>
+      <c r="M62">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>39</v>
+      </c>
+      <c r="B63">
+        <v>0.43</v>
+      </c>
+      <c r="C63">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="D63">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="E63">
+        <v>0.104</v>
+      </c>
+      <c r="F63">
+        <v>0.128</v>
+      </c>
+      <c r="H63" t="s">
+        <v>49</v>
+      </c>
+      <c r="I63">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="J63">
+        <v>0.59</v>
+      </c>
+      <c r="L63">
+        <v>-0.128</v>
+      </c>
+      <c r="M63">
+        <v>0.221</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" t="s">
+        <v>18</v>
+      </c>
+      <c r="E66" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67">
+        <v>-0.16800000000000001</v>
+      </c>
+      <c r="C67">
+        <v>0.251</v>
+      </c>
+      <c r="E67">
+        <v>0.56499999999999995</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="E68">
+        <v>0.79200000000000004</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69">
+        <v>-0.20699999999999999</v>
+      </c>
+      <c r="D69">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="E69">
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="D70">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="E70">
+        <v>-0.18099999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>15</v>
+      </c>
+      <c r="B71">
+        <v>0.104</v>
+      </c>
+      <c r="D71">
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72">
+        <v>0.214</v>
+      </c>
+      <c r="C72">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="D72">
+        <v>-0.26600000000000001</v>
+      </c>
+      <c r="E72">
+        <v>0.151</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="D73">
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>9</v>
+      </c>
+      <c r="C74">
+        <v>0.66</v>
+      </c>
+      <c r="D74">
+        <v>0.318</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="C75">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="E75">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>10</v>
+      </c>
+      <c r="B76">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="C76">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="D76">
+        <v>-0.37</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>11</v>
+      </c>
+      <c r="B77">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="C78">
+        <v>-0.104</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
+        <v>50</v>
+      </c>
+      <c r="B79">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="D79">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="E79">
+        <v>-0.215</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A66:E79" xr:uid="{AC876D89-A98F-4B75-B9D9-2CB804013531}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A67:E79">
+      <sortCondition sortBy="cellColor" ref="E66:E79" dxfId="1"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="B2:G15">
+    <cfRule type="cellIs" dxfId="24" priority="9" operator="greaterThan">
+      <formula>0.399</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:O15">
+    <cfRule type="cellIs" dxfId="23" priority="8" operator="greaterThan">
+      <formula>0.399</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:G31">
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="greaterThan">
+      <formula>0.399</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18:O31">
+    <cfRule type="cellIs" dxfId="21" priority="6" operator="greaterThan">
+      <formula>0.399</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34:F47">
+    <cfRule type="cellIs" dxfId="20" priority="5" operator="greaterThan">
+      <formula>0.399</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34:M47">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="greaterThan">
+      <formula>0.399</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50:F63">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="greaterThan">
+      <formula>0.399</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I50:M63">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="greaterThan">
+      <formula>0.399</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B67:E79">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+      <formula>0.499</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C42105-EFDA-4FA3-8AB1-E5E42D4D4CA4}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView topLeftCell="F46" zoomScale="140" workbookViewId="0">
+    <sheetView topLeftCell="F45" zoomScale="140" workbookViewId="0">
       <selection activeCell="H46" sqref="H46:L59"/>
     </sheetView>
   </sheetViews>
@@ -9310,46 +12744,46 @@
   </sheetData>
   <autoFilter ref="H46:L59" xr:uid="{26C42105-EFDA-4FA3-8AB1-E5E42D4D4CA4}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H47:L59">
-      <sortCondition sortBy="cellColor" ref="L46:L59" dxfId="48"/>
+      <sortCondition sortBy="cellColor" ref="L46:L59" dxfId="170"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:F14">
-    <cfRule type="cellIs" dxfId="47" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="169" priority="8" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:M14">
-    <cfRule type="cellIs" dxfId="46" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="168" priority="7" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:F29">
-    <cfRule type="cellIs" dxfId="45" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="167" priority="6" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:M29">
-    <cfRule type="cellIs" dxfId="44" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="166" priority="5" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:E44">
-    <cfRule type="cellIs" dxfId="43" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="165" priority="4" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32:L44">
-    <cfRule type="cellIs" dxfId="42" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="164" priority="3" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:E59">
-    <cfRule type="cellIs" dxfId="41" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="163" priority="2" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47:L59">
-    <cfRule type="cellIs" dxfId="40" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="162" priority="1" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9358,11 +12792,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984B0D20-5E48-4763-A83B-7B371039BA3E}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -9555,7 +12989,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:E14">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="161" priority="1" operator="greaterThan">
       <formula>0.399</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9564,7 +12998,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87DCAE64-8530-4592-A838-A6CB5F75441C}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -9813,11 +13247,11 @@
   </sheetData>
   <autoFilter ref="A1:E14" xr:uid="{87DCAE64-8530-4592-A838-A6CB5F75441C}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E14">
-      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="38"/>
+      <sortCondition sortBy="cellColor" ref="E1:E14" dxfId="160"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E14">
-    <cfRule type="cellIs" dxfId="37" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="159" priority="1" operator="greaterThan">
       <formula>0.499</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9825,11 +13259,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D6D6342-FAB0-45B3-B96B-783C62CCE1DB}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D18"/>
     </sheetView>
   </sheetViews>
@@ -10056,7 +13490,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DF5018-9911-4233-8E1E-CFEBD8577F16}">
   <dimension ref="A1:W27"/>
   <sheetViews>
@@ -11195,47 +14629,47 @@
   </sheetData>
   <autoFilter ref="A15:E27" xr:uid="{00DF5018-9911-4233-8E1E-CFEBD8577F16}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:E27">
-      <sortCondition sortBy="cellColor" ref="E15:E27" dxfId="36"/>
+      <sortCondition sortBy="cellColor" ref="E15:E27" dxfId="158"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B2:D13">
-    <cfRule type="cellIs" dxfId="35" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="157" priority="8" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:I13">
-    <cfRule type="cellIs" dxfId="34" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="156" priority="7" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:N13">
-    <cfRule type="cellIs" dxfId="33" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="155" priority="6" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:S13">
-    <cfRule type="cellIs" dxfId="32" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="154" priority="5" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:E27">
-    <cfRule type="cellIs" dxfId="31" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="153" priority="4" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:K27">
-    <cfRule type="cellIs" dxfId="30" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="152" priority="3" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16:Q27">
-    <cfRule type="cellIs" dxfId="29" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="151" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16:W27">
-    <cfRule type="cellIs" dxfId="28" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="150" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11244,7 +14678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5509DC-DB05-43E6-A45B-32E76BC27DEA}">
   <dimension ref="A1:K23"/>
   <sheetViews>
@@ -11855,318 +15289,20 @@
   </sheetData>
   <autoFilter ref="H1:K16" xr:uid="{8B5509DC-DB05-43E6-A45B-32E76BC27DEA}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:K16">
-      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="27"/>
+      <sortCondition sortBy="cellColor" ref="K1:K16" dxfId="149"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="148" priority="2" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K16">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="147" priority="1" operator="greaterThan">
       <formula>0.299</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4883B1BD-E07A-48BB-9F66-A8C7003F2BEF}">
-  <dimension ref="A1:E16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="13.3984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>0.21</v>
-      </c>
-      <c r="C2">
-        <v>0.62</v>
-      </c>
-      <c r="D2">
-        <v>0.31</v>
-      </c>
-      <c r="E2">
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>0.23</v>
-      </c>
-      <c r="C3">
-        <v>0.59</v>
-      </c>
-      <c r="D3">
-        <v>0.24</v>
-      </c>
-      <c r="E3">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>0.63</v>
-      </c>
-      <c r="C4">
-        <v>0.12</v>
-      </c>
-      <c r="D4">
-        <v>-0.04</v>
-      </c>
-      <c r="E4">
-        <v>0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>0.12</v>
-      </c>
-      <c r="C5">
-        <v>0.3</v>
-      </c>
-      <c r="D5">
-        <v>0.22</v>
-      </c>
-      <c r="E5">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>0.2</v>
-      </c>
-      <c r="C6">
-        <v>0.05</v>
-      </c>
-      <c r="D6">
-        <v>0.27</v>
-      </c>
-      <c r="E6">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>0.25</v>
-      </c>
-      <c r="C7">
-        <v>0.52</v>
-      </c>
-      <c r="D7">
-        <v>0.52</v>
-      </c>
-      <c r="E7">
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>0.66</v>
-      </c>
-      <c r="C8">
-        <v>0.26</v>
-      </c>
-      <c r="D8">
-        <v>0.51</v>
-      </c>
-      <c r="E8">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>0.17</v>
-      </c>
-      <c r="C9">
-        <v>-0.04</v>
-      </c>
-      <c r="D9">
-        <v>0.78</v>
-      </c>
-      <c r="E9">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>0.06</v>
-      </c>
-      <c r="C10">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="D10">
-        <v>0.81</v>
-      </c>
-      <c r="E10">
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>0.2</v>
-      </c>
-      <c r="C11">
-        <v>0.72</v>
-      </c>
-      <c r="D11">
-        <v>0.23</v>
-      </c>
-      <c r="E11">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>0.11</v>
-      </c>
-      <c r="C12">
-        <v>0.71</v>
-      </c>
-      <c r="D12">
-        <v>-0.1</v>
-      </c>
-      <c r="E12">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>0.49</v>
-      </c>
-      <c r="C13">
-        <v>0.54</v>
-      </c>
-      <c r="D13">
-        <v>0.04</v>
-      </c>
-      <c r="E13">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>0.82</v>
-      </c>
-      <c r="C14">
-        <v>0.2</v>
-      </c>
-      <c r="D14">
-        <v>0.05</v>
-      </c>
-      <c r="E14">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>0.53</v>
-      </c>
-      <c r="C15">
-        <v>0.48</v>
-      </c>
-      <c r="D15">
-        <v>0.47</v>
-      </c>
-      <c r="E15">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>0.72</v>
-      </c>
-      <c r="C16">
-        <v>0.22</v>
-      </c>
-      <c r="D16">
-        <v>0.48</v>
-      </c>
-      <c r="E16">
-        <v>0.18</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="B1:E16" xr:uid="{4883B1BD-E07A-48BB-9F66-A8C7003F2BEF}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E16">
-      <sortCondition sortBy="cellColor" ref="E1:E16" dxfId="24"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="B2:E16">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
-      <formula>0.699</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>